<commit_message>
Update de Plazo Fijo 12-01-2023
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20393"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B625C7-FEF4-4677-A766-1794005A6753}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>Nombre</t>
   </si>
@@ -125,12 +126,51 @@
   </si>
   <si>
     <t>Consulta de Cuentas</t>
+  </si>
+  <si>
+    <t>Plazo Fijo</t>
+  </si>
+  <si>
+    <t>Liquidacion Plazo Fijo Ajustable</t>
+  </si>
+  <si>
+    <t>Impresión de Certificados y Formularios</t>
+  </si>
+  <si>
+    <t>Consulta de Plazo Fijo</t>
+  </si>
+  <si>
+    <t>Consulta Circulares Vigentes</t>
+  </si>
+  <si>
+    <t>Consulta Tasa Plazo Fijo</t>
+  </si>
+  <si>
+    <t>Consulta Indices</t>
+  </si>
+  <si>
+    <t>Altas/Pagos/Inm Pagados/Imm Impagos</t>
+  </si>
+  <si>
+    <t>Plazo Fijo Inmovilizado</t>
+  </si>
+  <si>
+    <t>PF Vencidos Inmovilizados Pagados</t>
+  </si>
+  <si>
+    <t>Consulta por Firmante</t>
+  </si>
+  <si>
+    <t>Monto Activo por Titular</t>
+  </si>
+  <si>
+    <t>Plazo Fijos Activos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -453,7 +493,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -502,7 +542,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -549,11 +589,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,11 +640,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,13 +699,70 @@
         <v>31</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Casos de comisiones - consultas de bonificacion
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B625C7-FEF4-4677-A766-1794005A6753}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB7E183-7573-42BB-A2D6-71563B60BDBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>Nombre</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>Plazo Fijos Activos</t>
+  </si>
+  <si>
+    <t>F00474</t>
+  </si>
+  <si>
+    <t>074</t>
   </si>
 </sst>
 </file>
@@ -590,10 +596,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,6 +637,14 @@
       </c>
       <c r="C4" s="4" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -643,7 +657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update 23-01-23: Plazo fijo
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B625C7-FEF4-4677-A766-1794005A6753}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258B8334-4D5E-41D4-8502-E75F14E4E7E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,6 +13,7 @@
     <sheet name="Users" sheetId="3" r:id="rId3"/>
     <sheet name="Modulos" sheetId="4" r:id="rId4"/>
     <sheet name="MsgError" sheetId="5" r:id="rId5"/>
+    <sheet name="DataUser" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>Nombre</t>
   </si>
@@ -165,6 +166,27 @@
   </si>
   <si>
     <t>Plazo Fijos Activos</t>
+  </si>
+  <si>
+    <t>PLAZO FIJO</t>
+  </si>
+  <si>
+    <t>ARCHIVOS PERSONAS</t>
+  </si>
+  <si>
+    <t>Consulta Pagos Plazo Fijo</t>
+  </si>
+  <si>
+    <t>Numero de Cuenta</t>
+  </si>
+  <si>
+    <t>IdPersona</t>
+  </si>
+  <si>
+    <t>NumeroOperacion</t>
+  </si>
+  <si>
+    <t>Consulta de Posicion en Linea</t>
   </si>
 </sst>
 </file>
@@ -641,10 +663,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,6 +776,26 @@
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -794,4 +836,40 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FCD75B7-3767-4AF4-8551-2556E8D90A6B}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>11918739</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Fix] Modificacion de perfil
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258B8334-4D5E-41D4-8502-E75F14E4E7E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98FB75C-1EA5-4214-8EA9-B20F315DB501}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>Nombre</t>
   </si>
@@ -33,9 +33,6 @@
     <t>IP</t>
   </si>
   <si>
-    <t>Test10</t>
-  </si>
-  <si>
     <t>10.160.5.10</t>
   </si>
   <si>
@@ -187,6 +184,18 @@
   </si>
   <si>
     <t>Consulta de Posicion en Linea</t>
+  </si>
+  <si>
+    <t>Tes11</t>
+  </si>
+  <si>
+    <t>10.169.1.7</t>
+  </si>
+  <si>
+    <t>Tes10</t>
+  </si>
+  <si>
+    <t>t24tes11</t>
   </si>
 </sst>
 </file>
@@ -222,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -235,6 +244,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -516,9 +528,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -536,10 +550,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -547,7 +561,7 @@
         <v>708</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -555,8 +569,20 @@
         <v>702</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -565,11 +591,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -578,15 +602,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -594,7 +618,7 @@
         <v>708</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -602,8 +626,19 @@
         <v>702</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
-      </c>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -622,37 +657,37 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -665,7 +700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -679,123 +714,123 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
       <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
         <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
         <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
         <v>37</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
         <v>44</v>
-      </c>
-      <c r="D12" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -819,18 +854,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -855,13 +890,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Feature] Creacion de Perfiles por Ambiente & modificacion Main Data
Se crearon perfiles por ambiente, y se ajustaron datos de Main Data/Modulos.
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98FB75C-1EA5-4214-8EA9-B20F315DB501}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21F18C6-AEDA-4F04-B8F3-5F256CFE138E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>Nombre</t>
   </si>
@@ -196,6 +196,21 @@
   </si>
   <si>
     <t>t24tes11</t>
+  </si>
+  <si>
+    <t>BCCL.E.CONS.TINT.ALTAS</t>
+  </si>
+  <si>
+    <t>BCCL.E.TINTERNAS.APAGAR</t>
+  </si>
+  <si>
+    <t>Transferencias Internas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consulta de Altas Transf. Internas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consulta de Altas Transf. Internas A Pagar </t>
   </si>
 </sst>
 </file>
@@ -593,7 +608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -698,16 +713,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" customWidth="1"/>
     <col min="3" max="3" width="40.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -828,9 +843,28 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] Edicion de Profiles & Scripts de Transferencias Internas
Se agregaron las keywords de ConfigEnvironment y Login a los casos de TI.
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21F18C6-AEDA-4F04-B8F3-5F256CFE138E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFC57C5-A4FD-4D05-B893-F9BF88E7B255}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
   <si>
     <t>Nombre</t>
   </si>
@@ -211,6 +211,45 @@
   </si>
   <si>
     <t xml:space="preserve">Consulta de Altas Transf. Internas A Pagar </t>
+  </si>
+  <si>
+    <t>F00289</t>
+  </si>
+  <si>
+    <t>F00073</t>
+  </si>
+  <si>
+    <t>F00473</t>
+  </si>
+  <si>
+    <t>F00474</t>
+  </si>
+  <si>
+    <t>ANOVELLO</t>
+  </si>
+  <si>
+    <t>F00274</t>
+  </si>
+  <si>
+    <t>073</t>
+  </si>
+  <si>
+    <t>074</t>
+  </si>
+  <si>
+    <t>Gerente Operativo</t>
+  </si>
+  <si>
+    <t>F02653</t>
+  </si>
+  <si>
+    <t>F00743</t>
+  </si>
+  <si>
+    <t>168</t>
+  </si>
+  <si>
+    <t>037</t>
   </si>
 </sst>
 </file>
@@ -662,13 +701,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="20" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -681,7 +723,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -699,10 +741,74 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -715,7 +821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[FEATURE] Kyw Habilitar Command Line
Se genero una parte de la kyw. No se termino, validacion de Command Line no funciona correctamente, y el llamado quedo dividido en dos partes. Hay que replantear su funcionamiento.
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFC57C5-A4FD-4D05-B893-F9BF88E7B255}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86712A73-CC23-4AE7-9113-A3B2B7242B0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="79">
   <si>
     <t>Nombre</t>
   </si>
@@ -250,6 +250,18 @@
   </si>
   <si>
     <t>037</t>
+  </si>
+  <si>
+    <t>CRECEREM</t>
+  </si>
+  <si>
+    <t>Usuario Emergencia</t>
+  </si>
+  <si>
+    <t>F02971</t>
+  </si>
+  <si>
+    <t>Usuario sin command line</t>
   </si>
 </sst>
 </file>
@@ -701,15 +713,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -809,6 +821,22 @@
       </c>
       <c r="C12" s="4" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE] Modulos sprint 06-03 y 20-03
Cheque Cancelatorio
Inventario Permanente
ONP
Fallas de Dispositivos
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86712A73-CC23-4AE7-9113-A3B2B7242B0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC15D4D0-FEA6-4DB6-AC7D-01290FC54207}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="85">
   <si>
     <t>Nombre</t>
   </si>
@@ -262,6 +262,24 @@
   </si>
   <si>
     <t>Usuario sin command line</t>
+  </si>
+  <si>
+    <t>026</t>
+  </si>
+  <si>
+    <t>F00273</t>
+  </si>
+  <si>
+    <t>F00644</t>
+  </si>
+  <si>
+    <t>F01106</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>F02547</t>
   </si>
 </sst>
 </file>
@@ -713,10 +731,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,6 +855,38 @@
       </c>
       <c r="C14" s="4" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] Movimientos Automaticos y Main Data
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB113AAE-A475-4F9F-A218-2675D673219F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DE26E8-71DA-44CE-898A-BF3617320A67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="88">
   <si>
     <t>Nombre</t>
   </si>
@@ -265,6 +265,30 @@
   </si>
   <si>
     <t>F00273</t>
+  </si>
+  <si>
+    <t>F00263</t>
+  </si>
+  <si>
+    <t>063</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>F00644</t>
+  </si>
+  <si>
+    <t>026</t>
+  </si>
+  <si>
+    <t>F01106</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>F02547</t>
   </si>
 </sst>
 </file>
@@ -716,10 +740,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +751,7 @@
     <col min="3" max="3" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -738,7 +762,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -746,7 +770,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -754,7 +778,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -762,7 +786,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -770,7 +794,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>63</v>
       </c>
@@ -778,7 +802,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -786,7 +810,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -794,7 +818,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -802,7 +826,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -810,7 +834,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>71</v>
       </c>
@@ -818,7 +842,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -826,7 +850,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -834,7 +858,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -842,13 +866,51 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>79</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="D15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[FEATURE] Nuevos casos de Bloqueo y Desbloqueo (BYD 01-05)
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20398"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73657EDD-05DE-4BAD-BCDE-AABABBE03CFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6F8672-9A4B-40DE-9A63-8BA6E6C83C26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="89">
   <si>
     <t>Nombre</t>
   </si>
@@ -286,6 +286,12 @@
   </si>
   <si>
     <t>F02547</t>
+  </si>
+  <si>
+    <t>F00076</t>
+  </si>
+  <si>
+    <t>076</t>
   </si>
 </sst>
 </file>
@@ -739,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +910,12 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="4"/>
+      <c r="A20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[FEATURE] [FIX] Aut. Suc, cheques y chequeras disponibles s20230724 y TEST-8704
Se agrego ASUC26, Y CCD01 AL CC09

Se realizaron pruebas de performance TEST-8704
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20400"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB767CD4-0EFF-418C-B6E3-314E091750AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647A61B3-BADB-453E-AEB4-B716F00B9871}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="97">
   <si>
     <t>Nombre</t>
   </si>
@@ -301,6 +301,21 @@
   </si>
   <si>
     <t>Casa central</t>
+  </si>
+  <si>
+    <t>F00319</t>
+  </si>
+  <si>
+    <t>F00044</t>
+  </si>
+  <si>
+    <t>044</t>
+  </si>
+  <si>
+    <t>OSANTOS</t>
+  </si>
+  <si>
+    <t>CRECERAD</t>
   </si>
 </sst>
 </file>
@@ -752,10 +767,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,6 +954,38 @@
         <v>90</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[FEATURE]Cheques y chequeras disp, mov pendientes cancelados, mov rechazados pendientes de imputacion s20230807, pruebas performance
Pruebas performance TEST-8788

Se agregaron casos de cheques y chequeras disponibles CCD10 al CCD14

Se agregaron casos de movimientos pendientes cancelados MPC01 Y MPC02

Se agregaron casos de movimientos rechazados pendientes de imputacion
MRPI01 MRPI02
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20400"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647A61B3-BADB-453E-AEB4-B716F00B9871}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E13321-1BE2-4100-B52F-C608DBBB138B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="101">
   <si>
     <t>Nombre</t>
   </si>
@@ -316,6 +316,18 @@
   </si>
   <si>
     <t>CRECERAD</t>
+  </si>
+  <si>
+    <t>F02062</t>
+  </si>
+  <si>
+    <t>F03153</t>
+  </si>
+  <si>
+    <t>F00191</t>
+  </si>
+  <si>
+    <t>F02729</t>
   </si>
 </sst>
 </file>
@@ -767,10 +779,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,6 +999,38 @@
       </c>
       <c r="C26" s="4" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE] TEST-8857 Alta de Cuentas - Performance NCD
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20400"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647A61B3-BADB-453E-AEB4-B716F00B9871}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92B8E11-3029-4BA3-BFB0-3474E23B3468}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="98">
   <si>
     <t>Nombre</t>
   </si>
@@ -316,6 +316,9 @@
   </si>
   <si>
     <t>CRECERAD</t>
+  </si>
+  <si>
+    <t>F00901</t>
   </si>
 </sst>
 </file>
@@ -767,10 +770,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,6 +990,14 @@
       </c>
       <c r="C26" s="4" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] Se soluciono problema con el archivo de usuarios
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92B8E11-3029-4BA3-BFB0-3474E23B3468}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB8E287-BBB9-42D5-A91C-ABE87D408EDA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="102">
   <si>
     <t>Nombre</t>
   </si>
@@ -319,6 +319,18 @@
   </si>
   <si>
     <t>F00901</t>
+  </si>
+  <si>
+    <t>F02062</t>
+  </si>
+  <si>
+    <t>F03153</t>
+  </si>
+  <si>
+    <t>F00191</t>
+  </si>
+  <si>
+    <t>F02729</t>
   </si>
 </sst>
 </file>
@@ -770,10 +782,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,9 +1006,41 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[FEATURE & UPDATE] Alta de cuenta + Pruebas performance
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB8E287-BBB9-42D5-A91C-ABE87D408EDA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{825D4A34-D066-49A2-93BA-99C6D994E65B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,9 +11,10 @@
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
     <sheet name="Test Server" sheetId="2" r:id="rId2"/>
     <sheet name="Users" sheetId="3" r:id="rId3"/>
-    <sheet name="Modulos" sheetId="4" r:id="rId4"/>
-    <sheet name="MsgError" sheetId="5" r:id="rId5"/>
-    <sheet name="DataUser" sheetId="6" r:id="rId6"/>
+    <sheet name="DatosNCD" sheetId="7" r:id="rId4"/>
+    <sheet name="Modulos" sheetId="4" r:id="rId5"/>
+    <sheet name="MsgError" sheetId="5" r:id="rId6"/>
+    <sheet name="DataUser" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="109">
   <si>
     <t>Nombre</t>
   </si>
@@ -331,6 +332,27 @@
   </si>
   <si>
     <t>F02729</t>
+  </si>
+  <si>
+    <t>DNI</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Codigo Producto</t>
+  </si>
+  <si>
+    <t>Tarifario</t>
+  </si>
+  <si>
+    <t>6001.6000</t>
+  </si>
+  <si>
+    <t>6002.6060</t>
+  </si>
+  <si>
+    <t>F00401</t>
   </si>
 </sst>
 </file>
@@ -346,12 +368,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -366,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -383,6 +411,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,10 +814,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,6 +1076,14 @@
         <v>22</v>
       </c>
     </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1051,6 +1091,797 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8058F8B-909F-4289-A69E-5DC86994C957}">
+  <dimension ref="A1:D75"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>14519407</v>
+      </c>
+      <c r="B2">
+        <v>20230125</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>14519407</v>
+      </c>
+      <c r="B3">
+        <v>20230125</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>31498548</v>
+      </c>
+      <c r="B4">
+        <v>20230125</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>31498548</v>
+      </c>
+      <c r="B5">
+        <v>20230125</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>25379158</v>
+      </c>
+      <c r="B6">
+        <v>20230125</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>25379158</v>
+      </c>
+      <c r="B7">
+        <v>20230125</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>22749003</v>
+      </c>
+      <c r="B8">
+        <v>20230125</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>22749003</v>
+      </c>
+      <c r="B9">
+        <v>20230125</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>12128869</v>
+      </c>
+      <c r="B10">
+        <v>20230125</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>12128869</v>
+      </c>
+      <c r="B11">
+        <v>20230125</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>26074710</v>
+      </c>
+      <c r="B12">
+        <v>20230125</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>26074710</v>
+      </c>
+      <c r="B13">
+        <v>20230125</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13340126</v>
+      </c>
+      <c r="B14">
+        <v>20230125</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13340126</v>
+      </c>
+      <c r="B15">
+        <v>20230125</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>26411749</v>
+      </c>
+      <c r="B16" s="7">
+        <v>20230125</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" s="7">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>35959549</v>
+      </c>
+      <c r="B17">
+        <v>20230125</v>
+      </c>
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18432020</v>
+      </c>
+      <c r="B18">
+        <v>20230125</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18432020</v>
+      </c>
+      <c r="B19">
+        <v>20230125</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1881859</v>
+      </c>
+      <c r="B20">
+        <v>20230125</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18432020</v>
+      </c>
+      <c r="B21">
+        <v>20230125</v>
+      </c>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>30571421352</v>
+      </c>
+      <c r="B22">
+        <v>20230125</v>
+      </c>
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22809322</v>
+      </c>
+      <c r="B23">
+        <v>20230125</v>
+      </c>
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3296392</v>
+      </c>
+      <c r="B24">
+        <v>20230125</v>
+      </c>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>4855059</v>
+      </c>
+      <c r="B25">
+        <v>20230125</v>
+      </c>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>14407569</v>
+      </c>
+      <c r="B26">
+        <v>20230125</v>
+      </c>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>33393013</v>
+      </c>
+      <c r="B27">
+        <v>20230125</v>
+      </c>
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>11022835</v>
+      </c>
+      <c r="B28">
+        <v>20230125</v>
+      </c>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>23208752</v>
+      </c>
+      <c r="B29">
+        <v>20230125</v>
+      </c>
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>93983321</v>
+      </c>
+      <c r="B30">
+        <v>20230125</v>
+      </c>
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>27500525</v>
+      </c>
+      <c r="B31">
+        <v>20230125</v>
+      </c>
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>4375526</v>
+      </c>
+      <c r="B32">
+        <v>20230125</v>
+      </c>
+      <c r="C32" s="6"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>27734299</v>
+      </c>
+      <c r="B33">
+        <v>20230125</v>
+      </c>
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>17047491</v>
+      </c>
+      <c r="B34">
+        <v>20230125</v>
+      </c>
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>92869150</v>
+      </c>
+      <c r="B35">
+        <v>20230125</v>
+      </c>
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>94196595</v>
+      </c>
+      <c r="B36">
+        <v>20230125</v>
+      </c>
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>20231784</v>
+      </c>
+      <c r="B37">
+        <v>20230125</v>
+      </c>
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>28533635</v>
+      </c>
+      <c r="B38">
+        <v>20230125</v>
+      </c>
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>27303681</v>
+      </c>
+      <c r="B39">
+        <v>20230125</v>
+      </c>
+      <c r="C39" s="6"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>29050435</v>
+      </c>
+      <c r="B40">
+        <v>20230125</v>
+      </c>
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>25871935</v>
+      </c>
+      <c r="B41">
+        <v>20230125</v>
+      </c>
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>25539972</v>
+      </c>
+      <c r="B42">
+        <v>20230125</v>
+      </c>
+      <c r="C42" s="6"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>13632437</v>
+      </c>
+      <c r="B43">
+        <v>20230125</v>
+      </c>
+      <c r="C43" s="6"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>27241376</v>
+      </c>
+      <c r="B44">
+        <v>20230125</v>
+      </c>
+      <c r="C44" s="6"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>5172107</v>
+      </c>
+      <c r="B45">
+        <v>20230125</v>
+      </c>
+      <c r="C45" s="6"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>12099068</v>
+      </c>
+      <c r="B46">
+        <v>20230125</v>
+      </c>
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>11139805</v>
+      </c>
+      <c r="B47">
+        <v>20230125</v>
+      </c>
+      <c r="C47" s="6"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>26349332</v>
+      </c>
+      <c r="B48">
+        <v>20230125</v>
+      </c>
+      <c r="C48" s="6"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>11425626</v>
+      </c>
+      <c r="B49">
+        <v>20230125</v>
+      </c>
+      <c r="C49" s="6"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>14707064</v>
+      </c>
+      <c r="B50">
+        <v>20230125</v>
+      </c>
+      <c r="C50" s="6"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>26411749</v>
+      </c>
+      <c r="B51">
+        <v>20230125</v>
+      </c>
+      <c r="C51" s="6"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>6931994</v>
+      </c>
+      <c r="B52">
+        <v>20230125</v>
+      </c>
+      <c r="C52" s="6"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>6486840</v>
+      </c>
+      <c r="B53">
+        <v>20230125</v>
+      </c>
+      <c r="C53" s="6"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>26932843</v>
+      </c>
+      <c r="B54">
+        <v>20230125</v>
+      </c>
+      <c r="C54" s="6"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>35959549</v>
+      </c>
+      <c r="B55">
+        <v>20230125</v>
+      </c>
+      <c r="C55" s="6"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>27880931</v>
+      </c>
+      <c r="B56">
+        <v>20230125</v>
+      </c>
+      <c r="C56" s="6"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>23417731</v>
+      </c>
+      <c r="B57">
+        <v>20230125</v>
+      </c>
+      <c r="C57" s="6"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>35959549</v>
+      </c>
+      <c r="B58">
+        <v>20230125</v>
+      </c>
+      <c r="C58" s="6"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>27880931</v>
+      </c>
+      <c r="B59">
+        <v>20230125</v>
+      </c>
+      <c r="C59" s="6"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>27568626</v>
+      </c>
+      <c r="B60">
+        <v>20230125</v>
+      </c>
+      <c r="C60" s="6"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>29873143</v>
+      </c>
+      <c r="B61">
+        <v>20230125</v>
+      </c>
+      <c r="C61" s="6"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>8310205</v>
+      </c>
+      <c r="B62">
+        <v>20230125</v>
+      </c>
+      <c r="C62" s="6"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>23175354</v>
+      </c>
+      <c r="B63">
+        <v>20230125</v>
+      </c>
+      <c r="C63" s="6"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>92898243</v>
+      </c>
+      <c r="B64">
+        <v>20230125</v>
+      </c>
+      <c r="C64" s="6"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>11942885</v>
+      </c>
+      <c r="B65">
+        <v>20230125</v>
+      </c>
+      <c r="C65" s="6"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>32450488</v>
+      </c>
+      <c r="B66">
+        <v>20230125</v>
+      </c>
+      <c r="C66" s="6"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>5699057</v>
+      </c>
+      <c r="B67">
+        <v>20230125</v>
+      </c>
+      <c r="C67" s="6"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>12062626</v>
+      </c>
+      <c r="B68">
+        <v>20230125</v>
+      </c>
+      <c r="C68" s="6"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>14519407</v>
+      </c>
+      <c r="B69">
+        <v>20230125</v>
+      </c>
+      <c r="C69" s="6"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>31498548</v>
+      </c>
+      <c r="B70">
+        <v>20230125</v>
+      </c>
+      <c r="C70" s="6"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>25379158</v>
+      </c>
+      <c r="B71">
+        <v>20230125</v>
+      </c>
+      <c r="C71" s="6"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>22749003</v>
+      </c>
+      <c r="B72">
+        <v>20230125</v>
+      </c>
+      <c r="C72" s="6"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>12128869</v>
+      </c>
+      <c r="B73">
+        <v>20230125</v>
+      </c>
+      <c r="C73" s="6"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>26074710</v>
+      </c>
+      <c r="B74">
+        <v>20230125</v>
+      </c>
+      <c r="C74" s="6"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>13340126</v>
+      </c>
+      <c r="B75">
+        <v>20230125</v>
+      </c>
+      <c r="C75" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -1211,7 +2042,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1246,7 +2077,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FCD75B7-3767-4AF4-8551-2556E8D90A6B}">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>

<commit_message>
[UPDATE][FEATURE] ENQ y nuevos casos Extraccion
REGRE ENQ Y  NUEVOS CASOSDE DEPOSITOS EN EFEC

Regresion ENQ TEST-9522

Se crearon nuevos casos de Extraccion, EXT01-13
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{825D4A34-D066-49A2-93BA-99C6D994E65B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C12D639-F5B2-4C9C-9CF1-0F8F60863A6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="111">
   <si>
     <t>Nombre</t>
   </si>
@@ -190,9 +190,6 @@
     <t>Tes11</t>
   </si>
   <si>
-    <t>10.169.1.7</t>
-  </si>
-  <si>
     <t>Tes10</t>
   </si>
   <si>
@@ -353,6 +350,15 @@
   </si>
   <si>
     <t>F00401</t>
+  </si>
+  <si>
+    <t>F00620</t>
+  </si>
+  <si>
+    <t>020</t>
+  </si>
+  <si>
+    <t>10.169.1.7:8080</t>
   </si>
 </sst>
 </file>
@@ -697,14 +703,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -717,7 +723,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
@@ -744,7 +750,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>54</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -774,7 +780,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -801,7 +807,7 @@
         <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -814,10 +820,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,7 +860,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>23</v>
@@ -870,103 +876,103 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>23</v>
@@ -974,23 +980,23 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>22</v>
@@ -998,15 +1004,15 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C23">
         <v>319</v>
@@ -1014,31 +1020,31 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>22</v>
@@ -1046,7 +1052,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>22</v>
@@ -1054,7 +1060,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>22</v>
@@ -1062,7 +1068,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>22</v>
@@ -1070,7 +1076,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>22</v>
@@ -1078,10 +1084,18 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1107,16 +1121,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
         <v>102</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>103</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>104</v>
-      </c>
-      <c r="D1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1127,7 +1141,7 @@
         <v>20230125</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D2">
         <v>402</v>
@@ -1141,7 +1155,7 @@
         <v>20230125</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3">
         <v>402</v>
@@ -1155,7 +1169,7 @@
         <v>20230125</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D4">
         <v>490</v>
@@ -1169,7 +1183,7 @@
         <v>20230125</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5">
         <v>490</v>
@@ -1183,7 +1197,7 @@
         <v>20230125</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D6">
         <v>402</v>
@@ -1197,7 +1211,7 @@
         <v>20230125</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D7">
         <v>402</v>
@@ -1211,7 +1225,7 @@
         <v>20230125</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8">
         <v>402</v>
@@ -1225,7 +1239,7 @@
         <v>20230125</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D9">
         <v>402</v>
@@ -1239,7 +1253,7 @@
         <v>20230125</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D10">
         <v>402</v>
@@ -1253,7 +1267,7 @@
         <v>20230125</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D11">
         <v>402</v>
@@ -1267,7 +1281,7 @@
         <v>20230125</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12">
         <v>490</v>
@@ -1281,7 +1295,7 @@
         <v>20230125</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D13">
         <v>490</v>
@@ -1295,7 +1309,7 @@
         <v>20230125</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D14">
         <v>490</v>
@@ -1309,7 +1323,7 @@
         <v>20230125</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D15">
         <v>490</v>
@@ -1323,7 +1337,7 @@
         <v>20230125</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D16" s="7">
         <v>490</v>
@@ -1346,7 +1360,7 @@
         <v>20230125</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D18">
         <v>402</v>
@@ -1360,7 +1374,7 @@
         <v>20230125</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D19">
         <v>402</v>
@@ -1374,7 +1388,7 @@
         <v>20230125</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D20">
         <v>402</v>
@@ -2020,21 +2034,21 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" t="s">
         <v>59</v>
       </c>
-      <c r="B18" t="s">
-        <v>60</v>
-      </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[UPDATE] Casos de consulta - Performance r11 r21
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{825D4A34-D066-49A2-93BA-99C6D994E65B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0FFE22-73E1-4F58-BBEE-BEB70C0D10D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
     <sheet name="Test Server" sheetId="2" r:id="rId2"/>
     <sheet name="Users" sheetId="3" r:id="rId3"/>
     <sheet name="DatosNCD" sheetId="7" r:id="rId4"/>
-    <sheet name="Modulos" sheetId="4" r:id="rId5"/>
-    <sheet name="MsgError" sheetId="5" r:id="rId6"/>
-    <sheet name="DataUser" sheetId="6" r:id="rId7"/>
+    <sheet name="Carga Saldos" sheetId="8" r:id="rId5"/>
+    <sheet name="Modulos" sheetId="4" r:id="rId6"/>
+    <sheet name="MsgError" sheetId="5" r:id="rId7"/>
+    <sheet name="DataUser" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="114">
   <si>
     <t>Nombre</t>
   </si>
@@ -190,9 +191,6 @@
     <t>Tes11</t>
   </si>
   <si>
-    <t>10.169.1.7</t>
-  </si>
-  <si>
     <t>Tes10</t>
   </si>
   <si>
@@ -346,13 +344,31 @@
     <t>Tarifario</t>
   </si>
   <si>
+    <t>6002.6060</t>
+  </si>
+  <si>
+    <t>F00401</t>
+  </si>
+  <si>
+    <t>10.169.1.7:8080</t>
+  </si>
+  <si>
+    <t>Num de Cuenta</t>
+  </si>
+  <si>
+    <t>Importe</t>
+  </si>
+  <si>
+    <t>Concepto</t>
+  </si>
+  <si>
+    <t>00730029258</t>
+  </si>
+  <si>
+    <t>18602AME</t>
+  </si>
+  <si>
     <t>6001.6000</t>
-  </si>
-  <si>
-    <t>6002.6060</t>
-  </si>
-  <si>
-    <t>F00401</t>
   </si>
 </sst>
 </file>
@@ -368,18 +384,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -411,10 +421,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,13 +708,13 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -717,7 +727,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
@@ -744,7 +754,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -774,7 +784,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -801,7 +811,7 @@
         <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -816,7 +826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -854,7 +864,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>23</v>
@@ -870,103 +880,103 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>23</v>
@@ -974,23 +984,23 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>22</v>
@@ -998,15 +1008,15 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C23">
         <v>319</v>
@@ -1014,31 +1024,31 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>22</v>
@@ -1046,7 +1056,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>22</v>
@@ -1054,7 +1064,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>22</v>
@@ -1062,7 +1072,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>22</v>
@@ -1070,7 +1080,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>22</v>
@@ -1078,7 +1088,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>22</v>
@@ -1092,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8058F8B-909F-4289-A69E-5DC86994C957}">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,773 +1117,213 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
         <v>102</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>103</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>104</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>17075433</v>
+      </c>
+      <c r="B2" s="7">
+        <v>20230125</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>14519407</v>
-      </c>
-      <c r="B2">
+      <c r="D2" s="7">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>1307838</v>
+      </c>
+      <c r="B3" s="7">
         <v>20230125</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>14519407</v>
-      </c>
-      <c r="B3">
+      <c r="C3" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="7">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>3057183</v>
+      </c>
+      <c r="B4" s="7">
         <v>20230125</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D3">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>31498548</v>
-      </c>
-      <c r="B4">
+      <c r="C4" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="7">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>1433904</v>
+      </c>
+      <c r="B5" s="7">
         <v>20230125</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4">
+      <c r="C5" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="7">
         <v>490</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>31498548</v>
-      </c>
-      <c r="B5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>30728940</v>
+      </c>
+      <c r="B6" s="7">
         <v>20230125</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5">
+      <c r="C6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="7">
         <v>490</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>25379158</v>
-      </c>
-      <c r="B6">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>43426225</v>
+      </c>
+      <c r="B7" s="7">
         <v>20230125</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D6">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>25379158</v>
-      </c>
-      <c r="B7">
+      <c r="C7" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="7">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>20371118</v>
+      </c>
+      <c r="B8" s="7">
         <v>20230125</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D7">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>22749003</v>
-      </c>
-      <c r="B8">
+      <c r="C8" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="7">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>73068401</v>
+      </c>
+      <c r="B9" s="7">
         <v>20230125</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>22749003</v>
-      </c>
-      <c r="B9">
+      <c r="C9" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="7">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>10962379</v>
+      </c>
+      <c r="B10" s="7">
         <v>20230125</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D9">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>12128869</v>
-      </c>
-      <c r="B10">
+      <c r="C10" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="7">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>33338466</v>
+      </c>
+      <c r="B11" s="7">
         <v>20230125</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>12128869</v>
-      </c>
-      <c r="B11">
+      <c r="C11" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="7">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>13367971</v>
+      </c>
+      <c r="B12" s="7">
         <v>20230125</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>26074710</v>
-      </c>
-      <c r="B12">
+      <c r="C12" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="7">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>25401899</v>
+      </c>
+      <c r="B13" s="7">
         <v>20230125</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12">
+      <c r="C13" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="7">
         <v>490</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>26074710</v>
-      </c>
-      <c r="B13">
-        <v>20230125</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D13">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13340126</v>
+        <v>25401899</v>
       </c>
       <c r="B14">
         <v>20230125</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D14">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13340126</v>
+        <v>13562987</v>
       </c>
       <c r="B15">
         <v>20230125</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>107</v>
+      <c r="C15" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="D15">
         <v>490</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
-        <v>26411749</v>
-      </c>
-      <c r="B16" s="7">
-        <v>20230125</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D16" s="7">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>35959549</v>
-      </c>
-      <c r="B17">
-        <v>20230125</v>
-      </c>
-      <c r="C17" s="9"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>18432020</v>
-      </c>
-      <c r="B18">
-        <v>20230125</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18432020</v>
-      </c>
-      <c r="B19">
-        <v>20230125</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D19">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1881859</v>
-      </c>
-      <c r="B20">
-        <v>20230125</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D20">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>18432020</v>
-      </c>
-      <c r="B21">
-        <v>20230125</v>
-      </c>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>30571421352</v>
-      </c>
-      <c r="B22">
-        <v>20230125</v>
-      </c>
-      <c r="C22" s="6"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22809322</v>
-      </c>
-      <c r="B23">
-        <v>20230125</v>
-      </c>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>3296392</v>
-      </c>
-      <c r="B24">
-        <v>20230125</v>
-      </c>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>4855059</v>
-      </c>
-      <c r="B25">
-        <v>20230125</v>
-      </c>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>14407569</v>
-      </c>
-      <c r="B26">
-        <v>20230125</v>
-      </c>
-      <c r="C26" s="6"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>33393013</v>
-      </c>
-      <c r="B27">
-        <v>20230125</v>
-      </c>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>11022835</v>
-      </c>
-      <c r="B28">
-        <v>20230125</v>
-      </c>
-      <c r="C28" s="6"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>23208752</v>
-      </c>
-      <c r="B29">
-        <v>20230125</v>
-      </c>
-      <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>93983321</v>
-      </c>
-      <c r="B30">
-        <v>20230125</v>
-      </c>
-      <c r="C30" s="6"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>27500525</v>
-      </c>
-      <c r="B31">
-        <v>20230125</v>
-      </c>
-      <c r="C31" s="6"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>4375526</v>
-      </c>
-      <c r="B32">
-        <v>20230125</v>
-      </c>
-      <c r="C32" s="6"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>27734299</v>
-      </c>
-      <c r="B33">
-        <v>20230125</v>
-      </c>
-      <c r="C33" s="6"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>17047491</v>
-      </c>
-      <c r="B34">
-        <v>20230125</v>
-      </c>
-      <c r="C34" s="6"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>92869150</v>
-      </c>
-      <c r="B35">
-        <v>20230125</v>
-      </c>
-      <c r="C35" s="6"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>94196595</v>
-      </c>
-      <c r="B36">
-        <v>20230125</v>
-      </c>
-      <c r="C36" s="6"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>20231784</v>
-      </c>
-      <c r="B37">
-        <v>20230125</v>
-      </c>
-      <c r="C37" s="6"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>28533635</v>
-      </c>
-      <c r="B38">
-        <v>20230125</v>
-      </c>
-      <c r="C38" s="6"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>27303681</v>
-      </c>
-      <c r="B39">
-        <v>20230125</v>
-      </c>
-      <c r="C39" s="6"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>29050435</v>
-      </c>
-      <c r="B40">
-        <v>20230125</v>
-      </c>
-      <c r="C40" s="6"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>25871935</v>
-      </c>
-      <c r="B41">
-        <v>20230125</v>
-      </c>
-      <c r="C41" s="6"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>25539972</v>
-      </c>
-      <c r="B42">
-        <v>20230125</v>
-      </c>
-      <c r="C42" s="6"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>13632437</v>
-      </c>
-      <c r="B43">
-        <v>20230125</v>
-      </c>
-      <c r="C43" s="6"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>27241376</v>
-      </c>
-      <c r="B44">
-        <v>20230125</v>
-      </c>
-      <c r="C44" s="6"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>5172107</v>
-      </c>
-      <c r="B45">
-        <v>20230125</v>
-      </c>
-      <c r="C45" s="6"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>12099068</v>
-      </c>
-      <c r="B46">
-        <v>20230125</v>
-      </c>
-      <c r="C46" s="6"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>11139805</v>
-      </c>
-      <c r="B47">
-        <v>20230125</v>
-      </c>
-      <c r="C47" s="6"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>26349332</v>
-      </c>
-      <c r="B48">
-        <v>20230125</v>
-      </c>
-      <c r="C48" s="6"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>11425626</v>
-      </c>
-      <c r="B49">
-        <v>20230125</v>
-      </c>
-      <c r="C49" s="6"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>14707064</v>
-      </c>
-      <c r="B50">
-        <v>20230125</v>
-      </c>
-      <c r="C50" s="6"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>26411749</v>
-      </c>
-      <c r="B51">
-        <v>20230125</v>
-      </c>
-      <c r="C51" s="6"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>6931994</v>
-      </c>
-      <c r="B52">
-        <v>20230125</v>
-      </c>
-      <c r="C52" s="6"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>6486840</v>
-      </c>
-      <c r="B53">
-        <v>20230125</v>
-      </c>
-      <c r="C53" s="6"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>26932843</v>
-      </c>
-      <c r="B54">
-        <v>20230125</v>
-      </c>
-      <c r="C54" s="6"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>35959549</v>
-      </c>
-      <c r="B55">
-        <v>20230125</v>
-      </c>
-      <c r="C55" s="6"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>27880931</v>
-      </c>
-      <c r="B56">
-        <v>20230125</v>
-      </c>
-      <c r="C56" s="6"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>23417731</v>
-      </c>
-      <c r="B57">
-        <v>20230125</v>
-      </c>
-      <c r="C57" s="6"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>35959549</v>
-      </c>
-      <c r="B58">
-        <v>20230125</v>
-      </c>
-      <c r="C58" s="6"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>27880931</v>
-      </c>
-      <c r="B59">
-        <v>20230125</v>
-      </c>
-      <c r="C59" s="6"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>27568626</v>
-      </c>
-      <c r="B60">
-        <v>20230125</v>
-      </c>
-      <c r="C60" s="6"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>29873143</v>
-      </c>
-      <c r="B61">
-        <v>20230125</v>
-      </c>
-      <c r="C61" s="6"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>8310205</v>
-      </c>
-      <c r="B62">
-        <v>20230125</v>
-      </c>
-      <c r="C62" s="6"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>23175354</v>
-      </c>
-      <c r="B63">
-        <v>20230125</v>
-      </c>
-      <c r="C63" s="6"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>92898243</v>
-      </c>
-      <c r="B64">
-        <v>20230125</v>
-      </c>
-      <c r="C64" s="6"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>11942885</v>
-      </c>
-      <c r="B65">
-        <v>20230125</v>
-      </c>
-      <c r="C65" s="6"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>32450488</v>
-      </c>
-      <c r="B66">
-        <v>20230125</v>
-      </c>
-      <c r="C66" s="6"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>5699057</v>
-      </c>
-      <c r="B67">
-        <v>20230125</v>
-      </c>
-      <c r="C67" s="6"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>12062626</v>
-      </c>
-      <c r="B68">
-        <v>20230125</v>
-      </c>
-      <c r="C68" s="6"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>14519407</v>
-      </c>
-      <c r="B69">
-        <v>20230125</v>
-      </c>
-      <c r="C69" s="6"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>31498548</v>
-      </c>
-      <c r="B70">
-        <v>20230125</v>
-      </c>
-      <c r="C70" s="6"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>25379158</v>
-      </c>
-      <c r="B71">
-        <v>20230125</v>
-      </c>
-      <c r="C71" s="6"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>22749003</v>
-      </c>
-      <c r="B72">
-        <v>20230125</v>
-      </c>
-      <c r="C72" s="6"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>12128869</v>
-      </c>
-      <c r="B73">
-        <v>20230125</v>
-      </c>
-      <c r="C73" s="6"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>26074710</v>
-      </c>
-      <c r="B74">
-        <v>20230125</v>
-      </c>
-      <c r="C74" s="6"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>13340126</v>
-      </c>
-      <c r="B75">
-        <v>20230125</v>
-      </c>
-      <c r="C75" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1882,6 +1332,45 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C254FE54-CA8F-4700-A15D-D5898A98510D}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -2020,21 +1509,21 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" t="s">
         <v>59</v>
       </c>
-      <c r="B18" t="s">
-        <v>60</v>
-      </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2042,7 +1531,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2077,7 +1566,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FCD75B7-3767-4AF4-8551-2556E8D90A6B}">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>

<commit_message>
[UPDATE] Se actualizaron scripts y objetos para la ejecucion de las ENQ
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEB701E-849E-42B9-99B2-5AE08DE99BC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEB14E2-758F-4B60-A5BC-9860F25768FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="127">
   <si>
     <t>Nombre</t>
   </si>
@@ -375,6 +375,39 @@
   </si>
   <si>
     <t>020</t>
+  </si>
+  <si>
+    <t>CCUENCA</t>
+  </si>
+  <si>
+    <t>F04033</t>
+  </si>
+  <si>
+    <t>533</t>
+  </si>
+  <si>
+    <t>F04169</t>
+  </si>
+  <si>
+    <t>369</t>
+  </si>
+  <si>
+    <t>F00463</t>
+  </si>
+  <si>
+    <t>JANDINO</t>
+  </si>
+  <si>
+    <t>F00219</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>F00089</t>
+  </si>
+  <si>
+    <t>102</t>
   </si>
 </sst>
 </file>
@@ -830,10 +863,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,6 +1140,71 @@
       <c r="C33" s="4" t="s">
         <v>115</v>
       </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>123</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>125</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="4"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="4"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[FIX][FEATURE] Pruebas performance y casos migrados desde UFT
[FIX] Se cambiaron las propiedades de los objetos para que sean
compatibles en 708

[FEATURE] Ajustes Monetarios (AM05-AM07), Cuentas (C13-C12), Comisiones
(COM35 al COM40), Depositos y Ext (DE01-DE02), Emision chequera
(EC07-EC11), Variacion deudora (VD01)
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C12D639-F5B2-4C9C-9CF1-0F8F60863A6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85492E3-709B-41B4-BCCB-39B1C5A1066E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="120">
   <si>
     <t>Nombre</t>
   </si>
@@ -359,6 +359,33 @@
   </si>
   <si>
     <t>10.169.1.7:8080</t>
+  </si>
+  <si>
+    <t>CCUENCA</t>
+  </si>
+  <si>
+    <t>F04033</t>
+  </si>
+  <si>
+    <t>F04169</t>
+  </si>
+  <si>
+    <t>369</t>
+  </si>
+  <si>
+    <t>F00463</t>
+  </si>
+  <si>
+    <t>JANDINO</t>
+  </si>
+  <si>
+    <t>F00219</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>F00089</t>
   </si>
 </sst>
 </file>
@@ -703,7 +730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -820,10 +847,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,6 +1123,62 @@
       </c>
       <c r="C33" s="4" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>115</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE] Migracion UFT consultas performance MONEX y Res de Cta
MON22 al MON31 - RC21 al RC24
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C12D639-F5B2-4C9C-9CF1-0F8F60863A6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFCCEC3-2F54-409D-A5C0-4090016671F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="122">
   <si>
     <t>Nombre</t>
   </si>
@@ -359,6 +359,39 @@
   </si>
   <si>
     <t>10.169.1.7:8080</t>
+  </si>
+  <si>
+    <t>CCUENCA</t>
+  </si>
+  <si>
+    <t>F04033</t>
+  </si>
+  <si>
+    <t>F04169</t>
+  </si>
+  <si>
+    <t>F00463</t>
+  </si>
+  <si>
+    <t>JANDINO</t>
+  </si>
+  <si>
+    <t>F00219</t>
+  </si>
+  <si>
+    <t>F00089</t>
+  </si>
+  <si>
+    <t>533</t>
+  </si>
+  <si>
+    <t>369</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>102</t>
   </si>
 </sst>
 </file>
@@ -703,7 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -820,10 +853,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,6 +1129,62 @@
       </c>
       <c r="C33" s="4" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX][FEATURE] Pruebas Performance y casos migrados de UFT
[FIX] Se cambio propiedades de los objetos para que funcionen en 708

[FEATURE] se agregaron ASUC27 - ASUC41, C14 - C17, CS03 - CS04, F04 -
F06 , CP01 - CP06
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{825D4A34-D066-49A2-93BA-99C6D994E65B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE440CAE-0F95-4B78-A628-1DB5E36B6F7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="119">
   <si>
     <t>Nombre</t>
   </si>
@@ -190,9 +190,6 @@
     <t>Tes11</t>
   </si>
   <si>
-    <t>10.169.1.7</t>
-  </si>
-  <si>
     <t>Tes10</t>
   </si>
   <si>
@@ -353,6 +350,39 @@
   </si>
   <si>
     <t>F00401</t>
+  </si>
+  <si>
+    <t>CCUENCA</t>
+  </si>
+  <si>
+    <t>F04033</t>
+  </si>
+  <si>
+    <t>F04169</t>
+  </si>
+  <si>
+    <t>F00463</t>
+  </si>
+  <si>
+    <t>F00620</t>
+  </si>
+  <si>
+    <t>JANDINO</t>
+  </si>
+  <si>
+    <t>F00219</t>
+  </si>
+  <si>
+    <t>F00089</t>
+  </si>
+  <si>
+    <t>10.169.1.7:8080</t>
+  </si>
+  <si>
+    <t>020</t>
+  </si>
+  <si>
+    <t>019</t>
   </si>
 </sst>
 </file>
@@ -698,13 +728,13 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -717,7 +747,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
@@ -744,7 +774,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -774,7 +804,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -801,7 +831,7 @@
         <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -814,10 +844,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,7 +884,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>23</v>
@@ -870,103 +900,103 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>23</v>
@@ -974,23 +1004,23 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>22</v>
@@ -998,15 +1028,15 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C23">
         <v>319</v>
@@ -1014,31 +1044,31 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>22</v>
@@ -1046,7 +1076,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>22</v>
@@ -1054,7 +1084,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>22</v>
@@ -1062,7 +1092,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>22</v>
@@ -1070,7 +1100,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>22</v>
@@ -1078,10 +1108,74 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>110</v>
+      </c>
+      <c r="C36">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1107,16 +1201,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
         <v>102</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>103</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>104</v>
-      </c>
-      <c r="D1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1127,7 +1221,7 @@
         <v>20230125</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D2">
         <v>402</v>
@@ -1141,7 +1235,7 @@
         <v>20230125</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3">
         <v>402</v>
@@ -1155,7 +1249,7 @@
         <v>20230125</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D4">
         <v>490</v>
@@ -1169,7 +1263,7 @@
         <v>20230125</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5">
         <v>490</v>
@@ -1183,7 +1277,7 @@
         <v>20230125</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D6">
         <v>402</v>
@@ -1197,7 +1291,7 @@
         <v>20230125</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D7">
         <v>402</v>
@@ -1211,7 +1305,7 @@
         <v>20230125</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8">
         <v>402</v>
@@ -1225,7 +1319,7 @@
         <v>20230125</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D9">
         <v>402</v>
@@ -1239,7 +1333,7 @@
         <v>20230125</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D10">
         <v>402</v>
@@ -1253,7 +1347,7 @@
         <v>20230125</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D11">
         <v>402</v>
@@ -1267,7 +1361,7 @@
         <v>20230125</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12">
         <v>490</v>
@@ -1281,7 +1375,7 @@
         <v>20230125</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D13">
         <v>490</v>
@@ -1295,7 +1389,7 @@
         <v>20230125</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D14">
         <v>490</v>
@@ -1309,7 +1403,7 @@
         <v>20230125</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D15">
         <v>490</v>
@@ -1323,7 +1417,7 @@
         <v>20230125</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D16" s="7">
         <v>490</v>
@@ -1346,7 +1440,7 @@
         <v>20230125</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D18">
         <v>402</v>
@@ -1360,7 +1454,7 @@
         <v>20230125</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D19">
         <v>402</v>
@@ -1374,7 +1468,7 @@
         <v>20230125</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D20">
         <v>402</v>
@@ -2020,21 +2114,21 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" t="s">
         <v>59</v>
       </c>
-      <c r="B18" t="s">
-        <v>60</v>
-      </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] Se actualiza excel de usuarios
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE440CAE-0F95-4B78-A628-1DB5E36B6F7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C6E189-D73B-43EB-9810-E93BC3558B52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="122">
   <si>
     <t>Nombre</t>
   </si>
@@ -383,6 +383,15 @@
   </si>
   <si>
     <t>019</t>
+  </si>
+  <si>
+    <t>JBORDOY</t>
+  </si>
+  <si>
+    <t>CRECERAC</t>
+  </si>
+  <si>
+    <t>F00074</t>
   </si>
 </sst>
 </file>
@@ -844,10 +853,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,6 +1185,30 @@
       </c>
       <c r="C40" s="4" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>120</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE] Se agregaron casos de los modulos ASUC 42 - 43 Y CP07
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE440CAE-0F95-4B78-A628-1DB5E36B6F7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D59B829-AFF0-4F92-9080-07AC192002CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="122">
   <si>
     <t>Nombre</t>
   </si>
@@ -383,6 +383,15 @@
   </si>
   <si>
     <t>019</t>
+  </si>
+  <si>
+    <t>JBORDOY</t>
+  </si>
+  <si>
+    <t>CRECERAC</t>
+  </si>
+  <si>
+    <t>F00074</t>
   </si>
 </sst>
 </file>
@@ -844,10 +853,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,6 +1185,30 @@
       </c>
       <c r="C40" s="4" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="4">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>120</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE] Compensacion Coelsa + cambios regresion
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,18 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C6E189-D73B-43EB-9810-E93BC3558B52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03F6315-C918-4313-844B-F8386E48AF81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
     <sheet name="Test Server" sheetId="2" r:id="rId2"/>
     <sheet name="Users" sheetId="3" r:id="rId3"/>
-    <sheet name="DatosNCD" sheetId="7" r:id="rId4"/>
-    <sheet name="Modulos" sheetId="4" r:id="rId5"/>
-    <sheet name="MsgError" sheetId="5" r:id="rId6"/>
-    <sheet name="DataUser" sheetId="6" r:id="rId7"/>
+    <sheet name="Carga Saldos" sheetId="8" r:id="rId4"/>
+    <sheet name="DatosNCD" sheetId="7" r:id="rId5"/>
+    <sheet name="Modulos" sheetId="4" r:id="rId6"/>
+    <sheet name="MsgError" sheetId="5" r:id="rId7"/>
+    <sheet name="DataUser" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="126">
   <si>
     <t>Nombre</t>
   </si>
@@ -392,6 +393,18 @@
   </si>
   <si>
     <t>F00074</t>
+  </si>
+  <si>
+    <t>Cuenta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Importe </t>
+  </si>
+  <si>
+    <t>Concepto</t>
+  </si>
+  <si>
+    <t>18602AME</t>
   </si>
 </sst>
 </file>
@@ -855,7 +868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
@@ -1218,6 +1231,46 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F86E7B-4061-45F1-9FC5-D02253AB0909}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10010656046</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8058F8B-909F-4289-A69E-5DC86994C957}">
   <dimension ref="A1:D75"/>
   <sheetViews>
@@ -2008,7 +2061,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -2169,7 +2222,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2204,7 +2257,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FCD75B7-3767-4AF4-8551-2556E8D90A6B}">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>

<commit_message>
[FEATURE] Migracion de casos UFT
Se agregaron casos de los siguientes modulos
Administracion de Piezas (APT08 - APT16)
Cheques Rechazados (CHR12)
Comisiones (COM41 - COM42)
Consulta Chq Ingresados por Camara y Canje (CICC05 - CICC08)
Cierre de cuenta (CDC10 - CDC12)
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03F6315-C918-4313-844B-F8386E48AF81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FFBDC56-9A4B-4E32-9840-9BD60E7912B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="131">
   <si>
     <t>Nombre</t>
   </si>
@@ -248,9 +248,6 @@
     <t>168</t>
   </si>
   <si>
-    <t>037</t>
-  </si>
-  <si>
     <t>CRECEREM</t>
   </si>
   <si>
@@ -405,6 +402,24 @@
   </si>
   <si>
     <t>18602AME</t>
+  </si>
+  <si>
+    <t>F00068</t>
+  </si>
+  <si>
+    <t>068</t>
+  </si>
+  <si>
+    <t>MSORACE</t>
+  </si>
+  <si>
+    <t>F00419</t>
+  </si>
+  <si>
+    <t>ATORRA</t>
+  </si>
+  <si>
+    <t>CRECERAB</t>
   </si>
 </sst>
 </file>
@@ -796,7 +811,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -866,10 +881,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,28 +988,28 @@
         <v>71</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>73</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>67</v>
@@ -1002,23 +1017,23 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>23</v>
@@ -1026,23 +1041,23 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>22</v>
@@ -1050,15 +1065,15 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C23">
         <v>319</v>
@@ -1066,31 +1081,31 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>22</v>
@@ -1098,7 +1113,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>22</v>
@@ -1106,7 +1121,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>22</v>
@@ -1114,7 +1129,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>22</v>
@@ -1122,7 +1137,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>22</v>
@@ -1130,7 +1145,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>22</v>
@@ -1138,15 +1153,15 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>22</v>
@@ -1154,7 +1169,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C35">
         <v>533</v>
@@ -1162,7 +1177,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C36">
         <v>369</v>
@@ -1170,15 +1185,15 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C38">
         <v>102</v>
@@ -1186,15 +1201,15 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>23</v>
@@ -1202,7 +1217,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C41">
         <v>173</v>
@@ -1210,18 +1225,58 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>125</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>128</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1234,7 +1289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F86E7B-4061-45F1-9FC5-D02253AB0909}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1245,13 +1300,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" t="s">
         <v>122</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>123</v>
-      </c>
-      <c r="C1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1262,7 +1317,7 @@
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1287,16 +1342,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
         <v>101</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>102</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>103</v>
-      </c>
-      <c r="D1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1307,7 +1362,7 @@
         <v>20230125</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2">
         <v>402</v>
@@ -1321,7 +1376,7 @@
         <v>20230125</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D3">
         <v>402</v>
@@ -1335,7 +1390,7 @@
         <v>20230125</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D4">
         <v>490</v>
@@ -1349,7 +1404,7 @@
         <v>20230125</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5">
         <v>490</v>
@@ -1363,7 +1418,7 @@
         <v>20230125</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6">
         <v>402</v>
@@ -1377,7 +1432,7 @@
         <v>20230125</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D7">
         <v>402</v>
@@ -1391,7 +1446,7 @@
         <v>20230125</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D8">
         <v>402</v>
@@ -1405,7 +1460,7 @@
         <v>20230125</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D9">
         <v>402</v>
@@ -1419,7 +1474,7 @@
         <v>20230125</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D10">
         <v>402</v>
@@ -1433,7 +1488,7 @@
         <v>20230125</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D11">
         <v>402</v>
@@ -1447,7 +1502,7 @@
         <v>20230125</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D12">
         <v>490</v>
@@ -1461,7 +1516,7 @@
         <v>20230125</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D13">
         <v>490</v>
@@ -1475,7 +1530,7 @@
         <v>20230125</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D14">
         <v>490</v>
@@ -1489,7 +1544,7 @@
         <v>20230125</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D15">
         <v>490</v>
@@ -1503,7 +1558,7 @@
         <v>20230125</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D16" s="7">
         <v>490</v>
@@ -1526,7 +1581,7 @@
         <v>20230125</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D18">
         <v>402</v>
@@ -1540,7 +1595,7 @@
         <v>20230125</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D19">
         <v>402</v>
@@ -1554,7 +1609,7 @@
         <v>20230125</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D20">
         <v>402</v>

</xml_diff>

<commit_message>
[FEATURE] Posteos - migracion
Migracion de UFT PST04, 05 y 06
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03F6315-C918-4313-844B-F8386E48AF81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7F11AD-D428-4990-AADE-50E93D71C9BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="135">
   <si>
     <t>Nombre</t>
   </si>
@@ -245,12 +245,6 @@
     <t>F00743</t>
   </si>
   <si>
-    <t>168</t>
-  </si>
-  <si>
-    <t>037</t>
-  </si>
-  <si>
     <t>CRECEREM</t>
   </si>
   <si>
@@ -405,6 +399,39 @@
   </si>
   <si>
     <t>18602AME</t>
+  </si>
+  <si>
+    <t>F00068</t>
+  </si>
+  <si>
+    <t>068</t>
+  </si>
+  <si>
+    <t>MSORACE</t>
+  </si>
+  <si>
+    <t>F00419</t>
+  </si>
+  <si>
+    <t>ATORRA</t>
+  </si>
+  <si>
+    <t>CRECERAB</t>
+  </si>
+  <si>
+    <t>F00019</t>
+  </si>
+  <si>
+    <t>F02171</t>
+  </si>
+  <si>
+    <t>F00103</t>
+  </si>
+  <si>
+    <t>F02582</t>
+  </si>
+  <si>
+    <t>FMASTROIANNI</t>
   </si>
 </sst>
 </file>
@@ -446,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -467,6 +494,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,7 +826,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -866,10 +896,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,7 +995,7 @@
         <v>70</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -973,28 +1003,28 @@
         <v>71</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>73</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>67</v>
@@ -1002,23 +1032,23 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>23</v>
@@ -1026,23 +1056,23 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>22</v>
@@ -1050,15 +1080,15 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C23">
         <v>319</v>
@@ -1066,31 +1096,31 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>22</v>
@@ -1098,7 +1128,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>22</v>
@@ -1106,7 +1136,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>22</v>
@@ -1114,7 +1144,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>22</v>
@@ -1122,7 +1152,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>22</v>
@@ -1130,7 +1160,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>22</v>
@@ -1138,15 +1168,15 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>22</v>
@@ -1154,7 +1184,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C35">
         <v>533</v>
@@ -1162,7 +1192,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C36">
         <v>369</v>
@@ -1170,15 +1200,15 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C38">
         <v>102</v>
@@ -1186,15 +1216,15 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>23</v>
@@ -1202,7 +1232,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C41">
         <v>173</v>
@@ -1210,19 +1240,141 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>68</v>
       </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>124</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>126</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>128</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>130</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>131</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>132</v>
+      </c>
+      <c r="C51" s="10">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>133</v>
+      </c>
+      <c r="C52" s="10">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>134</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C54" s="10"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C55" s="10"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C56" s="10"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C57" s="10"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C58" s="10"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C59" s="10"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C60" s="10"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C61" s="10"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C62" s="10"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C63" s="10"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C64" s="10"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" s="10"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" s="10"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1234,7 +1386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F86E7B-4061-45F1-9FC5-D02253AB0909}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1245,13 +1397,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" t="s">
         <v>122</v>
-      </c>
-      <c r="B1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1262,7 +1414,7 @@
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1287,16 +1439,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
         <v>101</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>102</v>
-      </c>
-      <c r="C1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1307,7 +1459,7 @@
         <v>20230125</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D2">
         <v>402</v>
@@ -1321,7 +1473,7 @@
         <v>20230125</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D3">
         <v>402</v>
@@ -1335,7 +1487,7 @@
         <v>20230125</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D4">
         <v>490</v>
@@ -1349,7 +1501,7 @@
         <v>20230125</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D5">
         <v>490</v>
@@ -1363,7 +1515,7 @@
         <v>20230125</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D6">
         <v>402</v>
@@ -1377,7 +1529,7 @@
         <v>20230125</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D7">
         <v>402</v>
@@ -1391,7 +1543,7 @@
         <v>20230125</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D8">
         <v>402</v>
@@ -1405,7 +1557,7 @@
         <v>20230125</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D9">
         <v>402</v>
@@ -1419,7 +1571,7 @@
         <v>20230125</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D10">
         <v>402</v>
@@ -1433,7 +1585,7 @@
         <v>20230125</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D11">
         <v>402</v>
@@ -1447,7 +1599,7 @@
         <v>20230125</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D12">
         <v>490</v>
@@ -1461,7 +1613,7 @@
         <v>20230125</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D13">
         <v>490</v>
@@ -1475,7 +1627,7 @@
         <v>20230125</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D14">
         <v>490</v>
@@ -1489,7 +1641,7 @@
         <v>20230125</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D15">
         <v>490</v>
@@ -1503,7 +1655,7 @@
         <v>20230125</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D16" s="7">
         <v>490</v>
@@ -1526,7 +1678,7 @@
         <v>20230125</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D18">
         <v>402</v>
@@ -1540,7 +1692,7 @@
         <v>20230125</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D19">
         <v>402</v>
@@ -1554,7 +1706,7 @@
         <v>20230125</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D20">
         <v>402</v>

</xml_diff>

<commit_message>
[FEATURE] Migracion casos de UFT
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FFBDC56-9A4B-4E32-9840-9BD60E7912B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B692C1-ACC6-46F2-9B70-77B144C0A16D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="137">
   <si>
     <t>Nombre</t>
   </si>
@@ -420,6 +420,24 @@
   </si>
   <si>
     <t>CRECERAB</t>
+  </si>
+  <si>
+    <t>F00019</t>
+  </si>
+  <si>
+    <t>F02171</t>
+  </si>
+  <si>
+    <t>F00103</t>
+  </si>
+  <si>
+    <t>F02582</t>
+  </si>
+  <si>
+    <t>FMASTROIANNI</t>
+  </si>
+  <si>
+    <t>MABRUNI</t>
   </si>
 </sst>
 </file>
@@ -881,10 +899,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,6 +1295,54 @@
       </c>
       <c r="C48" s="4" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>133</v>
+      </c>
+      <c r="C51">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>134</v>
+      </c>
+      <c r="C52">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>135</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>136</v>
+      </c>
+      <c r="C54">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE] Remesas - Emision Chequeras - Cierre de Cuentas - Puntos Neutrales
Se agregaron los siguientes casos: REM11 - REM27, EC12 - EC14, CDC13 -
CDC16, PN01 - PN04
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FFBDC56-9A4B-4E32-9840-9BD60E7912B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA59D963-1111-4DF1-BCDF-FBBD4BF68A42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="137">
   <si>
     <t>Nombre</t>
   </si>
@@ -245,9 +245,6 @@
     <t>F00743</t>
   </si>
   <si>
-    <t>168</t>
-  </si>
-  <si>
     <t>CRECEREM</t>
   </si>
   <si>
@@ -420,6 +417,27 @@
   </si>
   <si>
     <t>CRECERAB</t>
+  </si>
+  <si>
+    <t>F00019</t>
+  </si>
+  <si>
+    <t>F02171</t>
+  </si>
+  <si>
+    <t>F00103</t>
+  </si>
+  <si>
+    <t>F02582</t>
+  </si>
+  <si>
+    <t>FMASTROIANNI</t>
+  </si>
+  <si>
+    <t>MABRUNI</t>
+  </si>
+  <si>
+    <t>F02357</t>
   </si>
 </sst>
 </file>
@@ -811,7 +829,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -881,10 +899,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,7 +998,7 @@
         <v>70</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -993,23 +1011,23 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>67</v>
@@ -1017,23 +1035,23 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>23</v>
@@ -1041,23 +1059,23 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>22</v>
@@ -1065,15 +1083,15 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23">
         <v>319</v>
@@ -1081,31 +1099,31 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>22</v>
@@ -1113,7 +1131,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>22</v>
@@ -1121,7 +1139,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>22</v>
@@ -1129,7 +1147,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>22</v>
@@ -1137,7 +1155,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>22</v>
@@ -1145,7 +1163,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>22</v>
@@ -1153,15 +1171,15 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>22</v>
@@ -1169,7 +1187,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C35">
         <v>533</v>
@@ -1177,7 +1195,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C36">
         <v>369</v>
@@ -1185,15 +1203,15 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C38">
         <v>102</v>
@@ -1201,15 +1219,15 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>23</v>
@@ -1217,7 +1235,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C41">
         <v>173</v>
@@ -1225,15 +1243,15 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>68</v>
@@ -1241,15 +1259,15 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>124</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>23</v>
@@ -1257,26 +1275,82 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>130</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>74</v>
+      <c r="C49" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>131</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>132</v>
+      </c>
+      <c r="C51">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>133</v>
+      </c>
+      <c r="C52">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>134</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>135</v>
+      </c>
+      <c r="C54">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>136</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1300,13 +1374,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
         <v>121</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>122</v>
-      </c>
-      <c r="C1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1317,7 +1391,7 @@
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1342,16 +1416,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
         <v>100</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>101</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>102</v>
-      </c>
-      <c r="D1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1362,7 +1436,7 @@
         <v>20230125</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D2">
         <v>402</v>
@@ -1376,7 +1450,7 @@
         <v>20230125</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3">
         <v>402</v>
@@ -1390,7 +1464,7 @@
         <v>20230125</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4">
         <v>490</v>
@@ -1404,7 +1478,7 @@
         <v>20230125</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D5">
         <v>490</v>
@@ -1418,7 +1492,7 @@
         <v>20230125</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6">
         <v>402</v>
@@ -1432,7 +1506,7 @@
         <v>20230125</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7">
         <v>402</v>
@@ -1446,7 +1520,7 @@
         <v>20230125</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D8">
         <v>402</v>
@@ -1460,7 +1534,7 @@
         <v>20230125</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D9">
         <v>402</v>
@@ -1474,7 +1548,7 @@
         <v>20230125</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D10">
         <v>402</v>
@@ -1488,7 +1562,7 @@
         <v>20230125</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D11">
         <v>402</v>
@@ -1502,7 +1576,7 @@
         <v>20230125</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D12">
         <v>490</v>
@@ -1516,7 +1590,7 @@
         <v>20230125</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D13">
         <v>490</v>
@@ -1530,7 +1604,7 @@
         <v>20230125</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D14">
         <v>490</v>
@@ -1544,7 +1618,7 @@
         <v>20230125</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D15">
         <v>490</v>
@@ -1558,7 +1632,7 @@
         <v>20230125</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D16" s="7">
         <v>490</v>
@@ -1581,7 +1655,7 @@
         <v>20230125</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D18">
         <v>402</v>
@@ -1595,7 +1669,7 @@
         <v>20230125</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D19">
         <v>402</v>
@@ -1609,7 +1683,7 @@
         <v>20230125</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D20">
         <v>402</v>

</xml_diff>

<commit_message>
[FEATURE] Migracion de UFT
Impuestos IMP23, IMP27 - Comisiones Manuales CMA01, CMA10  - Personas
P07, P14 - MAP MAP01, MAP04 - Resumen de Cuenta RC26, RC30
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03F6315-C918-4313-844B-F8386E48AF81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4419DCBE-3CCD-4579-B942-85CB79E12E11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="140">
   <si>
     <t>Nombre</t>
   </si>
@@ -248,9 +248,6 @@
     <t>168</t>
   </si>
   <si>
-    <t>037</t>
-  </si>
-  <si>
     <t>CRECEREM</t>
   </si>
   <si>
@@ -405,6 +402,51 @@
   </si>
   <si>
     <t>18602AME</t>
+  </si>
+  <si>
+    <t>F00068</t>
+  </si>
+  <si>
+    <t>068</t>
+  </si>
+  <si>
+    <t>MSORACE</t>
+  </si>
+  <si>
+    <t>F00419</t>
+  </si>
+  <si>
+    <t>ATORRA</t>
+  </si>
+  <si>
+    <t>CRECERAB</t>
+  </si>
+  <si>
+    <t>F00019</t>
+  </si>
+  <si>
+    <t>F02171</t>
+  </si>
+  <si>
+    <t>F00103</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>F02582</t>
+  </si>
+  <si>
+    <t>FMASTROIANNI</t>
+  </si>
+  <si>
+    <t>MABRUNI</t>
+  </si>
+  <si>
+    <t>F02357</t>
+  </si>
+  <si>
+    <t>F00834</t>
   </si>
 </sst>
 </file>
@@ -796,7 +838,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -866,10 +908,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,28 +1015,28 @@
         <v>71</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>73</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>67</v>
@@ -1002,23 +1044,23 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>23</v>
@@ -1026,23 +1068,23 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>22</v>
@@ -1050,15 +1092,15 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C23">
         <v>319</v>
@@ -1066,31 +1108,31 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>22</v>
@@ -1098,7 +1140,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>22</v>
@@ -1106,7 +1148,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>22</v>
@@ -1114,7 +1156,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>22</v>
@@ -1122,7 +1164,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>22</v>
@@ -1130,7 +1172,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>22</v>
@@ -1138,15 +1180,15 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>22</v>
@@ -1154,7 +1196,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C35">
         <v>533</v>
@@ -1162,7 +1204,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C36">
         <v>369</v>
@@ -1170,15 +1212,15 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C38">
         <v>102</v>
@@ -1186,15 +1228,15 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>23</v>
@@ -1202,7 +1244,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C41">
         <v>173</v>
@@ -1210,18 +1252,122 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>125</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>128</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>133</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>135</v>
+      </c>
+      <c r="C52">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>136</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>137</v>
+      </c>
+      <c r="C54">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>138</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>139</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1234,7 +1380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F86E7B-4061-45F1-9FC5-D02253AB0909}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1245,13 +1391,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" t="s">
         <v>122</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>123</v>
-      </c>
-      <c r="C1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1262,7 +1408,7 @@
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1287,16 +1433,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
         <v>101</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>102</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>103</v>
-      </c>
-      <c r="D1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1307,7 +1453,7 @@
         <v>20230125</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2">
         <v>402</v>
@@ -1321,7 +1467,7 @@
         <v>20230125</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D3">
         <v>402</v>
@@ -1335,7 +1481,7 @@
         <v>20230125</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D4">
         <v>490</v>
@@ -1349,7 +1495,7 @@
         <v>20230125</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5">
         <v>490</v>
@@ -1363,7 +1509,7 @@
         <v>20230125</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6">
         <v>402</v>
@@ -1377,7 +1523,7 @@
         <v>20230125</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D7">
         <v>402</v>
@@ -1391,7 +1537,7 @@
         <v>20230125</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D8">
         <v>402</v>
@@ -1405,7 +1551,7 @@
         <v>20230125</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D9">
         <v>402</v>
@@ -1419,7 +1565,7 @@
         <v>20230125</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D10">
         <v>402</v>
@@ -1433,7 +1579,7 @@
         <v>20230125</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D11">
         <v>402</v>
@@ -1447,7 +1593,7 @@
         <v>20230125</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D12">
         <v>490</v>
@@ -1461,7 +1607,7 @@
         <v>20230125</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D13">
         <v>490</v>
@@ -1475,7 +1621,7 @@
         <v>20230125</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D14">
         <v>490</v>
@@ -1489,7 +1635,7 @@
         <v>20230125</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D15">
         <v>490</v>
@@ -1503,7 +1649,7 @@
         <v>20230125</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D16" s="7">
         <v>490</v>
@@ -1526,7 +1672,7 @@
         <v>20230125</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D18">
         <v>402</v>
@@ -1540,7 +1686,7 @@
         <v>20230125</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D19">
         <v>402</v>
@@ -1554,7 +1700,7 @@
         <v>20230125</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D20">
         <v>402</v>

</xml_diff>

<commit_message>
[FIX][FEATURE] Se agregaron y actualizaron las test suite
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B692C1-ACC6-46F2-9B70-77B144C0A16D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6DDCEB-D05A-4F18-8E8B-5F80B3834BD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="139">
   <si>
     <t>Nombre</t>
   </si>
@@ -438,6 +438,12 @@
   </si>
   <si>
     <t>MABRUNI</t>
+  </si>
+  <si>
+    <t>F00834</t>
+  </si>
+  <si>
+    <t>F02357</t>
   </si>
 </sst>
 </file>
@@ -899,10 +905,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,6 +1349,22 @@
       </c>
       <c r="C54">
         <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>138</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>137</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE][FIX] Pases y Transferencias
PYT01 a PYT02, FIX CHC03
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA59D963-1111-4DF1-BCDF-FBBD4BF68A42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834319DD-0414-48B5-A8B5-D441D5FA337D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="138">
   <si>
     <t>Nombre</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>F02357</t>
+  </si>
+  <si>
+    <t>F00834</t>
   </si>
 </sst>
 </file>
@@ -899,10 +902,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,6 +1354,14 @@
       </c>
       <c r="C55" s="4" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>137</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] [FEATURE] Se actualiza parte 7 regre y se agregan casos
Ajustes monetarios AM08-AM14
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20407"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6DDCEB-D05A-4F18-8E8B-5F80B3834BD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0304E10D-011B-441A-956D-F68F0A5BEF2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="141">
   <si>
     <t>Nombre</t>
   </si>
@@ -444,6 +444,12 @@
   </si>
   <si>
     <t>F02357</t>
+  </si>
+  <si>
+    <t>F00020</t>
+  </si>
+  <si>
+    <t>F00847</t>
   </si>
 </sst>
 </file>
@@ -905,10 +911,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,6 +1371,22 @@
       </c>
       <c r="C56" s="4" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>139</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>140</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE] Migracion UFT - ANSES, Bloq y Desbloq
ANS01, ANS02
BYD21 al BYD26
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20407"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6DDCEB-D05A-4F18-8E8B-5F80B3834BD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48D1BC8-6C1D-4A7D-991A-47ABDF1CB5BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="142">
   <si>
     <t>Nombre</t>
   </si>
@@ -444,6 +444,15 @@
   </si>
   <si>
     <t>F02357</t>
+  </si>
+  <si>
+    <t>F00020</t>
+  </si>
+  <si>
+    <t>F00847</t>
+  </si>
+  <si>
+    <t>F03808</t>
   </si>
 </sst>
 </file>
@@ -905,10 +914,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,6 +1374,30 @@
       </c>
       <c r="C56" s="4" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>139</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>140</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>141</v>
+      </c>
+      <c r="C59">
+        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE][FIX] Puntos Neutrales, Pases y Transferencias, Cheques Rechazados, Automatizacion de Sucursales
Se agregaron los siguientes casos:
PYT03 y PYT04
ASUC45 hasta ASUC49
Se fixearon los siguientes casos:
CHR06, CHR08, CHR12
PN06,PN07
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20407"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6BE2AA-A263-4736-BC41-294408AEA37D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF0FEBD-5FDD-44A9-AA85-82B994A8B104}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="141">
   <si>
     <t>Nombre</t>
   </si>
@@ -447,6 +447,9 @@
   </si>
   <si>
     <t>F00847</t>
+  </si>
+  <si>
+    <t>F03808</t>
   </si>
 </sst>
 </file>
@@ -908,10 +911,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,6 +1387,14 @@
       </c>
       <c r="C58" s="4" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>140</v>
+      </c>
+      <c r="C59">
+        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE] Pases Entre Cajas
Se agregaron casos PAS09 hasta PAS14 excepto el PAS12
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20408"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48D1BC8-6C1D-4A7D-991A-47ABDF1CB5BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9D80EA-D1C0-46E3-8003-5D49CCE44DB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="145">
   <si>
     <t>Nombre</t>
   </si>
@@ -453,6 +453,15 @@
   </si>
   <si>
     <t>F03808</t>
+  </si>
+  <si>
+    <t>F00688</t>
+  </si>
+  <si>
+    <t>F00460</t>
+  </si>
+  <si>
+    <t>060</t>
   </si>
 </sst>
 </file>
@@ -914,10 +923,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1398,6 +1407,22 @@
       </c>
       <c r="C59">
         <v>322</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>143</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE] Se agregaron casos en los siguientes modulos
ASUC58 - ASUC59 , MEP04 - MEP05 - MEP06 , PAS12
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20407"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6DDCEB-D05A-4F18-8E8B-5F80B3834BD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B50EBF4-B0B5-49C2-8A8F-71A86E3F4D60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="146">
   <si>
     <t>Nombre</t>
   </si>
@@ -444,6 +444,27 @@
   </si>
   <si>
     <t>F02357</t>
+  </si>
+  <si>
+    <t>F00688</t>
+  </si>
+  <si>
+    <t>F00020</t>
+  </si>
+  <si>
+    <t>F00847</t>
+  </si>
+  <si>
+    <t>F03808</t>
+  </si>
+  <si>
+    <t>322</t>
+  </si>
+  <si>
+    <t>F00460</t>
+  </si>
+  <si>
+    <t>060</t>
   </si>
 </sst>
 </file>
@@ -905,10 +926,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,6 +1386,46 @@
       </c>
       <c r="C56" s="4" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>140</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>141</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>142</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>139</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>144</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE] Se agregaron casos Pases Entre Cajas y Remesas
Se agregaron los casos PAS23 Y REM28, REM29. Se modifico PAS01
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20408"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B50EBF4-B0B5-49C2-8A8F-71A86E3F4D60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE1B2B1-105B-4A58-803A-3EDAD9C07B50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="148">
   <si>
     <t>Nombre</t>
   </si>
@@ -465,6 +465,12 @@
   </si>
   <si>
     <t>060</t>
+  </si>
+  <si>
+    <t>F00481</t>
+  </si>
+  <si>
+    <t>081</t>
   </si>
 </sst>
 </file>
@@ -926,10 +932,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1426,6 +1432,14 @@
       </c>
       <c r="C61" s="4" t="s">
         <v>145</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>146</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[UPDATE][FEATURE] Modificando OR y agregando dos casos de MONEX
Se agregaron casos MONEX42 Y MONEX43
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20409"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE1B2B1-105B-4A58-803A-3EDAD9C07B50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1920B782-182B-4134-A39D-94CFE4B0D3D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="149">
   <si>
     <t>Nombre</t>
   </si>
@@ -471,6 +471,9 @@
   </si>
   <si>
     <t>081</t>
+  </si>
+  <si>
+    <t>F02214</t>
   </si>
 </sst>
 </file>
@@ -932,10 +935,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,6 +1443,14 @@
       </c>
       <c r="C62" s="4" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>148</v>
+      </c>
+      <c r="C63">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] Mantenimiento scripts Regresion 29-04-24
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20409"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE1B2B1-105B-4A58-803A-3EDAD9C07B50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C16F24C-CF91-44B7-B7CA-5E2FEBD13C67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="153">
   <si>
     <t>Nombre</t>
   </si>
@@ -471,6 +471,21 @@
   </si>
   <si>
     <t>081</t>
+  </si>
+  <si>
+    <t>F02214</t>
+  </si>
+  <si>
+    <t>F00197</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>F00042</t>
+  </si>
+  <si>
+    <t>042</t>
   </si>
 </sst>
 </file>
@@ -932,10 +947,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,6 +1455,30 @@
       </c>
       <c r="C62" s="4" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>148</v>
+      </c>
+      <c r="C63">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>149</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>151</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] se agregó usuario en main data
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20409"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C4717D-0122-430C-8044-B009C83F9CA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64FF9D2-B154-4294-9816-02BF93025617}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="154">
   <si>
     <t>Nombre</t>
   </si>
@@ -486,6 +486,9 @@
   </si>
   <si>
     <t>042</t>
+  </si>
+  <si>
+    <t>F01393</t>
   </si>
 </sst>
 </file>
@@ -947,10 +950,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1479,6 +1482,14 @@
       </c>
       <c r="C65" s="4" t="s">
         <v>152</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>153</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] Se arreglaron casos para los modulos VDF y RC
VDF05, VDF06, VDF08, VDF09, VDF12, VDF14, RC08, RC12, RC18, RC19, RC20
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20409"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B50EBF4-B0B5-49C2-8A8F-71A86E3F4D60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA5906D-39A0-4AA0-8864-29B292DCDE4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="153">
   <si>
     <t>Nombre</t>
   </si>
@@ -465,6 +465,27 @@
   </si>
   <si>
     <t>060</t>
+  </si>
+  <si>
+    <t>F00481</t>
+  </si>
+  <si>
+    <t>081</t>
+  </si>
+  <si>
+    <t>F02214</t>
+  </si>
+  <si>
+    <t>F00197</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>F00042</t>
+  </si>
+  <si>
+    <t>042</t>
   </si>
 </sst>
 </file>
@@ -926,10 +947,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1426,6 +1447,38 @@
       </c>
       <c r="C61" s="4" t="s">
         <v>145</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>146</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>148</v>
+      </c>
+      <c r="C63">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>149</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>151</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE][FIX][UPDATE] Command Line - Reversas en RC - MainData
Se agrego el caso de agregar commandLine a los user existentes. Se
implemento las reversas en los casos de RC y se actualizo el MainData
con la parametria de las fechas.
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64FF9D2-B154-4294-9816-02BF93025617}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7BA3E3-CAD9-4E98-AEC8-826A766BD375}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="Modulos" sheetId="4" r:id="rId6"/>
     <sheet name="MsgError" sheetId="5" r:id="rId7"/>
     <sheet name="DataUser" sheetId="6" r:id="rId8"/>
+    <sheet name="Fechas" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="166">
   <si>
     <t>Nombre</t>
   </si>
@@ -489,6 +490,42 @@
   </si>
   <si>
     <t>F01393</t>
+  </si>
+  <si>
+    <t>Tes12</t>
+  </si>
+  <si>
+    <t>t24tes12</t>
+  </si>
+  <si>
+    <t>10.169.1.36</t>
+  </si>
+  <si>
+    <t>COB</t>
+  </si>
+  <si>
+    <t>DIA</t>
+  </si>
+  <si>
+    <t>VALOR</t>
+  </si>
+  <si>
+    <t>TES10</t>
+  </si>
+  <si>
+    <t>TES11</t>
+  </si>
+  <si>
+    <t>TES12</t>
+  </si>
+  <si>
+    <t>20230612</t>
+  </si>
+  <si>
+    <t>20230901</t>
+  </si>
+  <si>
+    <t>20230829</t>
   </si>
 </sst>
 </file>
@@ -833,9 +870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -884,8 +919,12 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>156</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -896,7 +935,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -941,7 +982,12 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
+      <c r="A6" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" t="s">
+        <v>155</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -952,7 +998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+    <sheetView topLeftCell="A57" workbookViewId="0">
       <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
@@ -2559,4 +2605,91 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6F6505-72C5-407A-9E87-8F1DBAE9B164}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>702</v>
+      </c>
+      <c r="C1">
+        <v>708</v>
+      </c>
+      <c r="D1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[FEATURE][FIX] ASUC, Posteo y CDS
Se fixearon ASUC 11, 12, 13, 21, 23, 24, 25 Y 44
Se agrego el caso PST13
Se modificaron 3 lbl que tenian la palabra primero/a
Se cambio el titulo de los casos CDS8 hasta el 12
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64FF9D2-B154-4294-9816-02BF93025617}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2196BEFD-23B1-4D36-A2E7-C55E48582875}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -950,10 +950,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1491,6 +1491,9 @@
       <c r="C66" s="4" t="s">
         <v>150</v>
       </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C67" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[FEATURE] Deposito y Extracciones, Posteo
Se agregaron los casos DE15 y DE16
Se agregaron los casos PST 14 hasta PST17
Se agrego un caso para revisar de Posteo
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7BA3E3-CAD9-4E98-AEC8-826A766BD375}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A9687D-07EA-49C7-B5C7-7DEBBD394B82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="169">
   <si>
     <t>Nombre</t>
   </si>
@@ -526,6 +526,15 @@
   </si>
   <si>
     <t>20230829</t>
+  </si>
+  <si>
+    <t>F00282</t>
+  </si>
+  <si>
+    <t>082</t>
+  </si>
+  <si>
+    <t>F00482</t>
   </si>
 </sst>
 </file>
@@ -996,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,6 +1545,22 @@
       </c>
       <c r="C66" s="4" t="s">
         <v>150</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>166</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>168</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2611,7 +2636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6F6505-72C5-407A-9E87-8F1DBAE9B164}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[FIX]Common Steps, APT, RC
se arreglo RC05, APT03 y ajustes monetarios carga masiva
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7BA3E3-CAD9-4E98-AEC8-826A766BD375}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0FDBAD-6249-4869-BD0B-A3105F720977}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="DataUser" sheetId="6" r:id="rId8"/>
     <sheet name="Fechas" sheetId="9" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Carga Saldos'!$A$1:$F$192</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="360">
   <si>
     <t>Nombre</t>
   </si>
@@ -498,9 +501,6 @@
     <t>t24tes12</t>
   </si>
   <si>
-    <t>10.169.1.36</t>
-  </si>
-  <si>
     <t>COB</t>
   </si>
   <si>
@@ -526,16 +526,609 @@
   </si>
   <si>
     <t>20230829</t>
+  </si>
+  <si>
+    <t>sapa2122lx-vip.bancocredicoop.coop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11450157481 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03230059240 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10060347141 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11080064566 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12580016873 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11396201787 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10150076223 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03405529110 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13240145445 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11370044717 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12930072463 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12810024894 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10560084041 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13640011652 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13460081318 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11190096323 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12520034239 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12260119610 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">04970101565 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10320039887 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11000112759 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10720198294 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11370060915 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03880065530 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">02600003665 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00080031833 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">01480029806 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11450064639 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10590131319 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00240127202 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10930393717 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10630179471 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11480029721 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00830413494 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">02190146193 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10180130203 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00690059296 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">01560012823 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12306204458 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">02650033717 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10010552085 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11680050224 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13180116187 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12880617116 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00385454397 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">01170103159 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11240036538 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11576205327 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10260159191 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03740026512 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03570015560 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10380505120 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">01275372153 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00320076608 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10490061802 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11050100658 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10760058301 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03500015064 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03445103916 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00015853015 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10910211970 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13450026215 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12300016631 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10830113837 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10326209059 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12440133573 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03160093053 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13190176575 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12190083139 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12400203384 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10950217871 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00795010086 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10300022865 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10630402627 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13640115163 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11420138131 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">01080165573 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10070018723 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11350032974 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03190196232 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03440109728 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">14900019425 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13440074198 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10100099137 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">14340133361 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10300240049 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">02740195622 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13710091218 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12910028712 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11400165979 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12720174614 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13490011693 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10540066810 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13150013946 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10250141650 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">02930059431 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11320267205 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12300036343 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11680248641 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03750193466 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10620117469 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00960145065 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10430208230 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00110107606 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13530015834 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">02885010842 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10850234873 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13690202011 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00015235581 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13220092806 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">01730052707 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10250141636 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12290225011 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11120174734 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11160193681 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10370241975 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00250282128 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">01480029813 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11000050545 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">14320038967 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11406207871 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11370083398 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13226207695 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10910192561 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">15370186828 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00475192293 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">02740645899 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00850090835 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00470114159 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10276205518 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">02920054945 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10960083127 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12660023139 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00210034499 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00080086000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">01365003118 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03595000336 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">02850008834 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13240166174 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12920094505 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03505023644 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12660063218 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10820077392 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10930015684 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">01560037257 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11400153989 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11740139867 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00675160777 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12540020430 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13360040631 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">01685122755 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11400123276 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12650062687 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10730037635 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">04295444433 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11000011032 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03710067923 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10930481083 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12590031651 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00010454480 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11410212302 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00890124792 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">01035156162 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10156208053 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11370144820 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13186208169 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12590016234 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11410213435 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12590002668 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11380012773 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">02265027828 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12590031989 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13770060524 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">01275436011 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10190191410 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13360042873 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12300124046 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13695623750 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13700027865 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10860133029 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13200081707 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11160208066 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00050070026 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">01395137447 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11370032628 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00190102551 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">02765010463 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12910062732 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10850262566 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10010330298 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">04945313043 </t>
+  </si>
+  <si>
+    <t>Comentario</t>
+  </si>
+  <si>
+    <t>NO - Monto excede valor permitido para txn LM.ACRED.ASL</t>
+  </si>
+  <si>
+    <t>20230905</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -564,10 +1157,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -588,8 +1182,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -870,12 +1468,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -922,11 +1522,14 @@
       <c r="A6" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>156</v>
+      <c r="B6" s="10" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="http://sapa2122lx-vip.bancocredicoop.coop" xr:uid="{4ABD9D4D-0A0A-4DED-B86D-DD0D95231A94}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1546,18 +2149,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F86E7B-4061-45F1-9FC5-D02253AB0909}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F192"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>121</v>
       </c>
@@ -1567,20 +2169,2178 @@
       <c r="C1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>10010656046</v>
+      <c r="E1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>166</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>1000000</v>
       </c>
       <c r="C2" t="s">
         <v>124</v>
       </c>
+      <c r="E2" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3">
+        <v>1000000</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4">
+        <v>1000000</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5">
+        <v>1000000</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="F5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B6">
+        <v>1000000</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7">
+        <v>1000000</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8">
+        <v>1000000</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9">
+        <v>1000000</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B10">
+        <v>1000000</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="F10" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11">
+        <v>1000000</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12">
+        <v>1000000</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B13">
+        <v>1000000</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14">
+        <v>1000000</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B15">
+        <v>1000000</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B16">
+        <v>1000000</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B17">
+        <v>1000000</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B18">
+        <v>1000000</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B19">
+        <v>1000000</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B20">
+        <v>1000000</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B21">
+        <v>1000000</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B22">
+        <v>1000000</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B23">
+        <v>1000000</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B24">
+        <v>1000000</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B25">
+        <v>1000000</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B26">
+        <v>1000000</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B27">
+        <v>1000000</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B28">
+        <v>1000000</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B29">
+        <v>1000000</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="B30">
+        <v>1000000</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B31">
+        <v>1000000</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="B32">
+        <v>1000000</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B33">
+        <v>1000000</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B34">
+        <v>1000000</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="B35">
+        <v>1000000</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B36">
+        <v>1000000</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B37">
+        <v>1000000</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B38">
+        <v>1000000</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B39">
+        <v>1000000</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B40">
+        <v>1000000</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="F40" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B41">
+        <v>1000000</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B42">
+        <v>1000000</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B43">
+        <v>1000000</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="B44">
+        <v>1000000</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B45">
+        <v>1000000</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B46">
+        <v>1000000</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B47">
+        <v>1000000</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B48">
+        <v>1000000</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B49">
+        <v>1000000</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B50">
+        <v>1000000</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B51">
+        <v>1000000</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B52">
+        <v>1000000</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B53">
+        <v>1000000</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B54">
+        <v>1000000</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="B55">
+        <v>1000000</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="B56">
+        <v>1000000</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="B57">
+        <v>1000000</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B58">
+        <v>1000000</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="B59">
+        <v>1000000</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B60">
+        <v>1000000</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B61">
+        <v>1000000</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="B62">
+        <v>1000000</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B63">
+        <v>1000000</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B64">
+        <v>1000000</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B65">
+        <v>1000000</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B66">
+        <v>1000000</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B67">
+        <v>1000000</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B68">
+        <v>1000000</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="B69">
+        <v>1000000</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B70">
+        <v>1000000</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="B71">
+        <v>1000000</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B72">
+        <v>1000000</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="B73">
+        <v>1000000</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B74">
+        <v>1000000</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="B75">
+        <v>1000000</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="F75" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B76">
+        <v>1000000</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="B77">
+        <v>1000000</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="B78">
+        <v>1000000</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="B79">
+        <v>1000000</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="B80">
+        <v>1000000</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B81">
+        <v>1000000</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B82">
+        <v>1000000</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B83">
+        <v>1000000</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B84">
+        <v>1000000</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="B85">
+        <v>1000000</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B86">
+        <v>1000000</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B87">
+        <v>1000000</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="F87" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B88">
+        <v>1000000</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="B89">
+        <v>1000000</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B90">
+        <v>1000000</v>
+      </c>
+      <c r="E90" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="B91">
+        <v>1000000</v>
+      </c>
+      <c r="E91" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="B92">
+        <v>1000000</v>
+      </c>
+      <c r="E92" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="F92" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="B93">
+        <v>1000000</v>
+      </c>
+      <c r="E93" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="B94">
+        <v>1000000</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="B95">
+        <v>1000000</v>
+      </c>
+      <c r="E95" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="B96">
+        <v>1000000</v>
+      </c>
+      <c r="E96" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="F96" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="B97">
+        <v>1000000</v>
+      </c>
+      <c r="E97" s="6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="B98">
+        <v>1000000</v>
+      </c>
+      <c r="E98" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="F98" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="B99">
+        <v>1000000</v>
+      </c>
+      <c r="E99" s="6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="B100">
+        <v>1000000</v>
+      </c>
+      <c r="E100" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="B101">
+        <v>1000000</v>
+      </c>
+      <c r="E101" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="B102">
+        <v>1000000</v>
+      </c>
+      <c r="E102" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="F102" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="B103">
+        <v>1000000</v>
+      </c>
+      <c r="E103" s="6" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="B104">
+        <v>1000000</v>
+      </c>
+      <c r="E104" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="B105">
+        <v>1000000</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="B106">
+        <v>1000000</v>
+      </c>
+      <c r="E106" s="6" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="B107">
+        <v>1000000</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="B108">
+        <v>1000000</v>
+      </c>
+      <c r="E108" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="F108" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B109">
+        <v>1000000</v>
+      </c>
+      <c r="E109" s="6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="B110">
+        <v>1000000</v>
+      </c>
+      <c r="E110" s="6" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="B111">
+        <v>1000000</v>
+      </c>
+      <c r="E111" s="6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="B112">
+        <v>1000000</v>
+      </c>
+      <c r="E112" s="6" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="B113">
+        <v>1000000</v>
+      </c>
+      <c r="E113" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="F113" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="B114">
+        <v>1000000</v>
+      </c>
+      <c r="E114" s="6" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="B115">
+        <v>1000000</v>
+      </c>
+      <c r="E115" s="6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="B116">
+        <v>1000000</v>
+      </c>
+      <c r="E116" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="B117">
+        <v>1000000</v>
+      </c>
+      <c r="E117" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="B118">
+        <v>1000000</v>
+      </c>
+      <c r="E118" s="6" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="B119">
+        <v>1000000</v>
+      </c>
+      <c r="E119" s="6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="B120">
+        <v>1000000</v>
+      </c>
+      <c r="E120" s="6" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="B121">
+        <v>1000000</v>
+      </c>
+      <c r="E121" s="6" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="B122">
+        <v>1000000</v>
+      </c>
+      <c r="E122" s="6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="B123">
+        <v>1000000</v>
+      </c>
+      <c r="E123" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="F123" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="B124">
+        <v>1000000</v>
+      </c>
+      <c r="E124" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="B125">
+        <v>1000000</v>
+      </c>
+      <c r="E125" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="B126">
+        <v>1000000</v>
+      </c>
+      <c r="E126" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="B127">
+        <v>1000000</v>
+      </c>
+      <c r="E127" s="6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="B128">
+        <v>1000000</v>
+      </c>
+      <c r="E128" s="6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="B129">
+        <v>1000000</v>
+      </c>
+      <c r="E129" s="6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="B130">
+        <v>1000000</v>
+      </c>
+      <c r="E130" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="B131">
+        <v>1000000</v>
+      </c>
+      <c r="E131" s="6" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="B132">
+        <v>1000000</v>
+      </c>
+      <c r="E132" s="6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="B133">
+        <v>1000000</v>
+      </c>
+      <c r="E133" s="6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="B134">
+        <v>1000000</v>
+      </c>
+      <c r="E134" s="6" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="B135">
+        <v>1000000</v>
+      </c>
+      <c r="E135" s="6" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="B136">
+        <v>1000000</v>
+      </c>
+      <c r="E136" s="6" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="B137">
+        <v>1000000</v>
+      </c>
+      <c r="E137" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="B138">
+        <v>1000000</v>
+      </c>
+      <c r="E138" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="B139">
+        <v>1000000</v>
+      </c>
+      <c r="E139" s="6" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="B140">
+        <v>1000000</v>
+      </c>
+      <c r="E140" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="F140" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="B141">
+        <v>1000000</v>
+      </c>
+      <c r="E141" s="6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="B142">
+        <v>1000000</v>
+      </c>
+      <c r="E142" s="6" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="B143">
+        <v>1000000</v>
+      </c>
+      <c r="E143" s="6" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="B144">
+        <v>1000000</v>
+      </c>
+      <c r="E144" s="6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="B145">
+        <v>1000000</v>
+      </c>
+      <c r="E145" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="B146">
+        <v>1000000</v>
+      </c>
+      <c r="E146" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="B147">
+        <v>1000000</v>
+      </c>
+      <c r="E147" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="F147" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="B148">
+        <v>1000000</v>
+      </c>
+      <c r="E148" s="6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="B149">
+        <v>1000000</v>
+      </c>
+      <c r="E149" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="B150">
+        <v>1000000</v>
+      </c>
+      <c r="E150" s="6" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="B151">
+        <v>1000000</v>
+      </c>
+      <c r="E151" s="6" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B152">
+        <v>1000000</v>
+      </c>
+      <c r="E152" s="6" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="B153">
+        <v>1000000</v>
+      </c>
+      <c r="E153" s="6" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="B154">
+        <v>1000000</v>
+      </c>
+      <c r="E154" s="6" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="B155">
+        <v>1000000</v>
+      </c>
+      <c r="E155" s="6" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="B156">
+        <v>1000000</v>
+      </c>
+      <c r="E156" s="6" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="B157">
+        <v>1000000</v>
+      </c>
+      <c r="E157" s="6" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="B158">
+        <v>1000000</v>
+      </c>
+      <c r="E158" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B159">
+        <v>1000000</v>
+      </c>
+      <c r="E159" s="6" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="B160">
+        <v>1000000</v>
+      </c>
+      <c r="E160" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="F160" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="B161">
+        <v>1000000</v>
+      </c>
+      <c r="E161" s="6" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B162">
+        <v>1000000</v>
+      </c>
+      <c r="E162" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="F162" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="B163">
+        <v>1000000</v>
+      </c>
+      <c r="E163" s="6" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="B164">
+        <v>1000000</v>
+      </c>
+      <c r="E164" s="6" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="B165">
+        <v>1000000</v>
+      </c>
+      <c r="E165" s="6" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="B166">
+        <v>1000000</v>
+      </c>
+      <c r="E166" s="6" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="B167">
+        <v>1000000</v>
+      </c>
+      <c r="E167" s="6" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="B168">
+        <v>1000000</v>
+      </c>
+      <c r="E168" s="6" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="B169">
+        <v>1000000</v>
+      </c>
+      <c r="E169" s="6" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="B170">
+        <v>1000000</v>
+      </c>
+      <c r="E170" s="6" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="B171">
+        <v>1000000</v>
+      </c>
+      <c r="E171" s="6" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="B172">
+        <v>1000000</v>
+      </c>
+      <c r="E172" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="F172" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="B173">
+        <v>1000000</v>
+      </c>
+      <c r="E173" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="F173" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="B174">
+        <v>1000000</v>
+      </c>
+      <c r="E174" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="F174" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="B175">
+        <v>1000000</v>
+      </c>
+      <c r="E175" s="6" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="B176">
+        <v>1000000</v>
+      </c>
+      <c r="E176" s="6" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="B177">
+        <v>1000000</v>
+      </c>
+      <c r="E177" s="6" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="B178">
+        <v>1000000</v>
+      </c>
+      <c r="E178" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="B179">
+        <v>1000000</v>
+      </c>
+      <c r="E179" s="6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="B180">
+        <v>1000000</v>
+      </c>
+      <c r="E180" s="6" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="B181">
+        <v>1000000</v>
+      </c>
+      <c r="E181" s="6" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="B182">
+        <v>1000000</v>
+      </c>
+      <c r="E182" s="6" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="B183">
+        <v>1000000</v>
+      </c>
+      <c r="E183" s="6" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B184">
+        <v>1000000</v>
+      </c>
+      <c r="E184" s="6" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="B185">
+        <v>1000000</v>
+      </c>
+      <c r="E185" s="6" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="B186">
+        <v>1000000</v>
+      </c>
+      <c r="E186" s="6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="B187">
+        <v>1000000</v>
+      </c>
+      <c r="E187" s="6" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="B188">
+        <v>1000000</v>
+      </c>
+      <c r="E188" s="6" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="B189">
+        <v>1000000</v>
+      </c>
+      <c r="E189" s="6" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="B190">
+        <v>1000000</v>
+      </c>
+      <c r="E190" s="6" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="B191">
+        <v>1000000</v>
+      </c>
+      <c r="E191" s="6" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="B192">
+        <v>1000000</v>
+      </c>
+      <c r="E192" s="6" t="s">
+        <v>356</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F192" xr:uid="{0777326F-014B-4D17-A6E3-AD22C12F9AF4}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2611,8 +5371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6F6505-72C5-407A-9E87-8F1DBAE9B164}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2625,68 +5385,74 @@
         <v>708</v>
       </c>
       <c r="D1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" t="s">
         <v>160</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>161</v>
-      </c>
-      <c r="F1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>359</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[FIX] Movimientos Automaticos y Cheque Cancelatorio
Se fixeo todo el modulo de MA y CHC01
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20411"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A9687D-07EA-49C7-B5C7-7DEBBD394B82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C967052-FABE-4D41-A2C7-E6072DAB6687}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="171">
   <si>
     <t>Nombre</t>
   </si>
@@ -535,6 +535,12 @@
   </si>
   <si>
     <t>F00482</t>
+  </si>
+  <si>
+    <t>F02244</t>
+  </si>
+  <si>
+    <t>030</t>
   </si>
 </sst>
 </file>
@@ -1005,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,6 +1567,14 @@
       </c>
       <c r="C68" s="4" t="s">
         <v>167</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>169</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se arreglo la parte 7 de regresion
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20411"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C967052-FABE-4D41-A2C7-E6072DAB6687}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BD9D58-6799-4F51-897F-07FF222089E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="176">
   <si>
     <t>Nombre</t>
   </si>
@@ -541,6 +541,21 @@
   </si>
   <si>
     <t>030</t>
+  </si>
+  <si>
+    <t>F01050</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>F00519</t>
+  </si>
+  <si>
+    <t>F00025</t>
+  </si>
+  <si>
+    <t>025</t>
   </si>
 </sst>
 </file>
@@ -1011,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1575,6 +1590,30 @@
       </c>
       <c r="C69" s="4" t="s">
         <v>170</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>171</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>173</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>174</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE][FIX] AM, MON, PST, RC
Se agregaron casos de AM22 y 23
Se fixeo caso 13 de POSTEO
Se agrego caso 44 de MONEX
Se fixeo caso SIN DATA de MA
Se Fixeo el modulo de Resumen de Cuenta (faltan 11 casos)
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20411"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C967052-FABE-4D41-A2C7-E6072DAB6687}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C359FE91-EBB1-46AC-B0BC-B7337660C73E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="176">
   <si>
     <t>Nombre</t>
   </si>
@@ -541,6 +541,21 @@
   </si>
   <si>
     <t>030</t>
+  </si>
+  <si>
+    <t>F01050</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>F00519</t>
+  </si>
+  <si>
+    <t>F00025</t>
+  </si>
+  <si>
+    <t>025</t>
   </si>
 </sst>
 </file>
@@ -1011,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1575,6 +1590,30 @@
       </c>
       <c r="C69" s="4" t="s">
         <v>170</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>171</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>173</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>174</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] Administracion de Piezas, Alta de cuenta MASIVA
Optimizacion del OR - APT. Se modifico el caso alta cuentas MASIVAS.
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20412"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31731A22-07FB-4B36-AA7D-93A9227F14E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9EB352-B24F-4E83-9886-8EF1E59E3F04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="213">
   <si>
     <t>Nombre</t>
   </si>
@@ -345,9 +345,6 @@
     <t>6001.6000</t>
   </si>
   <si>
-    <t>6002.6060</t>
-  </si>
-  <si>
     <t>F00401</t>
   </si>
   <si>
@@ -559,6 +556,117 @@
   </si>
   <si>
     <t>GT</t>
+  </si>
+  <si>
+    <t>10010660988</t>
+  </si>
+  <si>
+    <t>10010660995</t>
+  </si>
+  <si>
+    <t>10010661004</t>
+  </si>
+  <si>
+    <t>10010661042</t>
+  </si>
+  <si>
+    <t>10010661059</t>
+  </si>
+  <si>
+    <t>10010661066</t>
+  </si>
+  <si>
+    <t>10010661073</t>
+  </si>
+  <si>
+    <t>10010661080</t>
+  </si>
+  <si>
+    <t>10010661097</t>
+  </si>
+  <si>
+    <t>10010661103</t>
+  </si>
+  <si>
+    <t>10010661110</t>
+  </si>
+  <si>
+    <t>10010661127</t>
+  </si>
+  <si>
+    <t>10010661134</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>10010661158</t>
+  </si>
+  <si>
+    <t>10010661165</t>
+  </si>
+  <si>
+    <t>10010661172</t>
+  </si>
+  <si>
+    <t>10010661189</t>
+  </si>
+  <si>
+    <t>10010661196</t>
+  </si>
+  <si>
+    <t>10010661202</t>
+  </si>
+  <si>
+    <t>10010661219</t>
+  </si>
+  <si>
+    <t>10010661226</t>
+  </si>
+  <si>
+    <t>10010661233</t>
+  </si>
+  <si>
+    <t>10010661240</t>
+  </si>
+  <si>
+    <t>10010661257</t>
+  </si>
+  <si>
+    <t>10010661264</t>
+  </si>
+  <si>
+    <t>10010661271</t>
+  </si>
+  <si>
+    <t>10010661288</t>
+  </si>
+  <si>
+    <t>10010661295</t>
+  </si>
+  <si>
+    <t>10010661301</t>
+  </si>
+  <si>
+    <t>10010661318</t>
+  </si>
+  <si>
+    <t>10010661325</t>
+  </si>
+  <si>
+    <t>10010661349</t>
+  </si>
+  <si>
+    <t>10010661356</t>
+  </si>
+  <si>
+    <t>10010661363</t>
+  </si>
+  <si>
+    <t>10010661370</t>
+  </si>
+  <si>
+    <t>10010661387</t>
   </si>
 </sst>
 </file>
@@ -574,18 +682,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -600,7 +702,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -618,9 +720,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -909,8 +1009,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -950,15 +1050,15 @@
         <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1018,10 +1118,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" t="s">
         <v>154</v>
-      </c>
-      <c r="B6" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1033,13 +1133,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1053,7 +1153,7 @@
         <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1064,7 +1164,7 @@
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1075,7 +1175,7 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1086,7 +1186,7 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1097,7 +1197,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1108,7 +1208,7 @@
         <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1119,7 +1219,7 @@
         <v>67</v>
       </c>
       <c r="D7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1130,7 +1230,7 @@
         <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1149,7 +1249,7 @@
         <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1192,7 +1292,7 @@
         <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1325,26 +1425,26 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>22</v>
@@ -1352,7 +1452,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C35">
         <v>533</v>
@@ -1360,7 +1460,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C36">
         <v>369</v>
@@ -1368,18 +1468,18 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C38">
         <v>102</v>
@@ -1387,26 +1487,26 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C41">
         <v>173</v>
@@ -1414,7 +1514,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>74</v>
@@ -1422,7 +1522,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>68</v>
@@ -1430,15 +1530,15 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>124</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>23</v>
@@ -1446,15 +1546,15 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>89</v>
@@ -1462,7 +1562,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>74</v>
@@ -1470,23 +1570,23 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C51">
         <v>103</v>
@@ -1494,7 +1594,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C52">
         <v>103</v>
@@ -1502,7 +1602,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>89</v>
@@ -1510,7 +1610,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C54">
         <v>102</v>
@@ -1518,7 +1618,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>23</v>
@@ -1526,7 +1626,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>79</v>
@@ -1534,15 +1634,15 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>68</v>
@@ -1550,15 +1650,15 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>141</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>23</v>
@@ -1566,23 +1666,23 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>143</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>145</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C63">
         <v>221</v>
@@ -1590,50 +1690,50 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>148</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>150</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>164</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>167</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>168</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1644,44 +1744,1750 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F86E7B-4061-45F1-9FC5-D02253AB0909}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
         <v>121</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>122</v>
       </c>
-      <c r="C1" t="s">
-        <v>123</v>
-      </c>
       <c r="D1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>12660063218</v>
+        <v>11450157481</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>4000000</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D2" t="s">
-        <v>172</v>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3230059240</v>
+      </c>
+      <c r="B3">
+        <v>4000000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10060347141</v>
+      </c>
+      <c r="B4">
+        <v>4000000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>11396201787</v>
+      </c>
+      <c r="B5">
+        <v>4000000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10150076223</v>
+      </c>
+      <c r="B6">
+        <v>4000000</v>
+      </c>
+      <c r="C6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3405529110</v>
+      </c>
+      <c r="B7">
+        <v>4000000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>13240145445</v>
+      </c>
+      <c r="B8">
+        <v>4000000</v>
+      </c>
+      <c r="C8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>11370044717</v>
+      </c>
+      <c r="B9">
+        <v>4000000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>12930072463</v>
+      </c>
+      <c r="B10">
+        <v>4000000</v>
+      </c>
+      <c r="C10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>12810024894</v>
+      </c>
+      <c r="B11">
+        <v>4000000</v>
+      </c>
+      <c r="C11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10560084041</v>
+      </c>
+      <c r="B12">
+        <v>4000000</v>
+      </c>
+      <c r="C12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13640011652</v>
+      </c>
+      <c r="B13">
+        <v>4000000</v>
+      </c>
+      <c r="C13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13460081318</v>
+      </c>
+      <c r="B14">
+        <v>4000000</v>
+      </c>
+      <c r="C14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>11190096323</v>
+      </c>
+      <c r="B15">
+        <v>4000000</v>
+      </c>
+      <c r="C15" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>12520034239</v>
+      </c>
+      <c r="B16">
+        <v>4000000</v>
+      </c>
+      <c r="C16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>12260119610</v>
+      </c>
+      <c r="B17">
+        <v>4000000</v>
+      </c>
+      <c r="C17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>4970101565</v>
+      </c>
+      <c r="B18">
+        <v>4000000</v>
+      </c>
+      <c r="C18" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>10320039887</v>
+      </c>
+      <c r="B19">
+        <v>4000000</v>
+      </c>
+      <c r="C19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>11000112759</v>
+      </c>
+      <c r="B20">
+        <v>4000000</v>
+      </c>
+      <c r="C20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>11370060915</v>
+      </c>
+      <c r="B21">
+        <v>4000000</v>
+      </c>
+      <c r="C21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2600003665</v>
+      </c>
+      <c r="B22">
+        <v>4000000</v>
+      </c>
+      <c r="C22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1480029806</v>
+      </c>
+      <c r="B23">
+        <v>4000000</v>
+      </c>
+      <c r="C23" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>11450064639</v>
+      </c>
+      <c r="B24">
+        <v>4000000</v>
+      </c>
+      <c r="C24" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>10720198294</v>
+      </c>
+      <c r="B25">
+        <v>4000000</v>
+      </c>
+      <c r="C25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3880065530</v>
+      </c>
+      <c r="B26">
+        <v>4000000</v>
+      </c>
+      <c r="C26" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>80031833</v>
+      </c>
+      <c r="B27">
+        <v>4000000</v>
+      </c>
+      <c r="C27" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>10590131319</v>
+      </c>
+      <c r="B28">
+        <v>4000000</v>
+      </c>
+      <c r="C28" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>240127202</v>
+      </c>
+      <c r="B29">
+        <v>4000000</v>
+      </c>
+      <c r="C29" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>10930393717</v>
+      </c>
+      <c r="B30">
+        <v>4000000</v>
+      </c>
+      <c r="C30" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>10630179471</v>
+      </c>
+      <c r="B31">
+        <v>4000000</v>
+      </c>
+      <c r="C31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>11480029721</v>
+      </c>
+      <c r="B32">
+        <v>4000000</v>
+      </c>
+      <c r="C32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>830413494</v>
+      </c>
+      <c r="B33">
+        <v>4000000</v>
+      </c>
+      <c r="C33" t="s">
+        <v>123</v>
+      </c>
+      <c r="D33" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2190146193</v>
+      </c>
+      <c r="B34">
+        <v>4000000</v>
+      </c>
+      <c r="C34" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>10180130203</v>
+      </c>
+      <c r="B35">
+        <v>4000000</v>
+      </c>
+      <c r="C35" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>690059296</v>
+      </c>
+      <c r="B36">
+        <v>4000000</v>
+      </c>
+      <c r="C36" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1560012823</v>
+      </c>
+      <c r="B37">
+        <v>4000000</v>
+      </c>
+      <c r="C37" t="s">
+        <v>123</v>
+      </c>
+      <c r="D37" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2650033717</v>
+      </c>
+      <c r="B38">
+        <v>4000000</v>
+      </c>
+      <c r="C38" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>10010552085</v>
+      </c>
+      <c r="B39">
+        <v>4000000</v>
+      </c>
+      <c r="C39" t="s">
+        <v>123</v>
+      </c>
+      <c r="D39" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>11680050224</v>
+      </c>
+      <c r="B40">
+        <v>4000000</v>
+      </c>
+      <c r="C40" t="s">
+        <v>123</v>
+      </c>
+      <c r="D40" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>13180116187</v>
+      </c>
+      <c r="B41">
+        <v>4000000</v>
+      </c>
+      <c r="C41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D41" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>12880617116</v>
+      </c>
+      <c r="B42">
+        <v>4000000</v>
+      </c>
+      <c r="C42" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>385454397</v>
+      </c>
+      <c r="B43">
+        <v>4000000</v>
+      </c>
+      <c r="C43" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1170103159</v>
+      </c>
+      <c r="B44">
+        <v>4000000</v>
+      </c>
+      <c r="C44" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>11240036538</v>
+      </c>
+      <c r="B45">
+        <v>4000000</v>
+      </c>
+      <c r="C45" t="s">
+        <v>123</v>
+      </c>
+      <c r="D45" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>11576205327</v>
+      </c>
+      <c r="B46">
+        <v>4000000</v>
+      </c>
+      <c r="C46" t="s">
+        <v>123</v>
+      </c>
+      <c r="D46" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>10260159191</v>
+      </c>
+      <c r="B47">
+        <v>4000000</v>
+      </c>
+      <c r="C47" t="s">
+        <v>123</v>
+      </c>
+      <c r="D47" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>3740026512</v>
+      </c>
+      <c r="B48">
+        <v>4000000</v>
+      </c>
+      <c r="C48" t="s">
+        <v>123</v>
+      </c>
+      <c r="D48" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>3570015560</v>
+      </c>
+      <c r="B49">
+        <v>4000000</v>
+      </c>
+      <c r="C49" t="s">
+        <v>123</v>
+      </c>
+      <c r="D49" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>12306204458</v>
+      </c>
+      <c r="B50">
+        <v>4000000</v>
+      </c>
+      <c r="C50" t="s">
+        <v>123</v>
+      </c>
+      <c r="D50" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>10380505120</v>
+      </c>
+      <c r="B51">
+        <v>4000000</v>
+      </c>
+      <c r="C51" t="s">
+        <v>123</v>
+      </c>
+      <c r="D51" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1275372153</v>
+      </c>
+      <c r="B52">
+        <v>4000000</v>
+      </c>
+      <c r="C52" t="s">
+        <v>123</v>
+      </c>
+      <c r="D52" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>320076608</v>
+      </c>
+      <c r="B53">
+        <v>4000000</v>
+      </c>
+      <c r="C53" t="s">
+        <v>123</v>
+      </c>
+      <c r="D53" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>10490061802</v>
+      </c>
+      <c r="B54">
+        <v>4000000</v>
+      </c>
+      <c r="C54" t="s">
+        <v>123</v>
+      </c>
+      <c r="D54" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>11050100658</v>
+      </c>
+      <c r="B55">
+        <v>4000000</v>
+      </c>
+      <c r="C55" t="s">
+        <v>123</v>
+      </c>
+      <c r="D55" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>10760058301</v>
+      </c>
+      <c r="B56">
+        <v>4000000</v>
+      </c>
+      <c r="C56" t="s">
+        <v>123</v>
+      </c>
+      <c r="D56" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>3500015064</v>
+      </c>
+      <c r="B57">
+        <v>4000000</v>
+      </c>
+      <c r="C57" t="s">
+        <v>123</v>
+      </c>
+      <c r="D57" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>3445103916</v>
+      </c>
+      <c r="B58">
+        <v>4000000</v>
+      </c>
+      <c r="C58" t="s">
+        <v>123</v>
+      </c>
+      <c r="D58" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>15853015</v>
+      </c>
+      <c r="B59">
+        <v>4000000</v>
+      </c>
+      <c r="C59" t="s">
+        <v>123</v>
+      </c>
+      <c r="D59" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>10910211970</v>
+      </c>
+      <c r="B60">
+        <v>4000000</v>
+      </c>
+      <c r="C60" t="s">
+        <v>123</v>
+      </c>
+      <c r="D60" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>13450026215</v>
+      </c>
+      <c r="B61">
+        <v>4000000</v>
+      </c>
+      <c r="C61" t="s">
+        <v>123</v>
+      </c>
+      <c r="D61" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>12300016631</v>
+      </c>
+      <c r="B62">
+        <v>4000000</v>
+      </c>
+      <c r="C62" t="s">
+        <v>123</v>
+      </c>
+      <c r="D62" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>10830113837</v>
+      </c>
+      <c r="B63">
+        <v>4000000</v>
+      </c>
+      <c r="C63" t="s">
+        <v>123</v>
+      </c>
+      <c r="D63" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>10326209059</v>
+      </c>
+      <c r="B64">
+        <v>4000000</v>
+      </c>
+      <c r="C64" t="s">
+        <v>123</v>
+      </c>
+      <c r="D64" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>12440133573</v>
+      </c>
+      <c r="B65">
+        <v>4000000</v>
+      </c>
+      <c r="C65" t="s">
+        <v>123</v>
+      </c>
+      <c r="D65" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>3160093053</v>
+      </c>
+      <c r="B66">
+        <v>4000000</v>
+      </c>
+      <c r="C66" t="s">
+        <v>123</v>
+      </c>
+      <c r="D66" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>13190176575</v>
+      </c>
+      <c r="B67">
+        <v>4000000</v>
+      </c>
+      <c r="C67" t="s">
+        <v>123</v>
+      </c>
+      <c r="D67" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>12190083139</v>
+      </c>
+      <c r="B68">
+        <v>4000000</v>
+      </c>
+      <c r="C68" t="s">
+        <v>123</v>
+      </c>
+      <c r="D68" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>12400203384</v>
+      </c>
+      <c r="B69">
+        <v>4000000</v>
+      </c>
+      <c r="C69" t="s">
+        <v>123</v>
+      </c>
+      <c r="D69" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>10950217871</v>
+      </c>
+      <c r="B70">
+        <v>4000000</v>
+      </c>
+      <c r="C70" t="s">
+        <v>123</v>
+      </c>
+      <c r="D70" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>795010086</v>
+      </c>
+      <c r="B71">
+        <v>4000000</v>
+      </c>
+      <c r="C71" t="s">
+        <v>123</v>
+      </c>
+      <c r="D71" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>10300022865</v>
+      </c>
+      <c r="B72">
+        <v>4000000</v>
+      </c>
+      <c r="C72" t="s">
+        <v>123</v>
+      </c>
+      <c r="D72" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>10630402627</v>
+      </c>
+      <c r="B73">
+        <v>4000000</v>
+      </c>
+      <c r="C73" t="s">
+        <v>123</v>
+      </c>
+      <c r="D73" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>13640115163</v>
+      </c>
+      <c r="B74">
+        <v>4000000</v>
+      </c>
+      <c r="C74" t="s">
+        <v>123</v>
+      </c>
+      <c r="D74" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>11420138131</v>
+      </c>
+      <c r="B75">
+        <v>4000000</v>
+      </c>
+      <c r="C75" t="s">
+        <v>123</v>
+      </c>
+      <c r="D75" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>1080165573</v>
+      </c>
+      <c r="B76">
+        <v>4000000</v>
+      </c>
+      <c r="C76" t="s">
+        <v>123</v>
+      </c>
+      <c r="D76" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>10070018723</v>
+      </c>
+      <c r="B77">
+        <v>4000000</v>
+      </c>
+      <c r="C77" t="s">
+        <v>123</v>
+      </c>
+      <c r="D77" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>11350032974</v>
+      </c>
+      <c r="B78">
+        <v>4000000</v>
+      </c>
+      <c r="C78" t="s">
+        <v>123</v>
+      </c>
+      <c r="D78" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>3190196232</v>
+      </c>
+      <c r="B79">
+        <v>4000000</v>
+      </c>
+      <c r="C79" t="s">
+        <v>123</v>
+      </c>
+      <c r="D79" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>3440109728</v>
+      </c>
+      <c r="B80">
+        <v>4000000</v>
+      </c>
+      <c r="C80" t="s">
+        <v>123</v>
+      </c>
+      <c r="D80" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>14900019425</v>
+      </c>
+      <c r="B81">
+        <v>4000000</v>
+      </c>
+      <c r="C81" t="s">
+        <v>123</v>
+      </c>
+      <c r="D81" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>13440074198</v>
+      </c>
+      <c r="B82">
+        <v>4000000</v>
+      </c>
+      <c r="C82" t="s">
+        <v>123</v>
+      </c>
+      <c r="D82" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>10100099137</v>
+      </c>
+      <c r="B83">
+        <v>4000000</v>
+      </c>
+      <c r="C83" t="s">
+        <v>123</v>
+      </c>
+      <c r="D83" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>14340133361</v>
+      </c>
+      <c r="B84">
+        <v>4000000</v>
+      </c>
+      <c r="C84" t="s">
+        <v>123</v>
+      </c>
+      <c r="D84" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>10300240049</v>
+      </c>
+      <c r="B85">
+        <v>4000000</v>
+      </c>
+      <c r="C85" t="s">
+        <v>123</v>
+      </c>
+      <c r="D85" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>2740195622</v>
+      </c>
+      <c r="B86">
+        <v>4000000</v>
+      </c>
+      <c r="C86" t="s">
+        <v>123</v>
+      </c>
+      <c r="D86" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>13710091218</v>
+      </c>
+      <c r="B87">
+        <v>4000000</v>
+      </c>
+      <c r="C87" t="s">
+        <v>123</v>
+      </c>
+      <c r="D87" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>12910028712</v>
+      </c>
+      <c r="B88">
+        <v>4000000</v>
+      </c>
+      <c r="C88" t="s">
+        <v>123</v>
+      </c>
+      <c r="D88" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>11400165979</v>
+      </c>
+      <c r="B89">
+        <v>4000000</v>
+      </c>
+      <c r="C89" t="s">
+        <v>123</v>
+      </c>
+      <c r="D89" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>12720174614</v>
+      </c>
+      <c r="B90">
+        <v>4000000</v>
+      </c>
+      <c r="C90" t="s">
+        <v>123</v>
+      </c>
+      <c r="D90" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>13490011693</v>
+      </c>
+      <c r="B91">
+        <v>4000000</v>
+      </c>
+      <c r="C91" t="s">
+        <v>123</v>
+      </c>
+      <c r="D91" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>10540066810</v>
+      </c>
+      <c r="B92">
+        <v>4000000</v>
+      </c>
+      <c r="C92" t="s">
+        <v>123</v>
+      </c>
+      <c r="D92" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>13150013946</v>
+      </c>
+      <c r="B93">
+        <v>4000000</v>
+      </c>
+      <c r="C93" t="s">
+        <v>123</v>
+      </c>
+      <c r="D93" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>10250141650</v>
+      </c>
+      <c r="B94">
+        <v>4000000</v>
+      </c>
+      <c r="C94" t="s">
+        <v>123</v>
+      </c>
+      <c r="D94" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>2930059431</v>
+      </c>
+      <c r="B95">
+        <v>4000000</v>
+      </c>
+      <c r="C95" t="s">
+        <v>123</v>
+      </c>
+      <c r="D95" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>11320267205</v>
+      </c>
+      <c r="B96">
+        <v>4000000</v>
+      </c>
+      <c r="C96" t="s">
+        <v>123</v>
+      </c>
+      <c r="D96" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>12300036343</v>
+      </c>
+      <c r="B97">
+        <v>4000000</v>
+      </c>
+      <c r="C97" t="s">
+        <v>123</v>
+      </c>
+      <c r="D97" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>11680248641</v>
+      </c>
+      <c r="B98">
+        <v>4000000</v>
+      </c>
+      <c r="C98" t="s">
+        <v>123</v>
+      </c>
+      <c r="D98" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>3750193466</v>
+      </c>
+      <c r="B99">
+        <v>4000000</v>
+      </c>
+      <c r="C99" t="s">
+        <v>123</v>
+      </c>
+      <c r="D99" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>960145065</v>
+      </c>
+      <c r="B100">
+        <v>4000000</v>
+      </c>
+      <c r="C100" t="s">
+        <v>123</v>
+      </c>
+      <c r="D100" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>110107606</v>
+      </c>
+      <c r="B101">
+        <v>4000000</v>
+      </c>
+      <c r="C101" t="s">
+        <v>123</v>
+      </c>
+      <c r="D101" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>13530015834</v>
+      </c>
+      <c r="B102">
+        <v>4000000</v>
+      </c>
+      <c r="C102" t="s">
+        <v>123</v>
+      </c>
+      <c r="D102" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>2885010842</v>
+      </c>
+      <c r="B103">
+        <v>4000000</v>
+      </c>
+      <c r="C103" t="s">
+        <v>123</v>
+      </c>
+      <c r="D103" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>13690202011</v>
+      </c>
+      <c r="B104">
+        <v>4000000</v>
+      </c>
+      <c r="C104" t="s">
+        <v>123</v>
+      </c>
+      <c r="D104" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>15235581</v>
+      </c>
+      <c r="B105">
+        <v>4000000</v>
+      </c>
+      <c r="C105" t="s">
+        <v>123</v>
+      </c>
+      <c r="D105" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>13220092806</v>
+      </c>
+      <c r="B106">
+        <v>4000000</v>
+      </c>
+      <c r="C106" t="s">
+        <v>123</v>
+      </c>
+      <c r="D106" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>1730052707</v>
+      </c>
+      <c r="B107">
+        <v>4000000</v>
+      </c>
+      <c r="C107" t="s">
+        <v>123</v>
+      </c>
+      <c r="D107" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>250282128</v>
+      </c>
+      <c r="B108">
+        <v>4000000</v>
+      </c>
+      <c r="C108" t="s">
+        <v>123</v>
+      </c>
+      <c r="D108" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>1480029813</v>
+      </c>
+      <c r="B109">
+        <v>4000000</v>
+      </c>
+      <c r="C109" t="s">
+        <v>123</v>
+      </c>
+      <c r="D109" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>13226207695</v>
+      </c>
+      <c r="B110">
+        <v>4000000</v>
+      </c>
+      <c r="C110" t="s">
+        <v>123</v>
+      </c>
+      <c r="D110" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>15370186828</v>
+      </c>
+      <c r="B111">
+        <v>4000000</v>
+      </c>
+      <c r="C111" t="s">
+        <v>123</v>
+      </c>
+      <c r="D111" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>475192293</v>
+      </c>
+      <c r="B112">
+        <v>4000000</v>
+      </c>
+      <c r="C112" t="s">
+        <v>123</v>
+      </c>
+      <c r="D112" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>2740645899</v>
+      </c>
+      <c r="B113">
+        <v>4000000</v>
+      </c>
+      <c r="C113" t="s">
+        <v>123</v>
+      </c>
+      <c r="D113" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>850090835</v>
+      </c>
+      <c r="B114">
+        <v>4000000</v>
+      </c>
+      <c r="C114" t="s">
+        <v>123</v>
+      </c>
+      <c r="D114" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>470114159</v>
+      </c>
+      <c r="B115">
+        <v>4000000</v>
+      </c>
+      <c r="C115" t="s">
+        <v>123</v>
+      </c>
+      <c r="D115" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>2920054945</v>
+      </c>
+      <c r="B116">
+        <v>4000000</v>
+      </c>
+      <c r="C116" t="s">
+        <v>123</v>
+      </c>
+      <c r="D116" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>210034499</v>
+      </c>
+      <c r="B117">
+        <v>4000000</v>
+      </c>
+      <c r="C117" t="s">
+        <v>123</v>
+      </c>
+      <c r="D117" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>80086000</v>
+      </c>
+      <c r="B118">
+        <v>4000000</v>
+      </c>
+      <c r="C118" t="s">
+        <v>123</v>
+      </c>
+      <c r="D118" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>1365003118</v>
+      </c>
+      <c r="B119">
+        <v>4000000</v>
+      </c>
+      <c r="C119" t="s">
+        <v>123</v>
+      </c>
+      <c r="D119" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>3595000336</v>
+      </c>
+      <c r="B120">
+        <v>4000000</v>
+      </c>
+      <c r="C120" t="s">
+        <v>123</v>
+      </c>
+      <c r="D120" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>2850008834</v>
+      </c>
+      <c r="B121">
+        <v>4000000</v>
+      </c>
+      <c r="C121" t="s">
+        <v>123</v>
+      </c>
+      <c r="D121" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>13240166174</v>
+      </c>
+      <c r="B122">
+        <v>4000000</v>
+      </c>
+      <c r="C122" t="s">
+        <v>123</v>
+      </c>
+      <c r="D122" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>12920094505</v>
+      </c>
+      <c r="B123">
+        <v>4000000</v>
+      </c>
+      <c r="C123" t="s">
+        <v>123</v>
+      </c>
+      <c r="D123" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>3505023644</v>
+      </c>
+      <c r="B124">
+        <v>4000000</v>
+      </c>
+      <c r="C124" t="s">
+        <v>123</v>
+      </c>
+      <c r="D124" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1691,20 +3497,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8058F8B-909F-4289-A69E-5DC86994C957}">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A15" sqref="A15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>100</v>
       </c>
@@ -1717,13 +3524,16 @@
       <c r="D1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>14519407</v>
+        <v>25871935</v>
       </c>
       <c r="B2">
-        <v>20230125</v>
+        <v>20240118</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>104</v>
@@ -1731,13 +3541,16 @@
       <c r="D2">
         <v>402</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>14519407</v>
+        <v>13632437</v>
       </c>
       <c r="B3">
-        <v>20230125</v>
+        <v>20240118</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>104</v>
@@ -1745,41 +3558,50 @@
       <c r="D3">
         <v>402</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>31498548</v>
+        <v>25453849</v>
       </c>
       <c r="B4">
-        <v>20230125</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>105</v>
+        <v>20240118</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="D4">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+      <c r="E4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>31498548</v>
+        <v>17454034</v>
       </c>
       <c r="B5">
-        <v>20230125</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>105</v>
+        <v>20240118</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="D5">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+      <c r="E5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>25379158</v>
+        <v>27241376</v>
       </c>
       <c r="B6">
-        <v>20230125</v>
+        <v>20240118</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>104</v>
@@ -1787,13 +3609,16 @@
       <c r="D6">
         <v>402</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>25379158</v>
+        <v>5172107</v>
       </c>
       <c r="B7">
-        <v>20230125</v>
+        <v>20240118</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>104</v>
@@ -1801,13 +3626,16 @@
       <c r="D7">
         <v>402</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>22749003</v>
+        <v>22828778</v>
       </c>
       <c r="B8">
-        <v>20230125</v>
+        <v>20240118</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>104</v>
@@ -1815,13 +3643,16 @@
       <c r="D8">
         <v>402</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>22749003</v>
+        <v>12099068</v>
       </c>
       <c r="B9">
-        <v>20230125</v>
+        <v>20240118</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>104</v>
@@ -1829,13 +3660,16 @@
       <c r="D9">
         <v>402</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>12128869</v>
+        <v>26349332</v>
       </c>
       <c r="B10">
-        <v>20230125</v>
+        <v>20240118</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>104</v>
@@ -1843,13 +3677,16 @@
       <c r="D10">
         <v>402</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>12128869</v>
+        <v>11425626</v>
       </c>
       <c r="B11">
-        <v>20230125</v>
+        <v>20240118</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>104</v>
@@ -1857,92 +3694,119 @@
       <c r="D11">
         <v>402</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>26074710</v>
+        <v>12004285</v>
       </c>
       <c r="B12">
-        <v>20230125</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>105</v>
+        <v>20240118</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="D12">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+      <c r="E12" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>26074710</v>
+        <v>8513552</v>
       </c>
       <c r="B13">
-        <v>20230125</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>105</v>
+        <v>20240118</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="D13">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+      <c r="E13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13340126</v>
+        <v>14707064</v>
       </c>
       <c r="B14">
-        <v>20230125</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>105</v>
+        <v>20240118</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="D14">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+      <c r="E14" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13340126</v>
+        <v>26411749</v>
       </c>
       <c r="B15">
-        <v>20230125</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>105</v>
+        <v>20240118</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="D15">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+      <c r="E15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
-        <v>26411749</v>
-      </c>
-      <c r="B16" s="7">
-        <v>20230125</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D16" s="7">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>20923333</v>
+      </c>
+      <c r="B16">
+        <v>20240118</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16">
+        <v>402</v>
+      </c>
+      <c r="E16" t="s">
+        <v>190</v>
+      </c>
+      <c r="F16"/>
+    </row>
+    <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>35959549</v>
+        <v>27750280</v>
       </c>
       <c r="B17">
-        <v>20230125</v>
-      </c>
-      <c r="C17" s="9"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20240118</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17">
+        <v>402</v>
+      </c>
+      <c r="E17" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>18432020</v>
+        <v>6931994</v>
       </c>
       <c r="B18">
-        <v>20230125</v>
+        <v>20240118</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>104</v>
@@ -1950,13 +3814,16 @@
       <c r="D18">
         <v>402</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18432020</v>
+        <v>6486840</v>
       </c>
       <c r="B19">
-        <v>20230125</v>
+        <v>20240118</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>104</v>
@@ -1964,13 +3831,16 @@
       <c r="D19">
         <v>402</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1881859</v>
+        <v>31498548</v>
       </c>
       <c r="B20">
-        <v>20230125</v>
+        <v>20240118</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>104</v>
@@ -1978,501 +3848,332 @@
       <c r="D20">
         <v>402</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>18432020</v>
+        <v>25871935</v>
       </c>
       <c r="B21">
-        <v>20230125</v>
-      </c>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20240118</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21">
+        <v>402</v>
+      </c>
+      <c r="E21" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>30571421352</v>
+        <v>13632437</v>
       </c>
       <c r="B22">
-        <v>20230125</v>
-      </c>
-      <c r="C22" s="6"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20240118</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22">
+        <v>402</v>
+      </c>
+      <c r="E22" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22809322</v>
+        <v>25453849</v>
       </c>
       <c r="B23">
-        <v>20230125</v>
-      </c>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20240118</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23">
+        <v>402</v>
+      </c>
+      <c r="E23" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>3296392</v>
+        <v>17454034</v>
       </c>
       <c r="B24">
-        <v>20230125</v>
-      </c>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20240118</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24">
+        <v>402</v>
+      </c>
+      <c r="E24" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>4855059</v>
+        <v>27241376</v>
       </c>
       <c r="B25">
-        <v>20230125</v>
-      </c>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20240118</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25">
+        <v>402</v>
+      </c>
+      <c r="E25" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>14407569</v>
+        <v>5172107</v>
       </c>
       <c r="B26">
-        <v>20230125</v>
-      </c>
-      <c r="C26" s="6"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20240118</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26">
+        <v>402</v>
+      </c>
+      <c r="E26" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>33393013</v>
+        <v>22828778</v>
       </c>
       <c r="B27">
-        <v>20230125</v>
-      </c>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20240118</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27">
+        <v>402</v>
+      </c>
+      <c r="E27" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>11022835</v>
+        <v>12099068</v>
       </c>
       <c r="B28">
-        <v>20230125</v>
-      </c>
-      <c r="C28" s="6"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20240118</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28">
+        <v>402</v>
+      </c>
+      <c r="E28" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>23208752</v>
+        <v>26349332</v>
       </c>
       <c r="B29">
-        <v>20230125</v>
-      </c>
-      <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20240118</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29">
+        <v>402</v>
+      </c>
+      <c r="E29" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>93983321</v>
+        <v>11425626</v>
       </c>
       <c r="B30">
-        <v>20230125</v>
-      </c>
-      <c r="C30" s="6"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20240118</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30">
+        <v>402</v>
+      </c>
+      <c r="E30" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>27500525</v>
+        <v>12004285</v>
       </c>
       <c r="B31">
-        <v>20230125</v>
-      </c>
-      <c r="C31" s="6"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20240118</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31">
+        <v>402</v>
+      </c>
+      <c r="E31" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>4375526</v>
+        <v>8513552</v>
       </c>
       <c r="B32">
-        <v>20230125</v>
-      </c>
-      <c r="C32" s="6"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20240118</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32">
+        <v>402</v>
+      </c>
+      <c r="E32" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>27734299</v>
+        <v>14707064</v>
       </c>
       <c r="B33">
-        <v>20230125</v>
-      </c>
-      <c r="C33" s="6"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20240118</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33">
+        <v>402</v>
+      </c>
+      <c r="E33" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>17047491</v>
+        <v>26411749</v>
       </c>
       <c r="B34">
-        <v>20230125</v>
-      </c>
-      <c r="C34" s="6"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>92869150</v>
+        <v>20240118</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34">
+        <v>402</v>
+      </c>
+      <c r="E34" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>20923333</v>
       </c>
       <c r="B35">
-        <v>20230125</v>
-      </c>
-      <c r="C35" s="6"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20240118</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D35">
+        <v>402</v>
+      </c>
+      <c r="E35" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>94196595</v>
+        <v>27750280</v>
       </c>
       <c r="B36">
-        <v>20230125</v>
-      </c>
-      <c r="C36" s="6"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20240118</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36">
+        <v>402</v>
+      </c>
+      <c r="E36" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>20231784</v>
+        <v>6931994</v>
       </c>
       <c r="B37">
-        <v>20230125</v>
-      </c>
-      <c r="C37" s="6"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20240118</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37">
+        <v>402</v>
+      </c>
+      <c r="E37" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>28533635</v>
+        <v>6486840</v>
       </c>
       <c r="B38">
-        <v>20230125</v>
-      </c>
-      <c r="C38" s="6"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20240118</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D38">
+        <v>402</v>
+      </c>
+      <c r="E38" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>27303681</v>
+        <v>31498548</v>
       </c>
       <c r="B39">
-        <v>20230125</v>
-      </c>
-      <c r="C39" s="6"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>29050435</v>
-      </c>
-      <c r="B40">
-        <v>20230125</v>
-      </c>
-      <c r="C40" s="6"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>25871935</v>
-      </c>
-      <c r="B41">
-        <v>20230125</v>
-      </c>
-      <c r="C41" s="6"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>25539972</v>
-      </c>
-      <c r="B42">
-        <v>20230125</v>
-      </c>
-      <c r="C42" s="6"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>13632437</v>
-      </c>
-      <c r="B43">
-        <v>20230125</v>
-      </c>
-      <c r="C43" s="6"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>27241376</v>
-      </c>
-      <c r="B44">
-        <v>20230125</v>
-      </c>
-      <c r="C44" s="6"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>5172107</v>
-      </c>
-      <c r="B45">
-        <v>20230125</v>
-      </c>
-      <c r="C45" s="6"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>12099068</v>
-      </c>
-      <c r="B46">
-        <v>20230125</v>
-      </c>
-      <c r="C46" s="6"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>11139805</v>
-      </c>
-      <c r="B47">
-        <v>20230125</v>
-      </c>
-      <c r="C47" s="6"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>26349332</v>
-      </c>
-      <c r="B48">
-        <v>20230125</v>
-      </c>
-      <c r="C48" s="6"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>11425626</v>
-      </c>
-      <c r="B49">
-        <v>20230125</v>
-      </c>
-      <c r="C49" s="6"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>14707064</v>
-      </c>
-      <c r="B50">
-        <v>20230125</v>
-      </c>
-      <c r="C50" s="6"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>26411749</v>
-      </c>
-      <c r="B51">
-        <v>20230125</v>
-      </c>
-      <c r="C51" s="6"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>6931994</v>
-      </c>
-      <c r="B52">
-        <v>20230125</v>
-      </c>
-      <c r="C52" s="6"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>6486840</v>
-      </c>
-      <c r="B53">
-        <v>20230125</v>
-      </c>
-      <c r="C53" s="6"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>26932843</v>
-      </c>
-      <c r="B54">
-        <v>20230125</v>
-      </c>
-      <c r="C54" s="6"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>35959549</v>
-      </c>
-      <c r="B55">
-        <v>20230125</v>
-      </c>
-      <c r="C55" s="6"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>27880931</v>
-      </c>
-      <c r="B56">
-        <v>20230125</v>
-      </c>
-      <c r="C56" s="6"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>23417731</v>
-      </c>
-      <c r="B57">
-        <v>20230125</v>
-      </c>
-      <c r="C57" s="6"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>35959549</v>
-      </c>
-      <c r="B58">
-        <v>20230125</v>
-      </c>
-      <c r="C58" s="6"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>27880931</v>
-      </c>
-      <c r="B59">
-        <v>20230125</v>
-      </c>
-      <c r="C59" s="6"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>27568626</v>
-      </c>
-      <c r="B60">
-        <v>20230125</v>
-      </c>
-      <c r="C60" s="6"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>29873143</v>
-      </c>
-      <c r="B61">
-        <v>20230125</v>
-      </c>
-      <c r="C61" s="6"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>8310205</v>
-      </c>
-      <c r="B62">
-        <v>20230125</v>
-      </c>
-      <c r="C62" s="6"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>23175354</v>
-      </c>
-      <c r="B63">
-        <v>20230125</v>
-      </c>
-      <c r="C63" s="6"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>92898243</v>
-      </c>
-      <c r="B64">
-        <v>20230125</v>
-      </c>
-      <c r="C64" s="6"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>11942885</v>
-      </c>
-      <c r="B65">
-        <v>20230125</v>
-      </c>
-      <c r="C65" s="6"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>32450488</v>
-      </c>
-      <c r="B66">
-        <v>20230125</v>
-      </c>
-      <c r="C66" s="6"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>5699057</v>
-      </c>
-      <c r="B67">
-        <v>20230125</v>
-      </c>
-      <c r="C67" s="6"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>12062626</v>
-      </c>
-      <c r="B68">
-        <v>20230125</v>
-      </c>
-      <c r="C68" s="6"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>14519407</v>
-      </c>
-      <c r="B69">
-        <v>20230125</v>
-      </c>
-      <c r="C69" s="6"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>31498548</v>
-      </c>
-      <c r="B70">
-        <v>20230125</v>
-      </c>
-      <c r="C70" s="6"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>25379158</v>
-      </c>
-      <c r="B71">
-        <v>20230125</v>
-      </c>
-      <c r="C71" s="6"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>22749003</v>
-      </c>
-      <c r="B72">
-        <v>20230125</v>
-      </c>
-      <c r="C72" s="6"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>12128869</v>
-      </c>
-      <c r="B73">
-        <v>20230125</v>
-      </c>
-      <c r="C73" s="6"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>26074710</v>
-      </c>
-      <c r="B74">
-        <v>20230125</v>
-      </c>
-      <c r="C74" s="6"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>13340126</v>
-      </c>
-      <c r="B75">
-        <v>20230125</v>
-      </c>
-      <c r="C75" s="6"/>
+        <v>20240118</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39">
+        <v>402</v>
+      </c>
+      <c r="E39" t="s">
+        <v>212</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2490,10 +4191,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="38.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="40.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2651,8 +4352,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2686,9 +4387,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2730,66 +4431,66 @@
         <v>708</v>
       </c>
       <c r="D1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" t="s">
         <v>159</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>160</v>
-      </c>
-      <c r="F1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>164</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>164</v>
       </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>164</v>
       </c>
       <c r="F4" s="4"/>
     </row>

</xml_diff>

<commit_message>
[FIX] Variable Fecha COB en Profiles
Se actualizo la variable global de fecha COB y se actualizaron los
scripts que la invocan
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20412"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9EB352-B24F-4E83-9886-8EF1E59E3F04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8BC257-45DF-434C-BB36-694647A731BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="214">
   <si>
     <t>Nombre</t>
   </si>
@@ -667,6 +667,9 @@
   </si>
   <si>
     <t>10010661387</t>
+  </si>
+  <si>
+    <t>20230830</t>
   </si>
 </sst>
 </file>
@@ -1746,7 +1749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F86E7B-4061-45F1-9FC5-D02253AB0909}">
   <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4417,8 +4420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6F6505-72C5-407A-9E87-8F1DBAE9B164}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4456,7 +4459,9 @@
       <c r="E2" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -4474,7 +4479,9 @@
       <c r="E3" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -4492,7 +4499,9 @@
       <c r="E4" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>213</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[FIX] Administracion de piezas, RegreTES12
Optimizacion del OR - APT y arreglo de scripts regresion
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20412"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8BC257-45DF-434C-BB36-694647A731BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728550AE-674F-486F-9437-0B2335CB6657}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="DataUser" sheetId="6" r:id="rId8"/>
     <sheet name="Fechas" sheetId="9" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Carga Saldos'!$A$1:$D$118</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="213">
   <si>
     <t>Nombre</t>
   </si>
@@ -541,9 +544,6 @@
   </si>
   <si>
     <t>Carga Realizada</t>
-  </si>
-  <si>
-    <t>SI</t>
   </si>
   <si>
     <t>Rol</t>
@@ -1156,7 +1156,7 @@
         <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1167,7 +1167,7 @@
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1178,7 +1178,7 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1189,7 +1189,7 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1200,7 +1200,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1211,7 +1211,7 @@
         <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1222,7 +1222,7 @@
         <v>67</v>
       </c>
       <c r="D7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1233,7 +1233,7 @@
         <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1252,7 +1252,7 @@
         <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1295,7 +1295,7 @@
         <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1434,7 +1434,7 @@
         <v>22</v>
       </c>
       <c r="D32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1477,7 +1477,7 @@
         <v>79</v>
       </c>
       <c r="D37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1504,7 +1504,7 @@
         <v>23</v>
       </c>
       <c r="D40" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1747,9 +1747,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F86E7B-4061-45F1-9FC5-D02253AB0909}">
-  <dimension ref="A1:D124"/>
+  <dimension ref="A1:D118"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1776,13 +1776,10 @@
         <v>11450157481</v>
       </c>
       <c r="B2">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C2" t="s">
         <v>123</v>
-      </c>
-      <c r="D2" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1790,13 +1787,10 @@
         <v>3230059240</v>
       </c>
       <c r="B3">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C3" t="s">
         <v>123</v>
-      </c>
-      <c r="D3" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1804,1696 +1798,1268 @@
         <v>10060347141</v>
       </c>
       <c r="B4">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C4" t="s">
         <v>123</v>
-      </c>
-      <c r="D4" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>11396201787</v>
+        <v>11080064566</v>
       </c>
       <c r="B5">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C5" t="s">
         <v>123</v>
-      </c>
-      <c r="D5" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>10150076223</v>
+        <v>12580016873</v>
       </c>
       <c r="B6">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C6" t="s">
         <v>123</v>
-      </c>
-      <c r="D6" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3405529110</v>
+        <v>11396201787</v>
       </c>
       <c r="B7">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C7" t="s">
         <v>123</v>
-      </c>
-      <c r="D7" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>13240145445</v>
+        <v>10150076223</v>
       </c>
       <c r="B8">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C8" t="s">
         <v>123</v>
-      </c>
-      <c r="D8" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>11370044717</v>
+        <v>3405529110</v>
       </c>
       <c r="B9">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C9" t="s">
         <v>123</v>
-      </c>
-      <c r="D9" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>12930072463</v>
+        <v>13240145445</v>
       </c>
       <c r="B10">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C10" t="s">
         <v>123</v>
-      </c>
-      <c r="D10" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>12810024894</v>
+        <v>11370044717</v>
       </c>
       <c r="B11">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C11" t="s">
         <v>123</v>
-      </c>
-      <c r="D11" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>10560084041</v>
+        <v>12930072463</v>
       </c>
       <c r="B12">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C12" t="s">
         <v>123</v>
-      </c>
-      <c r="D12" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>13640011652</v>
+        <v>12810024894</v>
       </c>
       <c r="B13">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C13" t="s">
         <v>123</v>
-      </c>
-      <c r="D13" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13460081318</v>
+        <v>10560084041</v>
       </c>
       <c r="B14">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C14" t="s">
         <v>123</v>
-      </c>
-      <c r="D14" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>11190096323</v>
+        <v>13640011652</v>
       </c>
       <c r="B15">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C15" t="s">
         <v>123</v>
-      </c>
-      <c r="D15" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>13460081318</v>
+      </c>
+      <c r="B16">
+        <v>100000000</v>
+      </c>
+      <c r="C16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>11190096323</v>
+      </c>
+      <c r="B17">
+        <v>100000000</v>
+      </c>
+      <c r="C17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>12520034239</v>
       </c>
-      <c r="B16">
-        <v>4000000</v>
-      </c>
-      <c r="C16" t="s">
-        <v>123</v>
-      </c>
-      <c r="D16" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="B18">
+        <v>100000000</v>
+      </c>
+      <c r="C18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>12260119610</v>
       </c>
-      <c r="B17">
-        <v>4000000</v>
-      </c>
-      <c r="C17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D17" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="B19">
+        <v>100000000</v>
+      </c>
+      <c r="C19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>4970101565</v>
       </c>
-      <c r="B18">
-        <v>4000000</v>
-      </c>
-      <c r="C18" t="s">
-        <v>123</v>
-      </c>
-      <c r="D18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="B20">
+        <v>100000000</v>
+      </c>
+      <c r="C20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>10320039887</v>
       </c>
-      <c r="B19">
-        <v>4000000</v>
-      </c>
-      <c r="C19" t="s">
-        <v>123</v>
-      </c>
-      <c r="D19" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="B21">
+        <v>100000000</v>
+      </c>
+      <c r="C21" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>11000112759</v>
       </c>
-      <c r="B20">
-        <v>4000000</v>
-      </c>
-      <c r="C20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D20" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="B22">
+        <v>100000000</v>
+      </c>
+      <c r="C22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>11370060915</v>
       </c>
-      <c r="B21">
-        <v>4000000</v>
-      </c>
-      <c r="C21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D21" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="B23">
+        <v>100000000</v>
+      </c>
+      <c r="C23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>2600003665</v>
       </c>
-      <c r="B22">
-        <v>4000000</v>
-      </c>
-      <c r="C22" t="s">
-        <v>123</v>
-      </c>
-      <c r="D22" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="B24">
+        <v>100000000</v>
+      </c>
+      <c r="C24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>1480029806</v>
       </c>
-      <c r="B23">
-        <v>4000000</v>
-      </c>
-      <c r="C23" t="s">
-        <v>123</v>
-      </c>
-      <c r="D23" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="B25">
+        <v>100000000</v>
+      </c>
+      <c r="C25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>11450064639</v>
       </c>
-      <c r="B24">
-        <v>4000000</v>
-      </c>
-      <c r="C24" t="s">
-        <v>123</v>
-      </c>
-      <c r="D24" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="B26">
+        <v>100000000</v>
+      </c>
+      <c r="C26" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>10720198294</v>
       </c>
-      <c r="B25">
-        <v>4000000</v>
-      </c>
-      <c r="C25" t="s">
-        <v>123</v>
-      </c>
-      <c r="D25" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="B27">
+        <v>100000000</v>
+      </c>
+      <c r="C27" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>3880065530</v>
       </c>
-      <c r="B26">
-        <v>4000000</v>
-      </c>
-      <c r="C26" t="s">
-        <v>123</v>
-      </c>
-      <c r="D26" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="B28">
+        <v>100000000</v>
+      </c>
+      <c r="C28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>80031833</v>
       </c>
-      <c r="B27">
-        <v>4000000</v>
-      </c>
-      <c r="C27" t="s">
-        <v>123</v>
-      </c>
-      <c r="D27" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="B29">
+        <v>100000000</v>
+      </c>
+      <c r="C29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>10590131319</v>
       </c>
-      <c r="B28">
-        <v>4000000</v>
-      </c>
-      <c r="C28" t="s">
-        <v>123</v>
-      </c>
-      <c r="D28" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="B30">
+        <v>100000000</v>
+      </c>
+      <c r="C30" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>240127202</v>
       </c>
-      <c r="B29">
-        <v>4000000</v>
-      </c>
-      <c r="C29" t="s">
-        <v>123</v>
-      </c>
-      <c r="D29" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="B31">
+        <v>100000000</v>
+      </c>
+      <c r="C31" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>10930393717</v>
       </c>
-      <c r="B30">
-        <v>4000000</v>
-      </c>
-      <c r="C30" t="s">
-        <v>123</v>
-      </c>
-      <c r="D30" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="B32">
+        <v>100000000</v>
+      </c>
+      <c r="C32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>10630179471</v>
       </c>
-      <c r="B31">
-        <v>4000000</v>
-      </c>
-      <c r="C31" t="s">
-        <v>123</v>
-      </c>
-      <c r="D31" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="B33">
+        <v>100000000</v>
+      </c>
+      <c r="C33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>11480029721</v>
       </c>
-      <c r="B32">
-        <v>4000000</v>
-      </c>
-      <c r="C32" t="s">
-        <v>123</v>
-      </c>
-      <c r="D32" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="B34">
+        <v>100000000</v>
+      </c>
+      <c r="C34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>830413494</v>
       </c>
-      <c r="B33">
-        <v>4000000</v>
-      </c>
-      <c r="C33" t="s">
-        <v>123</v>
-      </c>
-      <c r="D33" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="B35">
+        <v>100000000</v>
+      </c>
+      <c r="C35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>2190146193</v>
       </c>
-      <c r="B34">
-        <v>4000000</v>
-      </c>
-      <c r="C34" t="s">
-        <v>123</v>
-      </c>
-      <c r="D34" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="B36">
+        <v>100000000</v>
+      </c>
+      <c r="C36" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>10180130203</v>
       </c>
-      <c r="B35">
-        <v>4000000</v>
-      </c>
-      <c r="C35" t="s">
-        <v>123</v>
-      </c>
-      <c r="D35" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="B37">
+        <v>100000000</v>
+      </c>
+      <c r="C37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>690059296</v>
       </c>
-      <c r="B36">
-        <v>4000000</v>
-      </c>
-      <c r="C36" t="s">
-        <v>123</v>
-      </c>
-      <c r="D36" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="B38">
+        <v>100000000</v>
+      </c>
+      <c r="C38" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>1560012823</v>
       </c>
-      <c r="B37">
-        <v>4000000</v>
-      </c>
-      <c r="C37" t="s">
-        <v>123</v>
-      </c>
-      <c r="D37" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="B39">
+        <v>100000000</v>
+      </c>
+      <c r="C39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>2650033717</v>
       </c>
-      <c r="B38">
-        <v>4000000</v>
-      </c>
-      <c r="C38" t="s">
-        <v>123</v>
-      </c>
-      <c r="D38" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="B40">
+        <v>100000000</v>
+      </c>
+      <c r="C40" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>10010552085</v>
       </c>
-      <c r="B39">
-        <v>4000000</v>
-      </c>
-      <c r="C39" t="s">
-        <v>123</v>
-      </c>
-      <c r="D39" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="B41">
+        <v>100000000</v>
+      </c>
+      <c r="C41" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>11680050224</v>
       </c>
-      <c r="B40">
-        <v>4000000</v>
-      </c>
-      <c r="C40" t="s">
-        <v>123</v>
-      </c>
-      <c r="D40" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="B42">
+        <v>100000000</v>
+      </c>
+      <c r="C42" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>13180116187</v>
       </c>
-      <c r="B41">
-        <v>4000000</v>
-      </c>
-      <c r="C41" t="s">
-        <v>123</v>
-      </c>
-      <c r="D41" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="B43">
+        <v>100000000</v>
+      </c>
+      <c r="C43" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>12880617116</v>
       </c>
-      <c r="B42">
-        <v>4000000</v>
-      </c>
-      <c r="C42" t="s">
-        <v>123</v>
-      </c>
-      <c r="D42" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="B44">
+        <v>100000000</v>
+      </c>
+      <c r="C44" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>385454397</v>
       </c>
-      <c r="B43">
-        <v>4000000</v>
-      </c>
-      <c r="C43" t="s">
-        <v>123</v>
-      </c>
-      <c r="D43" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="B45">
+        <v>100000000</v>
+      </c>
+      <c r="C45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>1170103159</v>
       </c>
-      <c r="B44">
-        <v>4000000</v>
-      </c>
-      <c r="C44" t="s">
-        <v>123</v>
-      </c>
-      <c r="D44" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="B46">
+        <v>100000000</v>
+      </c>
+      <c r="C46" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>11240036538</v>
       </c>
-      <c r="B45">
-        <v>4000000</v>
-      </c>
-      <c r="C45" t="s">
-        <v>123</v>
-      </c>
-      <c r="D45" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="B47">
+        <v>100000000</v>
+      </c>
+      <c r="C47" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>11576205327</v>
       </c>
-      <c r="B46">
-        <v>4000000</v>
-      </c>
-      <c r="C46" t="s">
-        <v>123</v>
-      </c>
-      <c r="D46" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="B48">
+        <v>100000000</v>
+      </c>
+      <c r="C48" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
         <v>10260159191</v>
       </c>
-      <c r="B47">
-        <v>4000000</v>
-      </c>
-      <c r="C47" t="s">
-        <v>123</v>
-      </c>
-      <c r="D47" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="B49">
+        <v>100000000</v>
+      </c>
+      <c r="C49" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
         <v>3740026512</v>
       </c>
-      <c r="B48">
-        <v>4000000</v>
-      </c>
-      <c r="C48" t="s">
-        <v>123</v>
-      </c>
-      <c r="D48" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="B50">
+        <v>100000000</v>
+      </c>
+      <c r="C50" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
         <v>3570015560</v>
       </c>
-      <c r="B49">
-        <v>4000000</v>
-      </c>
-      <c r="C49" t="s">
-        <v>123</v>
-      </c>
-      <c r="D49" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="B51">
+        <v>100000000</v>
+      </c>
+      <c r="C51" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1080165573</v>
+      </c>
+      <c r="B52">
+        <v>100000000</v>
+      </c>
+      <c r="C52" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>10070018723</v>
+      </c>
+      <c r="B53">
+        <v>100000000</v>
+      </c>
+      <c r="C53" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>11350032974</v>
+      </c>
+      <c r="B54">
+        <v>100000000</v>
+      </c>
+      <c r="C54" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>3190196232</v>
+      </c>
+      <c r="B55">
+        <v>100000000</v>
+      </c>
+      <c r="C55" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>3440109728</v>
+      </c>
+      <c r="B56">
+        <v>100000000</v>
+      </c>
+      <c r="C56" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>14900019425</v>
+      </c>
+      <c r="B57">
+        <v>100000000</v>
+      </c>
+      <c r="C57" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>13440074198</v>
+      </c>
+      <c r="B58">
+        <v>100000000</v>
+      </c>
+      <c r="C58" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>10100099137</v>
+      </c>
+      <c r="B59">
+        <v>100000000</v>
+      </c>
+      <c r="C59" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>14340133361</v>
+      </c>
+      <c r="B60">
+        <v>100000000</v>
+      </c>
+      <c r="C60" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>10300240049</v>
+      </c>
+      <c r="B61">
+        <v>100000000</v>
+      </c>
+      <c r="C61" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>2740195622</v>
+      </c>
+      <c r="B62">
+        <v>100000000</v>
+      </c>
+      <c r="C62" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>13710091218</v>
+      </c>
+      <c r="B63">
+        <v>100000000</v>
+      </c>
+      <c r="C63" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>12910028712</v>
+      </c>
+      <c r="B64">
+        <v>100000000</v>
+      </c>
+      <c r="C64" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>11400165979</v>
+      </c>
+      <c r="B65">
+        <v>100000000</v>
+      </c>
+      <c r="C65" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>12720174614</v>
+      </c>
+      <c r="B66">
+        <v>100000000</v>
+      </c>
+      <c r="C66" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>13490011693</v>
+      </c>
+      <c r="B67">
+        <v>100000000</v>
+      </c>
+      <c r="C67" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>10540066810</v>
+      </c>
+      <c r="B68">
+        <v>100000000</v>
+      </c>
+      <c r="C68" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>13150013946</v>
+      </c>
+      <c r="B69">
+        <v>100000000</v>
+      </c>
+      <c r="C69" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>10250141650</v>
+      </c>
+      <c r="B70">
+        <v>100000000</v>
+      </c>
+      <c r="C70" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>2930059431</v>
+      </c>
+      <c r="B71">
+        <v>100000000</v>
+      </c>
+      <c r="C71" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>11320267205</v>
+      </c>
+      <c r="B72">
+        <v>100000000</v>
+      </c>
+      <c r="C72" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>12300036343</v>
+      </c>
+      <c r="B73">
+        <v>100000000</v>
+      </c>
+      <c r="C73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>11680248641</v>
+      </c>
+      <c r="B74">
+        <v>100000000</v>
+      </c>
+      <c r="C74" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>3750193466</v>
+      </c>
+      <c r="B75">
+        <v>100000000</v>
+      </c>
+      <c r="C75" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
         <v>12306204458</v>
       </c>
-      <c r="B50">
-        <v>4000000</v>
-      </c>
-      <c r="C50" t="s">
-        <v>123</v>
-      </c>
-      <c r="D50" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="B76">
+        <v>100000000</v>
+      </c>
+      <c r="C76" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
         <v>10380505120</v>
       </c>
-      <c r="B51">
-        <v>4000000</v>
-      </c>
-      <c r="C51" t="s">
-        <v>123</v>
-      </c>
-      <c r="D51" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="B77">
+        <v>100000000</v>
+      </c>
+      <c r="C77" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
         <v>1275372153</v>
       </c>
-      <c r="B52">
-        <v>4000000</v>
-      </c>
-      <c r="C52" t="s">
-        <v>123</v>
-      </c>
-      <c r="D52" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="B78">
+        <v>100000000</v>
+      </c>
+      <c r="C78" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
         <v>320076608</v>
       </c>
-      <c r="B53">
-        <v>4000000</v>
-      </c>
-      <c r="C53" t="s">
-        <v>123</v>
-      </c>
-      <c r="D53" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="B79">
+        <v>100000000</v>
+      </c>
+      <c r="C79" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
         <v>10490061802</v>
       </c>
-      <c r="B54">
-        <v>4000000</v>
-      </c>
-      <c r="C54" t="s">
-        <v>123</v>
-      </c>
-      <c r="D54" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="B80">
+        <v>100000000</v>
+      </c>
+      <c r="C80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
         <v>11050100658</v>
       </c>
-      <c r="B55">
-        <v>4000000</v>
-      </c>
-      <c r="C55" t="s">
-        <v>123</v>
-      </c>
-      <c r="D55" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="B81">
+        <v>100000000</v>
+      </c>
+      <c r="C81" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
         <v>10760058301</v>
       </c>
-      <c r="B56">
-        <v>4000000</v>
-      </c>
-      <c r="C56" t="s">
-        <v>123</v>
-      </c>
-      <c r="D56" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="B82">
+        <v>100000000</v>
+      </c>
+      <c r="C82" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83">
         <v>3500015064</v>
       </c>
-      <c r="B57">
-        <v>4000000</v>
-      </c>
-      <c r="C57" t="s">
-        <v>123</v>
-      </c>
-      <c r="D57" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="B83">
+        <v>100000000</v>
+      </c>
+      <c r="C83" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
         <v>3445103916</v>
       </c>
-      <c r="B58">
-        <v>4000000</v>
-      </c>
-      <c r="C58" t="s">
-        <v>123</v>
-      </c>
-      <c r="D58" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="B84">
+        <v>100000000</v>
+      </c>
+      <c r="C84" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
         <v>15853015</v>
       </c>
-      <c r="B59">
-        <v>4000000</v>
-      </c>
-      <c r="C59" t="s">
-        <v>123</v>
-      </c>
-      <c r="D59" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="B85">
+        <v>100000000</v>
+      </c>
+      <c r="C85" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
         <v>10910211970</v>
       </c>
-      <c r="B60">
-        <v>4000000</v>
-      </c>
-      <c r="C60" t="s">
-        <v>123</v>
-      </c>
-      <c r="D60" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61">
+      <c r="B86">
+        <v>100000000</v>
+      </c>
+      <c r="C86" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
         <v>13450026215</v>
       </c>
-      <c r="B61">
-        <v>4000000</v>
-      </c>
-      <c r="C61" t="s">
-        <v>123</v>
-      </c>
-      <c r="D61" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="B87">
+        <v>100000000</v>
+      </c>
+      <c r="C87" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
         <v>12300016631</v>
       </c>
-      <c r="B62">
-        <v>4000000</v>
-      </c>
-      <c r="C62" t="s">
-        <v>123</v>
-      </c>
-      <c r="D62" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63">
+      <c r="B88">
+        <v>100000000</v>
+      </c>
+      <c r="C88" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
         <v>10830113837</v>
       </c>
-      <c r="B63">
-        <v>4000000</v>
-      </c>
-      <c r="C63" t="s">
-        <v>123</v>
-      </c>
-      <c r="D63" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64">
+      <c r="B89">
+        <v>100000000</v>
+      </c>
+      <c r="C89" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90">
         <v>10326209059</v>
       </c>
-      <c r="B64">
-        <v>4000000</v>
-      </c>
-      <c r="C64" t="s">
-        <v>123</v>
-      </c>
-      <c r="D64" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65">
+      <c r="B90">
+        <v>100000000</v>
+      </c>
+      <c r="C90" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
         <v>12440133573</v>
       </c>
-      <c r="B65">
-        <v>4000000</v>
-      </c>
-      <c r="C65" t="s">
-        <v>123</v>
-      </c>
-      <c r="D65" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66">
+      <c r="B91">
+        <v>100000000</v>
+      </c>
+      <c r="C91" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
         <v>3160093053</v>
       </c>
-      <c r="B66">
-        <v>4000000</v>
-      </c>
-      <c r="C66" t="s">
-        <v>123</v>
-      </c>
-      <c r="D66" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67">
+      <c r="B92">
+        <v>100000000</v>
+      </c>
+      <c r="C92" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
         <v>13190176575</v>
       </c>
-      <c r="B67">
-        <v>4000000</v>
-      </c>
-      <c r="C67" t="s">
-        <v>123</v>
-      </c>
-      <c r="D67" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68">
+      <c r="B93">
+        <v>100000000</v>
+      </c>
+      <c r="C93" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94">
         <v>12190083139</v>
       </c>
-      <c r="B68">
-        <v>4000000</v>
-      </c>
-      <c r="C68" t="s">
-        <v>123</v>
-      </c>
-      <c r="D68" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69">
+      <c r="B94">
+        <v>100000000</v>
+      </c>
+      <c r="C94" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95">
         <v>12400203384</v>
       </c>
-      <c r="B69">
-        <v>4000000</v>
-      </c>
-      <c r="C69" t="s">
-        <v>123</v>
-      </c>
-      <c r="D69" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70">
+      <c r="B95">
+        <v>100000000</v>
+      </c>
+      <c r="C95" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96">
         <v>10950217871</v>
       </c>
-      <c r="B70">
-        <v>4000000</v>
-      </c>
-      <c r="C70" t="s">
-        <v>123</v>
-      </c>
-      <c r="D70" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71">
+      <c r="B96">
+        <v>100000000</v>
+      </c>
+      <c r="C96" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97">
         <v>795010086</v>
       </c>
-      <c r="B71">
-        <v>4000000</v>
-      </c>
-      <c r="C71" t="s">
-        <v>123</v>
-      </c>
-      <c r="D71" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72">
+      <c r="B97">
+        <v>100000000</v>
+      </c>
+      <c r="C97" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98">
         <v>10300022865</v>
       </c>
-      <c r="B72">
-        <v>4000000</v>
-      </c>
-      <c r="C72" t="s">
-        <v>123</v>
-      </c>
-      <c r="D72" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>10630402627</v>
-      </c>
-      <c r="B73">
-        <v>4000000</v>
-      </c>
-      <c r="C73" t="s">
-        <v>123</v>
-      </c>
-      <c r="D73" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74">
+      <c r="B98">
+        <v>100000000</v>
+      </c>
+      <c r="C98" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99">
         <v>13640115163</v>
       </c>
-      <c r="B74">
-        <v>4000000</v>
-      </c>
-      <c r="C74" t="s">
-        <v>123</v>
-      </c>
-      <c r="D74" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>11420138131</v>
-      </c>
-      <c r="B75">
-        <v>4000000</v>
-      </c>
-      <c r="C75" t="s">
-        <v>123</v>
-      </c>
-      <c r="D75" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>1080165573</v>
-      </c>
-      <c r="B76">
-        <v>4000000</v>
-      </c>
-      <c r="C76" t="s">
-        <v>123</v>
-      </c>
-      <c r="D76" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>10070018723</v>
-      </c>
-      <c r="B77">
-        <v>4000000</v>
-      </c>
-      <c r="C77" t="s">
-        <v>123</v>
-      </c>
-      <c r="D77" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>11350032974</v>
-      </c>
-      <c r="B78">
-        <v>4000000</v>
-      </c>
-      <c r="C78" t="s">
-        <v>123</v>
-      </c>
-      <c r="D78" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>3190196232</v>
-      </c>
-      <c r="B79">
-        <v>4000000</v>
-      </c>
-      <c r="C79" t="s">
-        <v>123</v>
-      </c>
-      <c r="D79" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>3440109728</v>
-      </c>
-      <c r="B80">
-        <v>4000000</v>
-      </c>
-      <c r="C80" t="s">
-        <v>123</v>
-      </c>
-      <c r="D80" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>14900019425</v>
-      </c>
-      <c r="B81">
-        <v>4000000</v>
-      </c>
-      <c r="C81" t="s">
-        <v>123</v>
-      </c>
-      <c r="D81" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>13440074198</v>
-      </c>
-      <c r="B82">
-        <v>4000000</v>
-      </c>
-      <c r="C82" t="s">
-        <v>123</v>
-      </c>
-      <c r="D82" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>10100099137</v>
-      </c>
-      <c r="B83">
-        <v>4000000</v>
-      </c>
-      <c r="C83" t="s">
-        <v>123</v>
-      </c>
-      <c r="D83" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>14340133361</v>
-      </c>
-      <c r="B84">
-        <v>4000000</v>
-      </c>
-      <c r="C84" t="s">
-        <v>123</v>
-      </c>
-      <c r="D84" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>10300240049</v>
-      </c>
-      <c r="B85">
-        <v>4000000</v>
-      </c>
-      <c r="C85" t="s">
-        <v>123</v>
-      </c>
-      <c r="D85" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>2740195622</v>
-      </c>
-      <c r="B86">
-        <v>4000000</v>
-      </c>
-      <c r="C86" t="s">
-        <v>123</v>
-      </c>
-      <c r="D86" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>13710091218</v>
-      </c>
-      <c r="B87">
-        <v>4000000</v>
-      </c>
-      <c r="C87" t="s">
-        <v>123</v>
-      </c>
-      <c r="D87" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>12910028712</v>
-      </c>
-      <c r="B88">
-        <v>4000000</v>
-      </c>
-      <c r="C88" t="s">
-        <v>123</v>
-      </c>
-      <c r="D88" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>11400165979</v>
-      </c>
-      <c r="B89">
-        <v>4000000</v>
-      </c>
-      <c r="C89" t="s">
-        <v>123</v>
-      </c>
-      <c r="D89" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>12720174614</v>
-      </c>
-      <c r="B90">
-        <v>4000000</v>
-      </c>
-      <c r="C90" t="s">
-        <v>123</v>
-      </c>
-      <c r="D90" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>13490011693</v>
-      </c>
-      <c r="B91">
-        <v>4000000</v>
-      </c>
-      <c r="C91" t="s">
-        <v>123</v>
-      </c>
-      <c r="D91" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>10540066810</v>
-      </c>
-      <c r="B92">
-        <v>4000000</v>
-      </c>
-      <c r="C92" t="s">
-        <v>123</v>
-      </c>
-      <c r="D92" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>13150013946</v>
-      </c>
-      <c r="B93">
-        <v>4000000</v>
-      </c>
-      <c r="C93" t="s">
-        <v>123</v>
-      </c>
-      <c r="D93" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>10250141650</v>
-      </c>
-      <c r="B94">
-        <v>4000000</v>
-      </c>
-      <c r="C94" t="s">
-        <v>123</v>
-      </c>
-      <c r="D94" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>2930059431</v>
-      </c>
-      <c r="B95">
-        <v>4000000</v>
-      </c>
-      <c r="C95" t="s">
-        <v>123</v>
-      </c>
-      <c r="D95" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>11320267205</v>
-      </c>
-      <c r="B96">
-        <v>4000000</v>
-      </c>
-      <c r="C96" t="s">
-        <v>123</v>
-      </c>
-      <c r="D96" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>12300036343</v>
-      </c>
-      <c r="B97">
-        <v>4000000</v>
-      </c>
-      <c r="C97" t="s">
-        <v>123</v>
-      </c>
-      <c r="D97" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>11680248641</v>
-      </c>
-      <c r="B98">
-        <v>4000000</v>
-      </c>
-      <c r="C98" t="s">
-        <v>123</v>
-      </c>
-      <c r="D98" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>3750193466</v>
-      </c>
       <c r="B99">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C99" t="s">
         <v>123</v>
       </c>
-      <c r="D99" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>960145065</v>
+        <v>10010330298</v>
       </c>
       <c r="B100">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C100" t="s">
         <v>123</v>
       </c>
-      <c r="D100" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>110107606</v>
+        <v>10156208053</v>
       </c>
       <c r="B101">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C101" t="s">
         <v>123</v>
       </c>
-      <c r="D101" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>13530015834</v>
+        <v>10190191410</v>
       </c>
       <c r="B102">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C102" t="s">
         <v>123</v>
       </c>
-      <c r="D102" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>2885010842</v>
+        <v>10250141636</v>
       </c>
       <c r="B103">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C103" t="s">
         <v>123</v>
       </c>
-      <c r="D103" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>13690202011</v>
+        <v>10276205518</v>
       </c>
       <c r="B104">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C104" t="s">
         <v>123</v>
       </c>
-      <c r="D104" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>15235581</v>
+        <v>10370241975</v>
       </c>
       <c r="B105">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C105" t="s">
         <v>123</v>
       </c>
-      <c r="D105" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>13220092806</v>
+        <v>10430208230</v>
       </c>
       <c r="B106">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C106" t="s">
         <v>123</v>
       </c>
-      <c r="D106" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>1730052707</v>
+        <v>10620117469</v>
       </c>
       <c r="B107">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C107" t="s">
         <v>123</v>
       </c>
-      <c r="D107" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>250282128</v>
+        <v>10730037635</v>
       </c>
       <c r="B108">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C108" t="s">
         <v>123</v>
       </c>
-      <c r="D108" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>1480029813</v>
+        <v>11000011032</v>
       </c>
       <c r="B109">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C109" t="s">
         <v>123</v>
       </c>
-      <c r="D109" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>13226207695</v>
+        <v>10820077392</v>
       </c>
       <c r="B110">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C110" t="s">
         <v>123</v>
       </c>
-      <c r="D110" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>15370186828</v>
+        <v>10850234873</v>
       </c>
       <c r="B111">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C111" t="s">
         <v>123</v>
       </c>
-      <c r="D111" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>475192293</v>
+        <v>10860133029</v>
       </c>
       <c r="B112">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C112" t="s">
         <v>123</v>
       </c>
-      <c r="D112" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>2740645899</v>
+        <v>10910192561</v>
       </c>
       <c r="B113">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C113" t="s">
         <v>123</v>
       </c>
-      <c r="D113" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>850090835</v>
+        <v>10930015684</v>
       </c>
       <c r="B114">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C114" t="s">
         <v>123</v>
       </c>
-      <c r="D114" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>470114159</v>
+        <v>10850262566</v>
       </c>
       <c r="B115">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C115" t="s">
         <v>123</v>
       </c>
-      <c r="D115" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>2920054945</v>
+        <v>10930481083</v>
       </c>
       <c r="B116">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C116" t="s">
         <v>123</v>
       </c>
-      <c r="D116" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>210034499</v>
+        <v>10960083127</v>
       </c>
       <c r="B117">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C117" t="s">
         <v>123</v>
       </c>
-      <c r="D117" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>80086000</v>
+        <v>11000050545</v>
       </c>
       <c r="B118">
-        <v>4000000</v>
+        <v>100000000</v>
       </c>
       <c r="C118" t="s">
         <v>123</v>
       </c>
-      <c r="D118" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119">
-        <v>1365003118</v>
-      </c>
-      <c r="B119">
-        <v>4000000</v>
-      </c>
-      <c r="C119" t="s">
-        <v>123</v>
-      </c>
-      <c r="D119" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120">
-        <v>3595000336</v>
-      </c>
-      <c r="B120">
-        <v>4000000</v>
-      </c>
-      <c r="C120" t="s">
-        <v>123</v>
-      </c>
-      <c r="D120" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121">
-        <v>2850008834</v>
-      </c>
-      <c r="B121">
-        <v>4000000</v>
-      </c>
-      <c r="C121" t="s">
-        <v>123</v>
-      </c>
-      <c r="D121" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122">
-        <v>13240166174</v>
-      </c>
-      <c r="B122">
-        <v>4000000</v>
-      </c>
-      <c r="C122" t="s">
-        <v>123</v>
-      </c>
-      <c r="D122" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123">
-        <v>12920094505</v>
-      </c>
-      <c r="B123">
-        <v>4000000</v>
-      </c>
-      <c r="C123" t="s">
-        <v>123</v>
-      </c>
-      <c r="D123" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124">
-        <v>3505023644</v>
-      </c>
-      <c r="B124">
-        <v>4000000</v>
-      </c>
-      <c r="C124" t="s">
-        <v>123</v>
-      </c>
-      <c r="D124" t="s">
-        <v>171</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D118" xr:uid="{3D988AC9-16EF-45E7-9C58-87D45D3FEEC3}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3545,7 +3111,7 @@
         <v>402</v>
       </c>
       <c r="E2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3562,7 +3128,7 @@
         <v>402</v>
       </c>
       <c r="E3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3579,7 +3145,7 @@
         <v>402</v>
       </c>
       <c r="E4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3596,7 +3162,7 @@
         <v>402</v>
       </c>
       <c r="E5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3613,7 +3179,7 @@
         <v>402</v>
       </c>
       <c r="E6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3630,7 +3196,7 @@
         <v>402</v>
       </c>
       <c r="E7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3647,7 +3213,7 @@
         <v>402</v>
       </c>
       <c r="E8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3664,7 +3230,7 @@
         <v>402</v>
       </c>
       <c r="E9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3681,7 +3247,7 @@
         <v>402</v>
       </c>
       <c r="E10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3698,7 +3264,7 @@
         <v>402</v>
       </c>
       <c r="E11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3715,7 +3281,7 @@
         <v>402</v>
       </c>
       <c r="E12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3732,7 +3298,7 @@
         <v>402</v>
       </c>
       <c r="E13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3749,7 +3315,7 @@
         <v>402</v>
       </c>
       <c r="E14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3766,7 +3332,7 @@
         <v>402</v>
       </c>
       <c r="E15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3783,7 +3349,7 @@
         <v>402</v>
       </c>
       <c r="E16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F16"/>
     </row>
@@ -3801,7 +3367,7 @@
         <v>402</v>
       </c>
       <c r="E17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3818,7 +3384,7 @@
         <v>402</v>
       </c>
       <c r="E18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3835,7 +3401,7 @@
         <v>402</v>
       </c>
       <c r="E19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3852,7 +3418,7 @@
         <v>402</v>
       </c>
       <c r="E20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3869,7 +3435,7 @@
         <v>402</v>
       </c>
       <c r="E21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3886,7 +3452,7 @@
         <v>402</v>
       </c>
       <c r="E22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3903,7 +3469,7 @@
         <v>402</v>
       </c>
       <c r="E23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3920,7 +3486,7 @@
         <v>402</v>
       </c>
       <c r="E24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3937,7 +3503,7 @@
         <v>402</v>
       </c>
       <c r="E25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3954,7 +3520,7 @@
         <v>402</v>
       </c>
       <c r="E26" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3971,7 +3537,7 @@
         <v>402</v>
       </c>
       <c r="E27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3988,7 +3554,7 @@
         <v>402</v>
       </c>
       <c r="E28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -4005,7 +3571,7 @@
         <v>402</v>
       </c>
       <c r="E29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -4022,7 +3588,7 @@
         <v>402</v>
       </c>
       <c r="E30" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -4039,7 +3605,7 @@
         <v>402</v>
       </c>
       <c r="E31" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -4056,7 +3622,7 @@
         <v>402</v>
       </c>
       <c r="E32" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -4073,7 +3639,7 @@
         <v>402</v>
       </c>
       <c r="E33" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -4090,7 +3656,7 @@
         <v>402</v>
       </c>
       <c r="E34" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -4107,7 +3673,7 @@
         <v>402</v>
       </c>
       <c r="E35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -4124,7 +3690,7 @@
         <v>402</v>
       </c>
       <c r="E36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -4141,7 +3707,7 @@
         <v>402</v>
       </c>
       <c r="E37" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -4158,7 +3724,7 @@
         <v>402</v>
       </c>
       <c r="E38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -4175,7 +3741,7 @@
         <v>402</v>
       </c>
       <c r="E39" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -4420,7 +3986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6F6505-72C5-407A-9E87-8F1DBAE9B164}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -4460,7 +4026,7 @@
         <v>163</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4480,7 +4046,7 @@
         <v>163</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4500,7 +4066,7 @@
         <v>163</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] Pases y Transferencias Entre Socios
Optimización modulo completo Pases y Transferencias Entre Socios
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20413"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728550AE-674F-486F-9437-0B2335CB6657}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B22F5D-AE5E-4D7C-8CD0-34F2D7D426BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="219">
   <si>
     <t>Nombre</t>
   </si>
@@ -670,6 +670,24 @@
   </si>
   <si>
     <t>20230830</t>
+  </si>
+  <si>
+    <t>F00031</t>
+  </si>
+  <si>
+    <t>031</t>
+  </si>
+  <si>
+    <t>F04815</t>
+  </si>
+  <si>
+    <t>340</t>
+  </si>
+  <si>
+    <t>NEFURNO</t>
+  </si>
+  <si>
+    <t>OM</t>
   </si>
 </sst>
 </file>
@@ -1134,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1699,7 +1717,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>150</v>
       </c>
@@ -1707,7 +1725,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>152</v>
       </c>
@@ -1715,7 +1733,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>164</v>
       </c>
@@ -1723,7 +1741,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>166</v>
       </c>
@@ -1731,12 +1749,36 @@
         <v>165</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>167</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>213</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>215</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>217</v>
+      </c>
+      <c r="D72" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -1749,7 +1791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F86E7B-4061-45F1-9FC5-D02253AB0909}">
   <dimension ref="A1:D118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
[FIX] Automatizacion de Sucursales
Se modificaron los casos de ASUC hasta el num 15
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20413"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728550AE-674F-486F-9437-0B2335CB6657}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F2D707-5475-4F15-BEF2-E771D9C19932}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="214">
   <si>
     <t>Nombre</t>
   </si>
@@ -516,15 +516,6 @@
     <t>TES12</t>
   </si>
   <si>
-    <t>20230612</t>
-  </si>
-  <si>
-    <t>20230901</t>
-  </si>
-  <si>
-    <t>20230829</t>
-  </si>
-  <si>
     <t>F00282</t>
   </si>
   <si>
@@ -669,7 +660,19 @@
     <t>10010661387</t>
   </si>
   <si>
-    <t>20230830</t>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>20240226</t>
+  </si>
+  <si>
+    <t>20230828</t>
+  </si>
+  <si>
+    <t>20230904</t>
+  </si>
+  <si>
+    <t>20240826</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1064,7 @@
         <v>153</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1136,7 +1139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1156,7 +1159,7 @@
         <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1167,7 +1170,7 @@
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1178,7 +1181,7 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1189,7 +1192,7 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1200,7 +1203,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1211,7 +1214,7 @@
         <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1222,7 +1225,7 @@
         <v>67</v>
       </c>
       <c r="D7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1233,7 +1236,7 @@
         <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1252,7 +1255,7 @@
         <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1295,7 +1298,7 @@
         <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1434,7 +1437,7 @@
         <v>22</v>
       </c>
       <c r="D32" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1477,7 +1480,7 @@
         <v>79</v>
       </c>
       <c r="D37" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1504,7 +1507,7 @@
         <v>23</v>
       </c>
       <c r="D40" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1717,26 +1720,26 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1749,7 +1752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F86E7B-4061-45F1-9FC5-D02253AB0909}">
   <dimension ref="A1:D118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1757,7 +1760,7 @@
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -1768,7 +1771,7 @@
         <v>122</v>
       </c>
       <c r="D1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1781,6 +1784,9 @@
       <c r="C2" t="s">
         <v>123</v>
       </c>
+      <c r="D2" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1792,6 +1798,9 @@
       <c r="C3" t="s">
         <v>123</v>
       </c>
+      <c r="D3" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1803,6 +1812,9 @@
       <c r="C4" t="s">
         <v>123</v>
       </c>
+      <c r="D4" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1814,6 +1826,9 @@
       <c r="C5" t="s">
         <v>123</v>
       </c>
+      <c r="D5" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1825,6 +1840,9 @@
       <c r="C6" t="s">
         <v>123</v>
       </c>
+      <c r="D6" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1836,6 +1854,9 @@
       <c r="C7" t="s">
         <v>123</v>
       </c>
+      <c r="D7" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1847,6 +1868,9 @@
       <c r="C8" t="s">
         <v>123</v>
       </c>
+      <c r="D8" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1858,6 +1882,9 @@
       <c r="C9" t="s">
         <v>123</v>
       </c>
+      <c r="D9" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1869,6 +1896,9 @@
       <c r="C10" t="s">
         <v>123</v>
       </c>
+      <c r="D10" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1880,6 +1910,9 @@
       <c r="C11" t="s">
         <v>123</v>
       </c>
+      <c r="D11" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1891,6 +1924,9 @@
       <c r="C12" t="s">
         <v>123</v>
       </c>
+      <c r="D12" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1902,6 +1938,9 @@
       <c r="C13" t="s">
         <v>123</v>
       </c>
+      <c r="D13" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1913,6 +1952,9 @@
       <c r="C14" t="s">
         <v>123</v>
       </c>
+      <c r="D14" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1924,6 +1966,9 @@
       <c r="C15" t="s">
         <v>123</v>
       </c>
+      <c r="D15" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1935,8 +1980,11 @@
       <c r="C16" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11190096323</v>
       </c>
@@ -1946,8 +1994,11 @@
       <c r="C17" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12520034239</v>
       </c>
@@ -1957,8 +2008,11 @@
       <c r="C18" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>12260119610</v>
       </c>
@@ -1968,8 +2022,11 @@
       <c r="C19" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4970101565</v>
       </c>
@@ -1979,8 +2036,11 @@
       <c r="C20" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10320039887</v>
       </c>
@@ -1990,8 +2050,11 @@
       <c r="C21" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>11000112759</v>
       </c>
@@ -2001,8 +2064,11 @@
       <c r="C22" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>11370060915</v>
       </c>
@@ -2012,8 +2078,11 @@
       <c r="C23" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2600003665</v>
       </c>
@@ -2023,8 +2092,11 @@
       <c r="C24" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1480029806</v>
       </c>
@@ -2034,8 +2106,11 @@
       <c r="C25" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>11450064639</v>
       </c>
@@ -2045,8 +2120,11 @@
       <c r="C26" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>10720198294</v>
       </c>
@@ -2056,8 +2134,11 @@
       <c r="C27" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3880065530</v>
       </c>
@@ -2067,8 +2148,11 @@
       <c r="C28" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>80031833</v>
       </c>
@@ -2078,8 +2162,11 @@
       <c r="C29" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>10590131319</v>
       </c>
@@ -2089,8 +2176,11 @@
       <c r="C30" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>240127202</v>
       </c>
@@ -2100,8 +2190,11 @@
       <c r="C31" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>10930393717</v>
       </c>
@@ -2111,8 +2204,11 @@
       <c r="C32" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>10630179471</v>
       </c>
@@ -2122,8 +2218,11 @@
       <c r="C33" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>11480029721</v>
       </c>
@@ -2133,8 +2232,11 @@
       <c r="C34" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>830413494</v>
       </c>
@@ -2144,8 +2246,11 @@
       <c r="C35" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2190146193</v>
       </c>
@@ -2155,8 +2260,11 @@
       <c r="C36" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>10180130203</v>
       </c>
@@ -2166,8 +2274,11 @@
       <c r="C37" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>690059296</v>
       </c>
@@ -2177,8 +2288,11 @@
       <c r="C38" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1560012823</v>
       </c>
@@ -2188,8 +2302,11 @@
       <c r="C39" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2650033717</v>
       </c>
@@ -2199,8 +2316,11 @@
       <c r="C40" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>10010552085</v>
       </c>
@@ -2210,8 +2330,11 @@
       <c r="C41" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>11680050224</v>
       </c>
@@ -2221,8 +2344,11 @@
       <c r="C42" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>13180116187</v>
       </c>
@@ -2232,8 +2358,11 @@
       <c r="C43" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>12880617116</v>
       </c>
@@ -2243,8 +2372,11 @@
       <c r="C44" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>385454397</v>
       </c>
@@ -2254,8 +2386,11 @@
       <c r="C45" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1170103159</v>
       </c>
@@ -2265,8 +2400,11 @@
       <c r="C46" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>11240036538</v>
       </c>
@@ -2276,8 +2414,11 @@
       <c r="C47" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>11576205327</v>
       </c>
@@ -2287,8 +2428,11 @@
       <c r="C48" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>10260159191</v>
       </c>
@@ -2298,8 +2442,11 @@
       <c r="C49" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3740026512</v>
       </c>
@@ -2309,8 +2456,11 @@
       <c r="C50" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>3570015560</v>
       </c>
@@ -2320,8 +2470,11 @@
       <c r="C51" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1080165573</v>
       </c>
@@ -2331,8 +2484,11 @@
       <c r="C52" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>10070018723</v>
       </c>
@@ -2342,8 +2498,11 @@
       <c r="C53" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>11350032974</v>
       </c>
@@ -2353,8 +2512,11 @@
       <c r="C54" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>3190196232</v>
       </c>
@@ -2364,8 +2526,11 @@
       <c r="C55" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>3440109728</v>
       </c>
@@ -2375,8 +2540,11 @@
       <c r="C56" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>14900019425</v>
       </c>
@@ -2386,8 +2554,11 @@
       <c r="C57" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>13440074198</v>
       </c>
@@ -2397,8 +2568,11 @@
       <c r="C58" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>10100099137</v>
       </c>
@@ -2408,8 +2582,11 @@
       <c r="C59" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>14340133361</v>
       </c>
@@ -2419,8 +2596,11 @@
       <c r="C60" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>10300240049</v>
       </c>
@@ -2430,8 +2610,11 @@
       <c r="C61" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2740195622</v>
       </c>
@@ -2441,8 +2624,11 @@
       <c r="C62" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>13710091218</v>
       </c>
@@ -2452,8 +2638,11 @@
       <c r="C63" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>12910028712</v>
       </c>
@@ -2463,8 +2652,11 @@
       <c r="C64" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>11400165979</v>
       </c>
@@ -2474,8 +2666,11 @@
       <c r="C65" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>12720174614</v>
       </c>
@@ -2485,8 +2680,11 @@
       <c r="C66" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>13490011693</v>
       </c>
@@ -2496,8 +2694,11 @@
       <c r="C67" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>10540066810</v>
       </c>
@@ -2507,8 +2708,11 @@
       <c r="C68" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>13150013946</v>
       </c>
@@ -2518,8 +2722,11 @@
       <c r="C69" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>10250141650</v>
       </c>
@@ -2529,8 +2736,11 @@
       <c r="C70" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2930059431</v>
       </c>
@@ -2540,8 +2750,11 @@
       <c r="C71" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>11320267205</v>
       </c>
@@ -2551,8 +2764,11 @@
       <c r="C72" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>12300036343</v>
       </c>
@@ -2562,8 +2778,11 @@
       <c r="C73" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>11680248641</v>
       </c>
@@ -2573,8 +2792,11 @@
       <c r="C74" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>3750193466</v>
       </c>
@@ -2584,8 +2806,11 @@
       <c r="C75" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>12306204458</v>
       </c>
@@ -2595,8 +2820,11 @@
       <c r="C76" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>10380505120</v>
       </c>
@@ -2606,8 +2834,11 @@
       <c r="C77" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1275372153</v>
       </c>
@@ -2617,8 +2848,11 @@
       <c r="C78" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>320076608</v>
       </c>
@@ -2628,8 +2862,11 @@
       <c r="C79" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>10490061802</v>
       </c>
@@ -2639,8 +2876,11 @@
       <c r="C80" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>11050100658</v>
       </c>
@@ -2650,8 +2890,11 @@
       <c r="C81" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>10760058301</v>
       </c>
@@ -2661,8 +2904,11 @@
       <c r="C82" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>3500015064</v>
       </c>
@@ -2672,8 +2918,11 @@
       <c r="C83" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>3445103916</v>
       </c>
@@ -2683,8 +2932,11 @@
       <c r="C84" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>15853015</v>
       </c>
@@ -2694,8 +2946,11 @@
       <c r="C85" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>10910211970</v>
       </c>
@@ -2705,8 +2960,11 @@
       <c r="C86" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>13450026215</v>
       </c>
@@ -2716,8 +2974,11 @@
       <c r="C87" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>12300016631</v>
       </c>
@@ -2727,8 +2988,11 @@
       <c r="C88" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>10830113837</v>
       </c>
@@ -2738,8 +3002,11 @@
       <c r="C89" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>10326209059</v>
       </c>
@@ -2749,8 +3016,11 @@
       <c r="C90" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>12440133573</v>
       </c>
@@ -2760,8 +3030,11 @@
       <c r="C91" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>3160093053</v>
       </c>
@@ -2771,8 +3044,11 @@
       <c r="C92" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>13190176575</v>
       </c>
@@ -2782,8 +3058,11 @@
       <c r="C93" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>12190083139</v>
       </c>
@@ -2793,8 +3072,11 @@
       <c r="C94" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>12400203384</v>
       </c>
@@ -2804,8 +3086,11 @@
       <c r="C95" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>10950217871</v>
       </c>
@@ -2815,8 +3100,11 @@
       <c r="C96" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>795010086</v>
       </c>
@@ -2826,8 +3114,11 @@
       <c r="C97" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>10300022865</v>
       </c>
@@ -2837,8 +3128,11 @@
       <c r="C98" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>13640115163</v>
       </c>
@@ -2848,8 +3142,11 @@
       <c r="C99" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>10010330298</v>
       </c>
@@ -2859,8 +3156,11 @@
       <c r="C100" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>10156208053</v>
       </c>
@@ -2870,8 +3170,11 @@
       <c r="C101" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>10190191410</v>
       </c>
@@ -2881,8 +3184,11 @@
       <c r="C102" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>10250141636</v>
       </c>
@@ -2892,8 +3198,11 @@
       <c r="C103" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>10276205518</v>
       </c>
@@ -2903,8 +3212,11 @@
       <c r="C104" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>10370241975</v>
       </c>
@@ -2914,8 +3226,11 @@
       <c r="C105" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>10430208230</v>
       </c>
@@ -2925,8 +3240,11 @@
       <c r="C106" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>10620117469</v>
       </c>
@@ -2936,8 +3254,11 @@
       <c r="C107" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>10730037635</v>
       </c>
@@ -2947,8 +3268,11 @@
       <c r="C108" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>11000011032</v>
       </c>
@@ -2958,8 +3282,11 @@
       <c r="C109" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>10820077392</v>
       </c>
@@ -2969,8 +3296,11 @@
       <c r="C110" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>10850234873</v>
       </c>
@@ -2980,8 +3310,11 @@
       <c r="C111" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>10860133029</v>
       </c>
@@ -2991,8 +3324,11 @@
       <c r="C112" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>10910192561</v>
       </c>
@@ -3002,8 +3338,11 @@
       <c r="C113" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>10930015684</v>
       </c>
@@ -3013,8 +3352,11 @@
       <c r="C114" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>10850262566</v>
       </c>
@@ -3024,8 +3366,11 @@
       <c r="C115" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>10930481083</v>
       </c>
@@ -3035,8 +3380,11 @@
       <c r="C116" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>10960083127</v>
       </c>
@@ -3046,8 +3394,11 @@
       <c r="C117" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>11000050545</v>
       </c>
@@ -3056,6 +3407,9 @@
       </c>
       <c r="C118" t="s">
         <v>123</v>
+      </c>
+      <c r="D118" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -3069,7 +3423,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:E15"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3111,7 +3465,7 @@
         <v>402</v>
       </c>
       <c r="E2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3128,7 +3482,7 @@
         <v>402</v>
       </c>
       <c r="E3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3145,7 +3499,7 @@
         <v>402</v>
       </c>
       <c r="E4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3162,7 +3516,7 @@
         <v>402</v>
       </c>
       <c r="E5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3179,7 +3533,7 @@
         <v>402</v>
       </c>
       <c r="E6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3196,7 +3550,7 @@
         <v>402</v>
       </c>
       <c r="E7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3213,7 +3567,7 @@
         <v>402</v>
       </c>
       <c r="E8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3230,7 +3584,7 @@
         <v>402</v>
       </c>
       <c r="E9" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3247,7 +3601,7 @@
         <v>402</v>
       </c>
       <c r="E10" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3264,7 +3618,7 @@
         <v>402</v>
       </c>
       <c r="E11" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3281,7 +3635,7 @@
         <v>402</v>
       </c>
       <c r="E12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3298,7 +3652,7 @@
         <v>402</v>
       </c>
       <c r="E13" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3315,7 +3669,7 @@
         <v>402</v>
       </c>
       <c r="E14" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3332,7 +3686,7 @@
         <v>402</v>
       </c>
       <c r="E15" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3349,7 +3703,7 @@
         <v>402</v>
       </c>
       <c r="E16" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F16"/>
     </row>
@@ -3367,7 +3721,7 @@
         <v>402</v>
       </c>
       <c r="E17" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3384,7 +3738,7 @@
         <v>402</v>
       </c>
       <c r="E18" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3401,7 +3755,7 @@
         <v>402</v>
       </c>
       <c r="E19" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3418,7 +3772,7 @@
         <v>402</v>
       </c>
       <c r="E20" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3435,7 +3789,7 @@
         <v>402</v>
       </c>
       <c r="E21" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3452,7 +3806,7 @@
         <v>402</v>
       </c>
       <c r="E22" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3469,7 +3823,7 @@
         <v>402</v>
       </c>
       <c r="E23" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3486,7 +3840,7 @@
         <v>402</v>
       </c>
       <c r="E24" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3503,7 +3857,7 @@
         <v>402</v>
       </c>
       <c r="E25" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3520,7 +3874,7 @@
         <v>402</v>
       </c>
       <c r="E26" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3537,7 +3891,7 @@
         <v>402</v>
       </c>
       <c r="E27" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3554,7 +3908,7 @@
         <v>402</v>
       </c>
       <c r="E28" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3571,7 +3925,7 @@
         <v>402</v>
       </c>
       <c r="E29" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3588,7 +3942,7 @@
         <v>402</v>
       </c>
       <c r="E30" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3605,7 +3959,7 @@
         <v>402</v>
       </c>
       <c r="E31" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -3622,7 +3976,7 @@
         <v>402</v>
       </c>
       <c r="E32" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3639,7 +3993,7 @@
         <v>402</v>
       </c>
       <c r="E33" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3656,7 +4010,7 @@
         <v>402</v>
       </c>
       <c r="E34" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3673,7 +4027,7 @@
         <v>402</v>
       </c>
       <c r="E35" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3690,7 +4044,7 @@
         <v>402</v>
       </c>
       <c r="E36" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3707,7 +4061,7 @@
         <v>402</v>
       </c>
       <c r="E37" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3724,7 +4078,7 @@
         <v>402</v>
       </c>
       <c r="E38" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3741,7 +4095,7 @@
         <v>402</v>
       </c>
       <c r="E39" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -3916,7 +4270,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A125"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3986,9 +4340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6F6505-72C5-407A-9E87-8F1DBAE9B164}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4014,19 +4366,19 @@
         <v>155</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>161</v>
+        <v>213</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>162</v>
+        <v>210</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>162</v>
+        <v>210</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>163</v>
+        <v>212</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4034,19 +4386,19 @@
         <v>156</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>161</v>
+        <v>213</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>162</v>
+        <v>210</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>162</v>
+        <v>210</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>163</v>
+        <v>212</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4054,19 +4406,19 @@
         <v>157</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>161</v>
+        <v>213</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>162</v>
+        <v>210</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>162</v>
+        <v>210</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>163</v>
+        <v>212</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] Sobregiros, LYA, Posteo
Se modifico la fecha en LYA02, SG05, PST01
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20413"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F2D707-5475-4F15-BEF2-E771D9C19932}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C5207A-CA6B-41D0-A4F4-B364BDB2432A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="220">
   <si>
     <t>Nombre</t>
   </si>
@@ -673,6 +673,24 @@
   </si>
   <si>
     <t>20240826</t>
+  </si>
+  <si>
+    <t>F00031</t>
+  </si>
+  <si>
+    <t>F04815</t>
+  </si>
+  <si>
+    <t>NEFURNO</t>
+  </si>
+  <si>
+    <t>F02059</t>
+  </si>
+  <si>
+    <t>OM</t>
+  </si>
+  <si>
+    <t>031</t>
   </si>
 </sst>
 </file>
@@ -1137,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1702,7 +1720,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>150</v>
       </c>
@@ -1710,7 +1728,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>152</v>
       </c>
@@ -1718,7 +1736,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>161</v>
       </c>
@@ -1726,7 +1744,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>163</v>
       </c>
@@ -1734,12 +1752,45 @@
         <v>162</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>164</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>214</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>215</v>
+      </c>
+      <c r="C71">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>216</v>
+      </c>
+      <c r="C72" s="4"/>
+      <c r="D72" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>217</v>
+      </c>
+      <c r="C73">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -4340,7 +4391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6F6505-72C5-407A-9E87-8F1DBAE9B164}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
[FEATURE][FIX] CHR, MON, PF, DE , ASUC, PAS, PN, CMA, REM , GEF , DIS
Se agregaron casos para revisar de Plazo Fijo
Se fixearon 11 modulos de la regresion parte 3 y 7
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20413"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F2D707-5475-4F15-BEF2-E771D9C19932}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B23984-9991-4113-BF5C-701A18B0911B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Carga Saldos'!$A$1:$D$118</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="221">
   <si>
     <t>Nombre</t>
   </si>
@@ -673,6 +673,27 @@
   </si>
   <si>
     <t>20240826</t>
+  </si>
+  <si>
+    <t>F00031</t>
+  </si>
+  <si>
+    <t>031</t>
+  </si>
+  <si>
+    <t>F04815</t>
+  </si>
+  <si>
+    <t>340</t>
+  </si>
+  <si>
+    <t>NEFURNO</t>
+  </si>
+  <si>
+    <t>OM</t>
+  </si>
+  <si>
+    <t>F02059</t>
   </si>
 </sst>
 </file>
@@ -1137,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1702,7 +1723,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>150</v>
       </c>
@@ -1710,7 +1731,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>152</v>
       </c>
@@ -1718,7 +1739,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>161</v>
       </c>
@@ -1726,7 +1747,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>163</v>
       </c>
@@ -1734,12 +1755,44 @@
         <v>162</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>164</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>214</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>216</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>218</v>
+      </c>
+      <c r="D72" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>220</v>
+      </c>
+      <c r="C73">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -4340,7 +4393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6F6505-72C5-407A-9E87-8F1DBAE9B164}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
[FIX] REGRESION PARTE 4 Y 5
se arreglaron los casos de los siguientes modulos:
Admin de Piezas
Cuentas
Deposito en Efect por caja
Emision chequera
Ingresos Egresos Varios
Mov Automaticos
Mov Pendientes Cancelados
Mov Rechazados
Pago de intereses
Posteo

se modifico funcion de verificacion de datos tabla
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20413"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C5207A-CA6B-41D0-A4F4-B364BDB2432A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8C90A5-3736-4661-9AD4-7EB6E190C6FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Carga Saldos'!$A$1:$D$118</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="221">
   <si>
     <t>Nombre</t>
   </si>
@@ -666,9 +666,6 @@
     <t>20240226</t>
   </si>
   <si>
-    <t>20230828</t>
-  </si>
-  <si>
     <t>20230904</t>
   </si>
   <si>
@@ -691,6 +688,12 @@
   </si>
   <si>
     <t>031</t>
+  </si>
+  <si>
+    <t>022</t>
+  </si>
+  <si>
+    <t>F01774</t>
   </si>
 </sst>
 </file>
@@ -1155,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,15 +1765,15 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C71">
         <v>340</v>
@@ -1778,19 +1781,27 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C73">
         <v>138</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>220</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -4391,7 +4402,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6F6505-72C5-407A-9E87-8F1DBAE9B164}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4417,7 +4430,7 @@
         <v>155</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>210</v>
@@ -4426,10 +4439,10 @@
         <v>210</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4437,7 +4450,7 @@
         <v>156</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>210</v>
@@ -4446,10 +4459,10 @@
         <v>210</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4457,7 +4470,7 @@
         <v>157</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>210</v>
@@ -4466,10 +4479,10 @@
         <v>210</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] Regresion parte 6 y 7 TES12
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20413"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C5207A-CA6B-41D0-A4F4-B364BDB2432A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9A2474-16DB-4A2A-92B4-86CF20566E7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="219">
   <si>
     <t>Nombre</t>
   </si>
@@ -664,9 +664,6 @@
   </si>
   <si>
     <t>20240226</t>
-  </si>
-  <si>
-    <t>20230828</t>
   </si>
   <si>
     <t>20230904</t>
@@ -1157,7 +1154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
@@ -1762,15 +1759,15 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C71">
         <v>340</v>
@@ -1778,16 +1775,16 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C73">
         <v>138</v>
@@ -4391,7 +4388,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6F6505-72C5-407A-9E87-8F1DBAE9B164}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4417,7 +4416,7 @@
         <v>155</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>210</v>
@@ -4426,10 +4425,10 @@
         <v>210</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4437,7 +4436,7 @@
         <v>156</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>210</v>
@@ -4446,10 +4445,10 @@
         <v>210</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4457,7 +4456,7 @@
         <v>157</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>210</v>
@@ -4466,10 +4465,10 @@
         <v>210</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] Optimizacion OR - ASUC
Se optimizaron casos de ASUC del 02 al 40
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20414"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C5207A-CA6B-41D0-A4F4-B364BDB2432A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477380C5-DB39-4CDA-9D38-2809163F4871}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="222">
   <si>
     <t>Nombre</t>
   </si>
@@ -660,15 +660,9 @@
     <t>10010661387</t>
   </si>
   <si>
-    <t>SI</t>
-  </si>
-  <si>
     <t>20240226</t>
   </si>
   <si>
-    <t>20230828</t>
-  </si>
-  <si>
     <t>20230904</t>
   </si>
   <si>
@@ -691,6 +685,18 @@
   </si>
   <si>
     <t>031</t>
+  </si>
+  <si>
+    <t>F01774</t>
+  </si>
+  <si>
+    <t>022</t>
+  </si>
+  <si>
+    <t>F00065</t>
+  </si>
+  <si>
+    <t>065</t>
   </si>
 </sst>
 </file>
@@ -1155,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,35 +1768,51 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>215</v>
-      </c>
-      <c r="C71">
+        <v>213</v>
+      </c>
+      <c r="C71" s="4">
         <v>340</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>217</v>
-      </c>
-      <c r="C73">
+        <v>215</v>
+      </c>
+      <c r="C73" s="4">
         <v>138</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>218</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>220</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -1801,7 +1823,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F86E7B-4061-45F1-9FC5-D02253AB0909}">
-  <dimension ref="A1:D118"/>
+  <dimension ref="A1:AC116"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1809,9 +1831,10 @@
   <cols>
     <col min="1" max="1" width="14" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -1824,8 +1847,17 @@
       <c r="D1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11450157481</v>
       </c>
@@ -1835,11 +1867,17 @@
       <c r="C2" t="s">
         <v>123</v>
       </c>
-      <c r="D2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA2">
+        <v>11450157481</v>
+      </c>
+      <c r="AB2">
+        <v>100000000</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3230059240</v>
       </c>
@@ -1849,11 +1887,17 @@
       <c r="C3" t="s">
         <v>123</v>
       </c>
-      <c r="D3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA3">
+        <v>3230059240</v>
+      </c>
+      <c r="AB3">
+        <v>100000000</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10060347141</v>
       </c>
@@ -1863,11 +1907,17 @@
       <c r="C4" t="s">
         <v>123</v>
       </c>
-      <c r="D4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA4">
+        <v>10060347141</v>
+      </c>
+      <c r="AB4">
+        <v>100000000</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11080064566</v>
       </c>
@@ -1877,11 +1927,17 @@
       <c r="C5" t="s">
         <v>123</v>
       </c>
-      <c r="D5" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA5">
+        <v>11080064566</v>
+      </c>
+      <c r="AB5">
+        <v>100000000</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>12580016873</v>
       </c>
@@ -1891,11 +1947,17 @@
       <c r="C6" t="s">
         <v>123</v>
       </c>
-      <c r="D6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA6">
+        <v>12580016873</v>
+      </c>
+      <c r="AB6">
+        <v>100000000</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>11396201787</v>
       </c>
@@ -1905,11 +1967,17 @@
       <c r="C7" t="s">
         <v>123</v>
       </c>
-      <c r="D7" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA7">
+        <v>11396201787</v>
+      </c>
+      <c r="AB7">
+        <v>100000000</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10150076223</v>
       </c>
@@ -1919,11 +1987,17 @@
       <c r="C8" t="s">
         <v>123</v>
       </c>
-      <c r="D8" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA8">
+        <v>10150076223</v>
+      </c>
+      <c r="AB8">
+        <v>100000000</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3405529110</v>
       </c>
@@ -1933,11 +2007,17 @@
       <c r="C9" t="s">
         <v>123</v>
       </c>
-      <c r="D9" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA9">
+        <v>3405529110</v>
+      </c>
+      <c r="AB9">
+        <v>100000000</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>13240145445</v>
       </c>
@@ -1947,11 +2027,17 @@
       <c r="C10" t="s">
         <v>123</v>
       </c>
-      <c r="D10" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA10">
+        <v>13240145445</v>
+      </c>
+      <c r="AB10">
+        <v>100000000</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11370044717</v>
       </c>
@@ -1961,11 +2047,17 @@
       <c r="C11" t="s">
         <v>123</v>
       </c>
-      <c r="D11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA11">
+        <v>11370044717</v>
+      </c>
+      <c r="AB11">
+        <v>100000000</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12930072463</v>
       </c>
@@ -1975,11 +2067,17 @@
       <c r="C12" t="s">
         <v>123</v>
       </c>
-      <c r="D12" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA12">
+        <v>12930072463</v>
+      </c>
+      <c r="AB12">
+        <v>100000000</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12810024894</v>
       </c>
@@ -1989,11 +2087,17 @@
       <c r="C13" t="s">
         <v>123</v>
       </c>
-      <c r="D13" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA13">
+        <v>12810024894</v>
+      </c>
+      <c r="AB13">
+        <v>100000000</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10560084041</v>
       </c>
@@ -2003,11 +2107,17 @@
       <c r="C14" t="s">
         <v>123</v>
       </c>
-      <c r="D14" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA14">
+        <v>10560084041</v>
+      </c>
+      <c r="AB14">
+        <v>100000000</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13640011652</v>
       </c>
@@ -2017,11 +2127,17 @@
       <c r="C15" t="s">
         <v>123</v>
       </c>
-      <c r="D15" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA15">
+        <v>13640011652</v>
+      </c>
+      <c r="AB15">
+        <v>100000000</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13460081318</v>
       </c>
@@ -2031,13 +2147,19 @@
       <c r="C16" t="s">
         <v>123</v>
       </c>
-      <c r="D16" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA16">
+        <v>13460081318</v>
+      </c>
+      <c r="AB16">
+        <v>100000000</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>11190096323</v>
+        <v>12520034239</v>
       </c>
       <c r="B17">
         <v>100000000</v>
@@ -2045,13 +2167,19 @@
       <c r="C17" t="s">
         <v>123</v>
       </c>
-      <c r="D17" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA17">
+        <v>12520034239</v>
+      </c>
+      <c r="AB17">
+        <v>100000000</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>12520034239</v>
+        <v>12260119610</v>
       </c>
       <c r="B18">
         <v>100000000</v>
@@ -2059,13 +2187,19 @@
       <c r="C18" t="s">
         <v>123</v>
       </c>
-      <c r="D18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA18">
+        <v>12260119610</v>
+      </c>
+      <c r="AB18">
+        <v>100000000</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>12260119610</v>
+        <v>4970101565</v>
       </c>
       <c r="B19">
         <v>100000000</v>
@@ -2073,13 +2207,19 @@
       <c r="C19" t="s">
         <v>123</v>
       </c>
-      <c r="D19" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA19">
+        <v>4970101565</v>
+      </c>
+      <c r="AB19">
+        <v>100000000</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>4970101565</v>
+        <v>10320039887</v>
       </c>
       <c r="B20">
         <v>100000000</v>
@@ -2087,13 +2227,19 @@
       <c r="C20" t="s">
         <v>123</v>
       </c>
-      <c r="D20" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA20">
+        <v>10320039887</v>
+      </c>
+      <c r="AB20">
+        <v>100000000</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>10320039887</v>
+        <v>11000112759</v>
       </c>
       <c r="B21">
         <v>100000000</v>
@@ -2101,13 +2247,19 @@
       <c r="C21" t="s">
         <v>123</v>
       </c>
-      <c r="D21" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA21">
+        <v>11000112759</v>
+      </c>
+      <c r="AB21">
+        <v>100000000</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>11000112759</v>
+        <v>11370060915</v>
       </c>
       <c r="B22">
         <v>100000000</v>
@@ -2115,13 +2267,19 @@
       <c r="C22" t="s">
         <v>123</v>
       </c>
-      <c r="D22" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA22">
+        <v>11370060915</v>
+      </c>
+      <c r="AB22">
+        <v>100000000</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>11370060915</v>
+        <v>2600003665</v>
       </c>
       <c r="B23">
         <v>100000000</v>
@@ -2129,13 +2287,19 @@
       <c r="C23" t="s">
         <v>123</v>
       </c>
-      <c r="D23" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA23">
+        <v>2600003665</v>
+      </c>
+      <c r="AB23">
+        <v>100000000</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2600003665</v>
+        <v>1480029806</v>
       </c>
       <c r="B24">
         <v>100000000</v>
@@ -2143,13 +2307,19 @@
       <c r="C24" t="s">
         <v>123</v>
       </c>
-      <c r="D24" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA24">
+        <v>1480029806</v>
+      </c>
+      <c r="AB24">
+        <v>100000000</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>1480029806</v>
+        <v>11450064639</v>
       </c>
       <c r="B25">
         <v>100000000</v>
@@ -2157,13 +2327,19 @@
       <c r="C25" t="s">
         <v>123</v>
       </c>
-      <c r="D25" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA25">
+        <v>11450064639</v>
+      </c>
+      <c r="AB25">
+        <v>100000000</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>11450064639</v>
+        <v>10720198294</v>
       </c>
       <c r="B26">
         <v>100000000</v>
@@ -2171,13 +2347,19 @@
       <c r="C26" t="s">
         <v>123</v>
       </c>
-      <c r="D26" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA26">
+        <v>10720198294</v>
+      </c>
+      <c r="AB26">
+        <v>100000000</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>10720198294</v>
+        <v>3880065530</v>
       </c>
       <c r="B27">
         <v>100000000</v>
@@ -2185,13 +2367,19 @@
       <c r="C27" t="s">
         <v>123</v>
       </c>
-      <c r="D27" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA27">
+        <v>3880065530</v>
+      </c>
+      <c r="AB27">
+        <v>100000000</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>3880065530</v>
+        <v>80031833</v>
       </c>
       <c r="B28">
         <v>100000000</v>
@@ -2199,13 +2387,19 @@
       <c r="C28" t="s">
         <v>123</v>
       </c>
-      <c r="D28" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA28">
+        <v>80031833</v>
+      </c>
+      <c r="AB28">
+        <v>100000000</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>80031833</v>
+        <v>10590131319</v>
       </c>
       <c r="B29">
         <v>100000000</v>
@@ -2213,13 +2407,19 @@
       <c r="C29" t="s">
         <v>123</v>
       </c>
-      <c r="D29" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA29">
+        <v>10590131319</v>
+      </c>
+      <c r="AB29">
+        <v>100000000</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>10590131319</v>
+        <v>240127202</v>
       </c>
       <c r="B30">
         <v>100000000</v>
@@ -2227,13 +2427,19 @@
       <c r="C30" t="s">
         <v>123</v>
       </c>
-      <c r="D30" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA30">
+        <v>240127202</v>
+      </c>
+      <c r="AB30">
+        <v>100000000</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>240127202</v>
+        <v>10930393717</v>
       </c>
       <c r="B31">
         <v>100000000</v>
@@ -2241,13 +2447,19 @@
       <c r="C31" t="s">
         <v>123</v>
       </c>
-      <c r="D31" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA31">
+        <v>10930393717</v>
+      </c>
+      <c r="AB31">
+        <v>100000000</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>10930393717</v>
+        <v>10630179471</v>
       </c>
       <c r="B32">
         <v>100000000</v>
@@ -2255,13 +2467,19 @@
       <c r="C32" t="s">
         <v>123</v>
       </c>
-      <c r="D32" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA32">
+        <v>10630179471</v>
+      </c>
+      <c r="AB32">
+        <v>100000000</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>10630179471</v>
+        <v>11480029721</v>
       </c>
       <c r="B33">
         <v>100000000</v>
@@ -2269,13 +2487,19 @@
       <c r="C33" t="s">
         <v>123</v>
       </c>
-      <c r="D33" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA33">
+        <v>11480029721</v>
+      </c>
+      <c r="AB33">
+        <v>100000000</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>11480029721</v>
+        <v>830413494</v>
       </c>
       <c r="B34">
         <v>100000000</v>
@@ -2283,13 +2507,19 @@
       <c r="C34" t="s">
         <v>123</v>
       </c>
-      <c r="D34" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA34">
+        <v>830413494</v>
+      </c>
+      <c r="AB34">
+        <v>100000000</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>830413494</v>
+        <v>2190146193</v>
       </c>
       <c r="B35">
         <v>100000000</v>
@@ -2297,13 +2527,19 @@
       <c r="C35" t="s">
         <v>123</v>
       </c>
-      <c r="D35" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA35">
+        <v>2190146193</v>
+      </c>
+      <c r="AB35">
+        <v>100000000</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>2190146193</v>
+        <v>10180130203</v>
       </c>
       <c r="B36">
         <v>100000000</v>
@@ -2311,13 +2547,19 @@
       <c r="C36" t="s">
         <v>123</v>
       </c>
-      <c r="D36" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA36">
+        <v>10180130203</v>
+      </c>
+      <c r="AB36">
+        <v>100000000</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>10180130203</v>
+        <v>690059296</v>
       </c>
       <c r="B37">
         <v>100000000</v>
@@ -2325,13 +2567,19 @@
       <c r="C37" t="s">
         <v>123</v>
       </c>
-      <c r="D37" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA37">
+        <v>690059296</v>
+      </c>
+      <c r="AB37">
+        <v>100000000</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>690059296</v>
+        <v>1560012823</v>
       </c>
       <c r="B38">
         <v>100000000</v>
@@ -2339,13 +2587,19 @@
       <c r="C38" t="s">
         <v>123</v>
       </c>
-      <c r="D38" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA38">
+        <v>1560012823</v>
+      </c>
+      <c r="AB38">
+        <v>100000000</v>
+      </c>
+      <c r="AC38" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>1560012823</v>
+        <v>2650033717</v>
       </c>
       <c r="B39">
         <v>100000000</v>
@@ -2353,13 +2607,19 @@
       <c r="C39" t="s">
         <v>123</v>
       </c>
-      <c r="D39" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA39">
+        <v>2650033717</v>
+      </c>
+      <c r="AB39">
+        <v>100000000</v>
+      </c>
+      <c r="AC39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>2650033717</v>
+        <v>10010552085</v>
       </c>
       <c r="B40">
         <v>100000000</v>
@@ -2367,13 +2627,19 @@
       <c r="C40" t="s">
         <v>123</v>
       </c>
-      <c r="D40" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA40">
+        <v>10010552085</v>
+      </c>
+      <c r="AB40">
+        <v>100000000</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>10010552085</v>
+        <v>11680050224</v>
       </c>
       <c r="B41">
         <v>100000000</v>
@@ -2381,13 +2647,19 @@
       <c r="C41" t="s">
         <v>123</v>
       </c>
-      <c r="D41" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA41">
+        <v>11680050224</v>
+      </c>
+      <c r="AB41">
+        <v>100000000</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>11680050224</v>
+        <v>13180116187</v>
       </c>
       <c r="B42">
         <v>100000000</v>
@@ -2395,13 +2667,19 @@
       <c r="C42" t="s">
         <v>123</v>
       </c>
-      <c r="D42" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA42">
+        <v>13180116187</v>
+      </c>
+      <c r="AB42">
+        <v>100000000</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>13180116187</v>
+        <v>12880617116</v>
       </c>
       <c r="B43">
         <v>100000000</v>
@@ -2409,13 +2687,19 @@
       <c r="C43" t="s">
         <v>123</v>
       </c>
-      <c r="D43" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA43">
+        <v>12880617116</v>
+      </c>
+      <c r="AB43">
+        <v>100000000</v>
+      </c>
+      <c r="AC43" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>12880617116</v>
+        <v>385454397</v>
       </c>
       <c r="B44">
         <v>100000000</v>
@@ -2423,13 +2707,19 @@
       <c r="C44" t="s">
         <v>123</v>
       </c>
-      <c r="D44" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA44">
+        <v>385454397</v>
+      </c>
+      <c r="AB44">
+        <v>100000000</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>385454397</v>
+        <v>1170103159</v>
       </c>
       <c r="B45">
         <v>100000000</v>
@@ -2437,13 +2727,19 @@
       <c r="C45" t="s">
         <v>123</v>
       </c>
-      <c r="D45" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA45">
+        <v>1170103159</v>
+      </c>
+      <c r="AB45">
+        <v>100000000</v>
+      </c>
+      <c r="AC45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>1170103159</v>
+        <v>11240036538</v>
       </c>
       <c r="B46">
         <v>100000000</v>
@@ -2451,13 +2747,19 @@
       <c r="C46" t="s">
         <v>123</v>
       </c>
-      <c r="D46" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA46">
+        <v>11240036538</v>
+      </c>
+      <c r="AB46">
+        <v>100000000</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>11240036538</v>
+        <v>11576205327</v>
       </c>
       <c r="B47">
         <v>100000000</v>
@@ -2465,13 +2767,19 @@
       <c r="C47" t="s">
         <v>123</v>
       </c>
-      <c r="D47" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA47">
+        <v>11576205327</v>
+      </c>
+      <c r="AB47">
+        <v>100000000</v>
+      </c>
+      <c r="AC47" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>11576205327</v>
+        <v>10260159191</v>
       </c>
       <c r="B48">
         <v>100000000</v>
@@ -2479,13 +2787,19 @@
       <c r="C48" t="s">
         <v>123</v>
       </c>
-      <c r="D48" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA48">
+        <v>10260159191</v>
+      </c>
+      <c r="AB48">
+        <v>100000000</v>
+      </c>
+      <c r="AC48" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>10260159191</v>
+        <v>3740026512</v>
       </c>
       <c r="B49">
         <v>100000000</v>
@@ -2493,13 +2807,19 @@
       <c r="C49" t="s">
         <v>123</v>
       </c>
-      <c r="D49" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA49">
+        <v>3740026512</v>
+      </c>
+      <c r="AB49">
+        <v>100000000</v>
+      </c>
+      <c r="AC49" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>3740026512</v>
+        <v>3570015560</v>
       </c>
       <c r="B50">
         <v>100000000</v>
@@ -2507,13 +2827,19 @@
       <c r="C50" t="s">
         <v>123</v>
       </c>
-      <c r="D50" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA50">
+        <v>3570015560</v>
+      </c>
+      <c r="AB50">
+        <v>100000000</v>
+      </c>
+      <c r="AC50" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>3570015560</v>
+        <v>1080165573</v>
       </c>
       <c r="B51">
         <v>100000000</v>
@@ -2521,13 +2847,19 @@
       <c r="C51" t="s">
         <v>123</v>
       </c>
-      <c r="D51" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA51">
+        <v>1080165573</v>
+      </c>
+      <c r="AB51">
+        <v>100000000</v>
+      </c>
+      <c r="AC51" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>1080165573</v>
+        <v>10070018723</v>
       </c>
       <c r="B52">
         <v>100000000</v>
@@ -2535,13 +2867,19 @@
       <c r="C52" t="s">
         <v>123</v>
       </c>
-      <c r="D52" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA52">
+        <v>10070018723</v>
+      </c>
+      <c r="AB52">
+        <v>100000000</v>
+      </c>
+      <c r="AC52" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>10070018723</v>
+        <v>11350032974</v>
       </c>
       <c r="B53">
         <v>100000000</v>
@@ -2549,13 +2887,19 @@
       <c r="C53" t="s">
         <v>123</v>
       </c>
-      <c r="D53" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA53">
+        <v>11350032974</v>
+      </c>
+      <c r="AB53">
+        <v>100000000</v>
+      </c>
+      <c r="AC53" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>11350032974</v>
+        <v>3190196232</v>
       </c>
       <c r="B54">
         <v>100000000</v>
@@ -2563,13 +2907,19 @@
       <c r="C54" t="s">
         <v>123</v>
       </c>
-      <c r="D54" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA54">
+        <v>3190196232</v>
+      </c>
+      <c r="AB54">
+        <v>100000000</v>
+      </c>
+      <c r="AC54" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>3190196232</v>
+        <v>3440109728</v>
       </c>
       <c r="B55">
         <v>100000000</v>
@@ -2577,13 +2927,19 @@
       <c r="C55" t="s">
         <v>123</v>
       </c>
-      <c r="D55" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA55">
+        <v>3440109728</v>
+      </c>
+      <c r="AB55">
+        <v>100000000</v>
+      </c>
+      <c r="AC55" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>3440109728</v>
+        <v>14900019425</v>
       </c>
       <c r="B56">
         <v>100000000</v>
@@ -2591,13 +2947,19 @@
       <c r="C56" t="s">
         <v>123</v>
       </c>
-      <c r="D56" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA56">
+        <v>14900019425</v>
+      </c>
+      <c r="AB56">
+        <v>100000000</v>
+      </c>
+      <c r="AC56" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>14900019425</v>
+        <v>13440074198</v>
       </c>
       <c r="B57">
         <v>100000000</v>
@@ -2605,13 +2967,19 @@
       <c r="C57" t="s">
         <v>123</v>
       </c>
-      <c r="D57" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA57">
+        <v>13440074198</v>
+      </c>
+      <c r="AB57">
+        <v>100000000</v>
+      </c>
+      <c r="AC57" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>13440074198</v>
+        <v>10100099137</v>
       </c>
       <c r="B58">
         <v>100000000</v>
@@ -2619,13 +2987,19 @@
       <c r="C58" t="s">
         <v>123</v>
       </c>
-      <c r="D58" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA58">
+        <v>10100099137</v>
+      </c>
+      <c r="AB58">
+        <v>100000000</v>
+      </c>
+      <c r="AC58" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>10100099137</v>
+        <v>14340133361</v>
       </c>
       <c r="B59">
         <v>100000000</v>
@@ -2633,13 +3007,19 @@
       <c r="C59" t="s">
         <v>123</v>
       </c>
-      <c r="D59" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA59">
+        <v>14340133361</v>
+      </c>
+      <c r="AB59">
+        <v>100000000</v>
+      </c>
+      <c r="AC59" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>14340133361</v>
+        <v>10300240049</v>
       </c>
       <c r="B60">
         <v>100000000</v>
@@ -2647,13 +3027,19 @@
       <c r="C60" t="s">
         <v>123</v>
       </c>
-      <c r="D60" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA60">
+        <v>10300240049</v>
+      </c>
+      <c r="AB60">
+        <v>100000000</v>
+      </c>
+      <c r="AC60" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>10300240049</v>
+        <v>13710091218</v>
       </c>
       <c r="B61">
         <v>100000000</v>
@@ -2661,13 +3047,19 @@
       <c r="C61" t="s">
         <v>123</v>
       </c>
-      <c r="D61" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA61">
+        <v>13710091218</v>
+      </c>
+      <c r="AB61">
+        <v>100000000</v>
+      </c>
+      <c r="AC61" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>2740195622</v>
+        <v>12910028712</v>
       </c>
       <c r="B62">
         <v>100000000</v>
@@ -2675,13 +3067,19 @@
       <c r="C62" t="s">
         <v>123</v>
       </c>
-      <c r="D62" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA62">
+        <v>12910028712</v>
+      </c>
+      <c r="AB62">
+        <v>100000000</v>
+      </c>
+      <c r="AC62" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>13710091218</v>
+        <v>11400165979</v>
       </c>
       <c r="B63">
         <v>100000000</v>
@@ -2689,13 +3087,19 @@
       <c r="C63" t="s">
         <v>123</v>
       </c>
-      <c r="D63" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA63">
+        <v>11400165979</v>
+      </c>
+      <c r="AB63">
+        <v>100000000</v>
+      </c>
+      <c r="AC63" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>12910028712</v>
+        <v>12720174614</v>
       </c>
       <c r="B64">
         <v>100000000</v>
@@ -2703,13 +3107,19 @@
       <c r="C64" t="s">
         <v>123</v>
       </c>
-      <c r="D64" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA64">
+        <v>12720174614</v>
+      </c>
+      <c r="AB64">
+        <v>100000000</v>
+      </c>
+      <c r="AC64" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>11400165979</v>
+        <v>13490011693</v>
       </c>
       <c r="B65">
         <v>100000000</v>
@@ -2717,13 +3127,19 @@
       <c r="C65" t="s">
         <v>123</v>
       </c>
-      <c r="D65" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA65">
+        <v>13490011693</v>
+      </c>
+      <c r="AB65">
+        <v>100000000</v>
+      </c>
+      <c r="AC65" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>12720174614</v>
+        <v>10540066810</v>
       </c>
       <c r="B66">
         <v>100000000</v>
@@ -2731,13 +3147,19 @@
       <c r="C66" t="s">
         <v>123</v>
       </c>
-      <c r="D66" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA66">
+        <v>10540066810</v>
+      </c>
+      <c r="AB66">
+        <v>100000000</v>
+      </c>
+      <c r="AC66" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>13490011693</v>
+        <v>13150013946</v>
       </c>
       <c r="B67">
         <v>100000000</v>
@@ -2745,13 +3167,19 @@
       <c r="C67" t="s">
         <v>123</v>
       </c>
-      <c r="D67" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA67">
+        <v>13150013946</v>
+      </c>
+      <c r="AB67">
+        <v>100000000</v>
+      </c>
+      <c r="AC67" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>10540066810</v>
+        <v>10250141650</v>
       </c>
       <c r="B68">
         <v>100000000</v>
@@ -2759,13 +3187,19 @@
       <c r="C68" t="s">
         <v>123</v>
       </c>
-      <c r="D68" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA68">
+        <v>10250141650</v>
+      </c>
+      <c r="AB68">
+        <v>100000000</v>
+      </c>
+      <c r="AC68" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>13150013946</v>
+        <v>2930059431</v>
       </c>
       <c r="B69">
         <v>100000000</v>
@@ -2773,13 +3207,19 @@
       <c r="C69" t="s">
         <v>123</v>
       </c>
-      <c r="D69" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA69">
+        <v>2930059431</v>
+      </c>
+      <c r="AB69">
+        <v>100000000</v>
+      </c>
+      <c r="AC69" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>10250141650</v>
+        <v>11320267205</v>
       </c>
       <c r="B70">
         <v>100000000</v>
@@ -2787,13 +3227,19 @@
       <c r="C70" t="s">
         <v>123</v>
       </c>
-      <c r="D70" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA70">
+        <v>11320267205</v>
+      </c>
+      <c r="AB70">
+        <v>100000000</v>
+      </c>
+      <c r="AC70" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>2930059431</v>
+        <v>12300036343</v>
       </c>
       <c r="B71">
         <v>100000000</v>
@@ -2801,13 +3247,19 @@
       <c r="C71" t="s">
         <v>123</v>
       </c>
-      <c r="D71" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA71">
+        <v>12300036343</v>
+      </c>
+      <c r="AB71">
+        <v>100000000</v>
+      </c>
+      <c r="AC71" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>11320267205</v>
+        <v>11680248641</v>
       </c>
       <c r="B72">
         <v>100000000</v>
@@ -2815,13 +3267,19 @@
       <c r="C72" t="s">
         <v>123</v>
       </c>
-      <c r="D72" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA72">
+        <v>11680248641</v>
+      </c>
+      <c r="AB72">
+        <v>100000000</v>
+      </c>
+      <c r="AC72" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>12300036343</v>
+        <v>3750193466</v>
       </c>
       <c r="B73">
         <v>100000000</v>
@@ -2829,13 +3287,19 @@
       <c r="C73" t="s">
         <v>123</v>
       </c>
-      <c r="D73" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA73">
+        <v>3750193466</v>
+      </c>
+      <c r="AB73">
+        <v>100000000</v>
+      </c>
+      <c r="AC73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="74" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>11680248641</v>
+        <v>12306204458</v>
       </c>
       <c r="B74">
         <v>100000000</v>
@@ -2843,13 +3307,19 @@
       <c r="C74" t="s">
         <v>123</v>
       </c>
-      <c r="D74" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA74">
+        <v>12306204458</v>
+      </c>
+      <c r="AB74">
+        <v>100000000</v>
+      </c>
+      <c r="AC74" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="75" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>3750193466</v>
+        <v>10380505120</v>
       </c>
       <c r="B75">
         <v>100000000</v>
@@ -2857,13 +3327,19 @@
       <c r="C75" t="s">
         <v>123</v>
       </c>
-      <c r="D75" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA75">
+        <v>10380505120</v>
+      </c>
+      <c r="AB75">
+        <v>100000000</v>
+      </c>
+      <c r="AC75" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="76" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>12306204458</v>
+        <v>1275372153</v>
       </c>
       <c r="B76">
         <v>100000000</v>
@@ -2871,13 +3347,19 @@
       <c r="C76" t="s">
         <v>123</v>
       </c>
-      <c r="D76" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA76">
+        <v>1275372153</v>
+      </c>
+      <c r="AB76">
+        <v>100000000</v>
+      </c>
+      <c r="AC76" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="77" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>10380505120</v>
+        <v>320076608</v>
       </c>
       <c r="B77">
         <v>100000000</v>
@@ -2885,13 +3367,19 @@
       <c r="C77" t="s">
         <v>123</v>
       </c>
-      <c r="D77" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA77">
+        <v>320076608</v>
+      </c>
+      <c r="AB77">
+        <v>100000000</v>
+      </c>
+      <c r="AC77" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="78" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>1275372153</v>
+        <v>10490061802</v>
       </c>
       <c r="B78">
         <v>100000000</v>
@@ -2899,13 +3387,19 @@
       <c r="C78" t="s">
         <v>123</v>
       </c>
-      <c r="D78" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA78">
+        <v>10490061802</v>
+      </c>
+      <c r="AB78">
+        <v>100000000</v>
+      </c>
+      <c r="AC78" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="79" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>320076608</v>
+        <v>11050100658</v>
       </c>
       <c r="B79">
         <v>100000000</v>
@@ -2913,13 +3407,19 @@
       <c r="C79" t="s">
         <v>123</v>
       </c>
-      <c r="D79" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA79">
+        <v>11050100658</v>
+      </c>
+      <c r="AB79">
+        <v>100000000</v>
+      </c>
+      <c r="AC79" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="80" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>10490061802</v>
+        <v>10760058301</v>
       </c>
       <c r="B80">
         <v>100000000</v>
@@ -2927,13 +3427,19 @@
       <c r="C80" t="s">
         <v>123</v>
       </c>
-      <c r="D80" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA80">
+        <v>10760058301</v>
+      </c>
+      <c r="AB80">
+        <v>100000000</v>
+      </c>
+      <c r="AC80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="81" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>11050100658</v>
+        <v>3500015064</v>
       </c>
       <c r="B81">
         <v>100000000</v>
@@ -2941,13 +3447,19 @@
       <c r="C81" t="s">
         <v>123</v>
       </c>
-      <c r="D81" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA81">
+        <v>3500015064</v>
+      </c>
+      <c r="AB81">
+        <v>100000000</v>
+      </c>
+      <c r="AC81" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="82" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>10760058301</v>
+        <v>3445103916</v>
       </c>
       <c r="B82">
         <v>100000000</v>
@@ -2955,13 +3467,19 @@
       <c r="C82" t="s">
         <v>123</v>
       </c>
-      <c r="D82" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA82">
+        <v>3445103916</v>
+      </c>
+      <c r="AB82">
+        <v>100000000</v>
+      </c>
+      <c r="AC82" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="83" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>3500015064</v>
+        <v>15853015</v>
       </c>
       <c r="B83">
         <v>100000000</v>
@@ -2969,13 +3487,19 @@
       <c r="C83" t="s">
         <v>123</v>
       </c>
-      <c r="D83" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA83">
+        <v>15853015</v>
+      </c>
+      <c r="AB83">
+        <v>100000000</v>
+      </c>
+      <c r="AC83" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="84" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>3445103916</v>
+        <v>10910211970</v>
       </c>
       <c r="B84">
         <v>100000000</v>
@@ -2983,13 +3507,19 @@
       <c r="C84" t="s">
         <v>123</v>
       </c>
-      <c r="D84" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA84">
+        <v>10910211970</v>
+      </c>
+      <c r="AB84">
+        <v>100000000</v>
+      </c>
+      <c r="AC84" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="85" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>15853015</v>
+        <v>13450026215</v>
       </c>
       <c r="B85">
         <v>100000000</v>
@@ -2997,13 +3527,19 @@
       <c r="C85" t="s">
         <v>123</v>
       </c>
-      <c r="D85" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA85">
+        <v>13450026215</v>
+      </c>
+      <c r="AB85">
+        <v>100000000</v>
+      </c>
+      <c r="AC85" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="86" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>10910211970</v>
+        <v>12300016631</v>
       </c>
       <c r="B86">
         <v>100000000</v>
@@ -3011,13 +3547,19 @@
       <c r="C86" t="s">
         <v>123</v>
       </c>
-      <c r="D86" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA86">
+        <v>12300016631</v>
+      </c>
+      <c r="AB86">
+        <v>100000000</v>
+      </c>
+      <c r="AC86" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="87" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>13450026215</v>
+        <v>10830113837</v>
       </c>
       <c r="B87">
         <v>100000000</v>
@@ -3025,13 +3567,19 @@
       <c r="C87" t="s">
         <v>123</v>
       </c>
-      <c r="D87" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA87">
+        <v>10830113837</v>
+      </c>
+      <c r="AB87">
+        <v>100000000</v>
+      </c>
+      <c r="AC87" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="88" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>12300016631</v>
+        <v>10326209059</v>
       </c>
       <c r="B88">
         <v>100000000</v>
@@ -3039,13 +3587,19 @@
       <c r="C88" t="s">
         <v>123</v>
       </c>
-      <c r="D88" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA88">
+        <v>10326209059</v>
+      </c>
+      <c r="AB88">
+        <v>100000000</v>
+      </c>
+      <c r="AC88" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="89" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>10830113837</v>
+        <v>12440133573</v>
       </c>
       <c r="B89">
         <v>100000000</v>
@@ -3053,13 +3607,19 @@
       <c r="C89" t="s">
         <v>123</v>
       </c>
-      <c r="D89" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA89">
+        <v>12440133573</v>
+      </c>
+      <c r="AB89">
+        <v>100000000</v>
+      </c>
+      <c r="AC89" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="90" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>10326209059</v>
+        <v>3160093053</v>
       </c>
       <c r="B90">
         <v>100000000</v>
@@ -3067,13 +3627,19 @@
       <c r="C90" t="s">
         <v>123</v>
       </c>
-      <c r="D90" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA90">
+        <v>3160093053</v>
+      </c>
+      <c r="AB90">
+        <v>100000000</v>
+      </c>
+      <c r="AC90" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="91" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>12440133573</v>
+        <v>13190176575</v>
       </c>
       <c r="B91">
         <v>100000000</v>
@@ -3081,13 +3647,19 @@
       <c r="C91" t="s">
         <v>123</v>
       </c>
-      <c r="D91" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA91">
+        <v>13190176575</v>
+      </c>
+      <c r="AB91">
+        <v>100000000</v>
+      </c>
+      <c r="AC91" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="92" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>3160093053</v>
+        <v>12190083139</v>
       </c>
       <c r="B92">
         <v>100000000</v>
@@ -3095,13 +3667,19 @@
       <c r="C92" t="s">
         <v>123</v>
       </c>
-      <c r="D92" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA92">
+        <v>12190083139</v>
+      </c>
+      <c r="AB92">
+        <v>100000000</v>
+      </c>
+      <c r="AC92" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="93" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>13190176575</v>
+        <v>12400203384</v>
       </c>
       <c r="B93">
         <v>100000000</v>
@@ -3109,13 +3687,19 @@
       <c r="C93" t="s">
         <v>123</v>
       </c>
-      <c r="D93" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA93">
+        <v>12400203384</v>
+      </c>
+      <c r="AB93">
+        <v>100000000</v>
+      </c>
+      <c r="AC93" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="94" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>12190083139</v>
+        <v>10950217871</v>
       </c>
       <c r="B94">
         <v>100000000</v>
@@ -3123,13 +3707,19 @@
       <c r="C94" t="s">
         <v>123</v>
       </c>
-      <c r="D94" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA94">
+        <v>10950217871</v>
+      </c>
+      <c r="AB94">
+        <v>100000000</v>
+      </c>
+      <c r="AC94" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="95" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>12400203384</v>
+        <v>795010086</v>
       </c>
       <c r="B95">
         <v>100000000</v>
@@ -3137,13 +3727,19 @@
       <c r="C95" t="s">
         <v>123</v>
       </c>
-      <c r="D95" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA95">
+        <v>795010086</v>
+      </c>
+      <c r="AB95">
+        <v>100000000</v>
+      </c>
+      <c r="AC95" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="96" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>10950217871</v>
+        <v>10300022865</v>
       </c>
       <c r="B96">
         <v>100000000</v>
@@ -3151,13 +3747,19 @@
       <c r="C96" t="s">
         <v>123</v>
       </c>
-      <c r="D96" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA96">
+        <v>10300022865</v>
+      </c>
+      <c r="AB96">
+        <v>100000000</v>
+      </c>
+      <c r="AC96" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="97" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>795010086</v>
+        <v>13640115163</v>
       </c>
       <c r="B97">
         <v>100000000</v>
@@ -3165,13 +3767,19 @@
       <c r="C97" t="s">
         <v>123</v>
       </c>
-      <c r="D97" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA97">
+        <v>13640115163</v>
+      </c>
+      <c r="AB97">
+        <v>100000000</v>
+      </c>
+      <c r="AC97" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="98" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>10300022865</v>
+        <v>10010330298</v>
       </c>
       <c r="B98">
         <v>100000000</v>
@@ -3179,13 +3787,19 @@
       <c r="C98" t="s">
         <v>123</v>
       </c>
-      <c r="D98" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA98">
+        <v>10010330298</v>
+      </c>
+      <c r="AB98">
+        <v>100000000</v>
+      </c>
+      <c r="AC98" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="99" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>13640115163</v>
+        <v>10156208053</v>
       </c>
       <c r="B99">
         <v>100000000</v>
@@ -3193,13 +3807,19 @@
       <c r="C99" t="s">
         <v>123</v>
       </c>
-      <c r="D99" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA99">
+        <v>10156208053</v>
+      </c>
+      <c r="AB99">
+        <v>100000000</v>
+      </c>
+      <c r="AC99" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="100" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>10010330298</v>
+        <v>10190191410</v>
       </c>
       <c r="B100">
         <v>100000000</v>
@@ -3207,13 +3827,19 @@
       <c r="C100" t="s">
         <v>123</v>
       </c>
-      <c r="D100" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA100">
+        <v>10190191410</v>
+      </c>
+      <c r="AB100">
+        <v>100000000</v>
+      </c>
+      <c r="AC100" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="101" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>10156208053</v>
+        <v>10250141636</v>
       </c>
       <c r="B101">
         <v>100000000</v>
@@ -3221,13 +3847,19 @@
       <c r="C101" t="s">
         <v>123</v>
       </c>
-      <c r="D101" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA101">
+        <v>10250141636</v>
+      </c>
+      <c r="AB101">
+        <v>100000000</v>
+      </c>
+      <c r="AC101" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="102" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>10190191410</v>
+        <v>10276205518</v>
       </c>
       <c r="B102">
         <v>100000000</v>
@@ -3235,13 +3867,19 @@
       <c r="C102" t="s">
         <v>123</v>
       </c>
-      <c r="D102" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA102">
+        <v>10276205518</v>
+      </c>
+      <c r="AB102">
+        <v>100000000</v>
+      </c>
+      <c r="AC102" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="103" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>10250141636</v>
+        <v>10370241975</v>
       </c>
       <c r="B103">
         <v>100000000</v>
@@ -3249,13 +3887,19 @@
       <c r="C103" t="s">
         <v>123</v>
       </c>
-      <c r="D103" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA103">
+        <v>10370241975</v>
+      </c>
+      <c r="AB103">
+        <v>100000000</v>
+      </c>
+      <c r="AC103" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="104" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>10276205518</v>
+        <v>10430208230</v>
       </c>
       <c r="B104">
         <v>100000000</v>
@@ -3263,13 +3907,19 @@
       <c r="C104" t="s">
         <v>123</v>
       </c>
-      <c r="D104" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA104">
+        <v>10430208230</v>
+      </c>
+      <c r="AB104">
+        <v>100000000</v>
+      </c>
+      <c r="AC104" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="105" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>10370241975</v>
+        <v>10620117469</v>
       </c>
       <c r="B105">
         <v>100000000</v>
@@ -3277,13 +3927,19 @@
       <c r="C105" t="s">
         <v>123</v>
       </c>
-      <c r="D105" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA105">
+        <v>10620117469</v>
+      </c>
+      <c r="AB105">
+        <v>100000000</v>
+      </c>
+      <c r="AC105" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="106" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>10430208230</v>
+        <v>10730037635</v>
       </c>
       <c r="B106">
         <v>100000000</v>
@@ -3291,13 +3947,19 @@
       <c r="C106" t="s">
         <v>123</v>
       </c>
-      <c r="D106" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA106">
+        <v>10730037635</v>
+      </c>
+      <c r="AB106">
+        <v>100000000</v>
+      </c>
+      <c r="AC106" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="107" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>10620117469</v>
+        <v>11000011032</v>
       </c>
       <c r="B107">
         <v>100000000</v>
@@ -3305,13 +3967,19 @@
       <c r="C107" t="s">
         <v>123</v>
       </c>
-      <c r="D107" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA107">
+        <v>11000011032</v>
+      </c>
+      <c r="AB107">
+        <v>100000000</v>
+      </c>
+      <c r="AC107" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="108" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>10730037635</v>
+        <v>10820077392</v>
       </c>
       <c r="B108">
         <v>100000000</v>
@@ -3319,13 +3987,19 @@
       <c r="C108" t="s">
         <v>123</v>
       </c>
-      <c r="D108" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA108">
+        <v>10820077392</v>
+      </c>
+      <c r="AB108">
+        <v>100000000</v>
+      </c>
+      <c r="AC108" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="109" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>11000011032</v>
+        <v>10850234873</v>
       </c>
       <c r="B109">
         <v>100000000</v>
@@ -3333,13 +4007,19 @@
       <c r="C109" t="s">
         <v>123</v>
       </c>
-      <c r="D109" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA109">
+        <v>10850234873</v>
+      </c>
+      <c r="AB109">
+        <v>100000000</v>
+      </c>
+      <c r="AC109" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="110" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>10820077392</v>
+        <v>10860133029</v>
       </c>
       <c r="B110">
         <v>100000000</v>
@@ -3347,13 +4027,19 @@
       <c r="C110" t="s">
         <v>123</v>
       </c>
-      <c r="D110" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA110">
+        <v>10860133029</v>
+      </c>
+      <c r="AB110">
+        <v>100000000</v>
+      </c>
+      <c r="AC110" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="111" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>10850234873</v>
+        <v>10910192561</v>
       </c>
       <c r="B111">
         <v>100000000</v>
@@ -3361,13 +4047,19 @@
       <c r="C111" t="s">
         <v>123</v>
       </c>
-      <c r="D111" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA111">
+        <v>10910192561</v>
+      </c>
+      <c r="AB111">
+        <v>100000000</v>
+      </c>
+      <c r="AC111" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="112" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>10860133029</v>
+        <v>10930015684</v>
       </c>
       <c r="B112">
         <v>100000000</v>
@@ -3375,13 +4067,19 @@
       <c r="C112" t="s">
         <v>123</v>
       </c>
-      <c r="D112" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA112">
+        <v>10930015684</v>
+      </c>
+      <c r="AB112">
+        <v>100000000</v>
+      </c>
+      <c r="AC112" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="113" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>10910192561</v>
+        <v>10850262566</v>
       </c>
       <c r="B113">
         <v>100000000</v>
@@ -3389,13 +4087,19 @@
       <c r="C113" t="s">
         <v>123</v>
       </c>
-      <c r="D113" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA113">
+        <v>10850262566</v>
+      </c>
+      <c r="AB113">
+        <v>100000000</v>
+      </c>
+      <c r="AC113" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="114" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>10930015684</v>
+        <v>10930481083</v>
       </c>
       <c r="B114">
         <v>100000000</v>
@@ -3403,13 +4107,19 @@
       <c r="C114" t="s">
         <v>123</v>
       </c>
-      <c r="D114" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA114">
+        <v>10930481083</v>
+      </c>
+      <c r="AB114">
+        <v>100000000</v>
+      </c>
+      <c r="AC114" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="115" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>10850262566</v>
+        <v>10960083127</v>
       </c>
       <c r="B115">
         <v>100000000</v>
@@ -3417,13 +4127,19 @@
       <c r="C115" t="s">
         <v>123</v>
       </c>
-      <c r="D115" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA115">
+        <v>10960083127</v>
+      </c>
+      <c r="AB115">
+        <v>100000000</v>
+      </c>
+      <c r="AC115" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="116" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>10930481083</v>
+        <v>11000050545</v>
       </c>
       <c r="B116">
         <v>100000000</v>
@@ -3431,36 +4147,14 @@
       <c r="C116" t="s">
         <v>123</v>
       </c>
-      <c r="D116" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117">
-        <v>10960083127</v>
-      </c>
-      <c r="B117">
-        <v>100000000</v>
-      </c>
-      <c r="C117" t="s">
-        <v>123</v>
-      </c>
-      <c r="D117" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118">
+      <c r="AA116">
         <v>11000050545</v>
       </c>
-      <c r="B118">
-        <v>100000000</v>
-      </c>
-      <c r="C118" t="s">
-        <v>123</v>
-      </c>
-      <c r="D118" t="s">
-        <v>209</v>
+      <c r="AB116">
+        <v>100000000</v>
+      </c>
+      <c r="AC116" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -4391,7 +5085,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6F6505-72C5-407A-9E87-8F1DBAE9B164}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4417,19 +5113,19 @@
         <v>155</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>212</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4437,19 +5133,19 @@
         <v>156</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>212</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4457,19 +5153,19 @@
         <v>157</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>212</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE] Fallas de Dispositivos, Movimientos Automaticos, Resumen de Cuentas, Cuentas, Tarjetas
Se agregaron los casos F18 hasta F21
Se agregO el caso C17
Se agrego el caso RC31
Se agrego el caso T01
Se agrego el caso MA20
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20414"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B91EFC1-8A4A-4C66-8FAE-0CEAA7463CA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D774E68C-A907-4A45-B3EB-538A5E9922F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server IP" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="225">
   <si>
     <t>Nombre</t>
   </si>
@@ -700,6 +700,12 @@
   </si>
   <si>
     <t>SI</t>
+  </si>
+  <si>
+    <t>LECHEVERRIA</t>
+  </si>
+  <si>
+    <t>102</t>
   </si>
 </sst>
 </file>
@@ -1164,10 +1170,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1818,6 +1824,14 @@
         <v>221</v>
       </c>
     </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>223</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1828,7 +1842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F86E7B-4061-45F1-9FC5-D02253AB0909}">
   <dimension ref="A1:AH157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>